<commit_message>
Finished default salaries database.
</commit_message>
<xml_diff>
--- a/SourceData/humanresources/HWModData.xlsx
+++ b/SourceData/humanresources/HWModData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proj\SpectrumEngine\DefaultData\SourceData\humanresources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDABA6C3-FC82-4EE0-8B82-41451B0B7053}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CB6CC9A-C75D-462F-A538-910E641DD400}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25320" yWindow="-1095" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1487,9 +1487,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H180"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:L1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -1498,10 +1496,10 @@
         <v>185</v>
       </c>
       <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
         <v>364</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -1524,10 +1522,10 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
         <v>186</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
       </c>
       <c r="D2">
         <v>970.38318130000005</v>
@@ -1550,10 +1548,10 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
         <v>187</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
       </c>
       <c r="D3">
         <v>2383.926665</v>
@@ -1576,10 +1574,10 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
         <v>188</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
       </c>
       <c r="D4">
         <v>4459.8694379999997</v>
@@ -1602,10 +1600,10 @@
         <v>24</v>
       </c>
       <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
         <v>189</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
       </c>
       <c r="D5">
         <v>4069.1682799999999</v>
@@ -1628,10 +1626,10 @@
         <v>32</v>
       </c>
       <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
         <v>190</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
       </c>
       <c r="D6">
         <v>4839.4223400000001</v>
@@ -1654,10 +1652,10 @@
         <v>51</v>
       </c>
       <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
         <v>191</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
       </c>
       <c r="D7">
         <v>1503.3972369999999</v>
@@ -1680,10 +1678,10 @@
         <v>36</v>
       </c>
       <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
         <v>192</v>
-      </c>
-      <c r="C8" t="s">
-        <v>12</v>
       </c>
       <c r="D8">
         <v>30820.62342</v>
@@ -1706,10 +1704,10 @@
         <v>40</v>
       </c>
       <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
         <v>193</v>
-      </c>
-      <c r="C9" t="s">
-        <v>13</v>
       </c>
       <c r="D9">
         <v>30610.24411</v>
@@ -1732,10 +1730,10 @@
         <v>31</v>
       </c>
       <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
         <v>194</v>
-      </c>
-      <c r="C10" t="s">
-        <v>14</v>
       </c>
       <c r="D10">
         <v>1486.842167</v>
@@ -1758,10 +1756,10 @@
         <v>44</v>
       </c>
       <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
         <v>195</v>
-      </c>
-      <c r="C11" t="s">
-        <v>15</v>
       </c>
       <c r="D11">
         <v>9233.1930790000006</v>
@@ -1784,10 +1782,10 @@
         <v>48</v>
       </c>
       <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
         <v>196</v>
-      </c>
-      <c r="C12" t="s">
-        <v>16</v>
       </c>
       <c r="D12">
         <v>21923.596539999999</v>
@@ -1810,10 +1808,10 @@
         <v>50</v>
       </c>
       <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" t="s">
         <v>197</v>
-      </c>
-      <c r="C13" t="s">
-        <v>17</v>
       </c>
       <c r="D13">
         <v>1255.088741</v>
@@ -1836,10 +1834,10 @@
         <v>52</v>
       </c>
       <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" t="s">
         <v>198</v>
-      </c>
-      <c r="C14" t="s">
-        <v>18</v>
       </c>
       <c r="D14">
         <v>6919.8844369999997</v>
@@ -1862,10 +1860,10 @@
         <v>112</v>
       </c>
       <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" t="s">
         <v>199</v>
-      </c>
-      <c r="C15" t="s">
-        <v>19</v>
       </c>
       <c r="D15">
         <v>2528.5908979999999</v>
@@ -1888,10 +1886,10 @@
         <v>56</v>
       </c>
       <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" t="s">
         <v>200</v>
-      </c>
-      <c r="C16" t="s">
-        <v>20</v>
       </c>
       <c r="D16">
         <v>30866.694469999999</v>
@@ -1914,10 +1912,10 @@
         <v>84</v>
       </c>
       <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" t="s">
         <v>201</v>
-      </c>
-      <c r="C17" t="s">
-        <v>21</v>
       </c>
       <c r="D17">
         <v>4578.8636619999997</v>
@@ -1940,10 +1938,10 @@
         <v>204</v>
       </c>
       <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" t="s">
         <v>202</v>
-      </c>
-      <c r="C18" t="s">
-        <v>22</v>
       </c>
       <c r="D18">
         <v>2046.6863249999999</v>
@@ -1966,10 +1964,10 @@
         <v>64</v>
       </c>
       <c r="B19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" t="s">
         <v>203</v>
-      </c>
-      <c r="C19" t="s">
-        <v>23</v>
       </c>
       <c r="D19">
         <v>1472.045478</v>
@@ -1992,10 +1990,10 @@
         <v>68</v>
       </c>
       <c r="B20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" t="s">
         <v>204</v>
-      </c>
-      <c r="C20" t="s">
-        <v>24</v>
       </c>
       <c r="D20">
         <v>2311.7824679999999</v>
@@ -2018,10 +2016,10 @@
         <v>70</v>
       </c>
       <c r="B21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" t="s">
         <v>205</v>
-      </c>
-      <c r="C21" t="s">
-        <v>25</v>
       </c>
       <c r="D21">
         <v>2341.9968119999999</v>
@@ -2044,10 +2042,10 @@
         <v>72</v>
       </c>
       <c r="B22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" t="s">
         <v>206</v>
-      </c>
-      <c r="C22" t="s">
-        <v>26</v>
       </c>
       <c r="D22">
         <v>6655.0979710000001</v>
@@ -2070,10 +2068,10 @@
         <v>76</v>
       </c>
       <c r="B23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" t="s">
         <v>207</v>
-      </c>
-      <c r="C23" t="s">
-        <v>27</v>
       </c>
       <c r="D23">
         <v>4737.2754180000002</v>
@@ -2096,10 +2094,10 @@
         <v>96</v>
       </c>
       <c r="B24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" t="s">
         <v>208</v>
-      </c>
-      <c r="C24" t="s">
-        <v>28</v>
       </c>
       <c r="D24">
         <v>27933.960060000001</v>
@@ -2122,10 +2120,10 @@
         <v>100</v>
       </c>
       <c r="B25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" t="s">
         <v>209</v>
-      </c>
-      <c r="C25" t="s">
-        <v>29</v>
       </c>
       <c r="D25">
         <v>2941.2037230000001</v>
@@ -2148,10 +2146,10 @@
         <v>854</v>
       </c>
       <c r="B26" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" t="s">
         <v>210</v>
-      </c>
-      <c r="C26" t="s">
-        <v>30</v>
       </c>
       <c r="D26">
         <v>1859.510996</v>
@@ -2174,10 +2172,10 @@
         <v>108</v>
       </c>
       <c r="B27" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" t="s">
         <v>211</v>
-      </c>
-      <c r="C27" t="s">
-        <v>31</v>
       </c>
       <c r="D27">
         <v>1526.757423</v>
@@ -2200,10 +2198,10 @@
         <v>116</v>
       </c>
       <c r="B28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" t="s">
         <v>212</v>
-      </c>
-      <c r="C28" t="s">
-        <v>32</v>
       </c>
       <c r="D28">
         <v>938.31894690000001</v>
@@ -2226,10 +2224,10 @@
         <v>120</v>
       </c>
       <c r="B29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" t="s">
         <v>213</v>
-      </c>
-      <c r="C29" t="s">
-        <v>33</v>
       </c>
       <c r="D29">
         <v>2854.3906539999998</v>
@@ -2252,10 +2250,10 @@
         <v>124</v>
       </c>
       <c r="B30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" t="s">
         <v>214</v>
-      </c>
-      <c r="C30" t="s">
-        <v>34</v>
       </c>
       <c r="D30">
         <v>29985.01153</v>
@@ -2278,10 +2276,10 @@
         <v>132</v>
       </c>
       <c r="B31" t="s">
+        <v>35</v>
+      </c>
+      <c r="C31" t="s">
         <v>215</v>
-      </c>
-      <c r="C31" t="s">
-        <v>35</v>
       </c>
       <c r="D31">
         <v>3887.6780939999999</v>
@@ -2304,10 +2302,10 @@
         <v>140</v>
       </c>
       <c r="B32" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" t="s">
         <v>216</v>
-      </c>
-      <c r="C32" t="s">
-        <v>36</v>
       </c>
       <c r="D32">
         <v>1654.2851069999999</v>
@@ -2330,10 +2328,10 @@
         <v>148</v>
       </c>
       <c r="B33" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33" t="s">
         <v>217</v>
-      </c>
-      <c r="C33" t="s">
-        <v>37</v>
       </c>
       <c r="D33">
         <v>2268.0479559999999</v>
@@ -2356,10 +2354,10 @@
         <v>152</v>
       </c>
       <c r="B34" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" t="s">
         <v>218</v>
-      </c>
-      <c r="C34" t="s">
-        <v>38</v>
       </c>
       <c r="D34">
         <v>5793.0180309999996</v>
@@ -2382,10 +2380,10 @@
         <v>156</v>
       </c>
       <c r="B35" t="s">
+        <v>39</v>
+      </c>
+      <c r="C35" t="s">
         <v>219</v>
-      </c>
-      <c r="C35" t="s">
-        <v>39</v>
       </c>
       <c r="D35">
         <v>1635.254312</v>
@@ -2408,10 +2406,10 @@
         <v>170</v>
       </c>
       <c r="B36" t="s">
+        <v>40</v>
+      </c>
+      <c r="C36" t="s">
         <v>220</v>
-      </c>
-      <c r="C36" t="s">
-        <v>40</v>
       </c>
       <c r="D36">
         <v>3489.6259580000001</v>
@@ -2434,10 +2432,10 @@
         <v>174</v>
       </c>
       <c r="B37" t="s">
+        <v>41</v>
+      </c>
+      <c r="C37" t="s">
         <v>221</v>
-      </c>
-      <c r="C37" t="s">
-        <v>41</v>
       </c>
       <c r="D37">
         <v>1953.5227609999999</v>
@@ -2460,10 +2458,10 @@
         <v>178</v>
       </c>
       <c r="B38" t="s">
+        <v>42</v>
+      </c>
+      <c r="C38" t="s">
         <v>222</v>
-      </c>
-      <c r="C38" t="s">
-        <v>42</v>
       </c>
       <c r="D38">
         <v>3664.4705949999998</v>
@@ -2486,10 +2484,10 @@
         <v>188</v>
       </c>
       <c r="B39" t="s">
+        <v>43</v>
+      </c>
+      <c r="C39" t="s">
         <v>223</v>
-      </c>
-      <c r="C39" t="s">
-        <v>43</v>
       </c>
       <c r="D39">
         <v>4527.536513</v>
@@ -2512,10 +2510,10 @@
         <v>384</v>
       </c>
       <c r="B40" t="s">
+        <v>44</v>
+      </c>
+      <c r="C40" t="s">
         <v>224</v>
-      </c>
-      <c r="C40" t="s">
-        <v>44</v>
       </c>
       <c r="D40">
         <v>2801.7736580000001</v>
@@ -2538,10 +2536,10 @@
         <v>191</v>
       </c>
       <c r="B41" t="s">
+        <v>45</v>
+      </c>
+      <c r="C41" t="s">
         <v>225</v>
-      </c>
-      <c r="C41" t="s">
-        <v>45</v>
       </c>
       <c r="D41">
         <v>16099.20571</v>
@@ -2564,10 +2562,10 @@
         <v>192</v>
       </c>
       <c r="B42" t="s">
+        <v>46</v>
+      </c>
+      <c r="C42" t="s">
         <v>226</v>
-      </c>
-      <c r="C42" t="s">
-        <v>46</v>
       </c>
       <c r="D42">
         <v>10863.882949999999</v>
@@ -2590,10 +2588,10 @@
         <v>196</v>
       </c>
       <c r="B43" t="s">
+        <v>47</v>
+      </c>
+      <c r="C43" t="s">
         <v>227</v>
-      </c>
-      <c r="C43" t="s">
-        <v>47</v>
       </c>
       <c r="D43">
         <v>24660.844959999999</v>
@@ -2616,10 +2614,10 @@
         <v>203</v>
       </c>
       <c r="B44" t="s">
+        <v>48</v>
+      </c>
+      <c r="C44" t="s">
         <v>228</v>
-      </c>
-      <c r="C44" t="s">
-        <v>48</v>
       </c>
       <c r="D44">
         <v>18648.902139999998</v>
@@ -2642,10 +2640,10 @@
         <v>408</v>
       </c>
       <c r="B45" t="s">
+        <v>49</v>
+      </c>
+      <c r="C45" t="s">
         <v>229</v>
-      </c>
-      <c r="C45" t="s">
-        <v>49</v>
       </c>
       <c r="D45">
         <v>113.74685839999999</v>
@@ -2668,10 +2666,10 @@
         <v>180</v>
       </c>
       <c r="B46" t="s">
+        <v>50</v>
+      </c>
+      <c r="C46" t="s">
         <v>230</v>
-      </c>
-      <c r="C46" t="s">
-        <v>50</v>
       </c>
       <c r="D46">
         <v>1049.5852379999999</v>
@@ -2694,10 +2692,10 @@
         <v>208</v>
       </c>
       <c r="B47" t="s">
+        <v>51</v>
+      </c>
+      <c r="C47" t="s">
         <v>231</v>
-      </c>
-      <c r="C47" t="s">
-        <v>51</v>
       </c>
       <c r="D47">
         <v>34176.872000000003</v>
@@ -2720,10 +2718,10 @@
         <v>262</v>
       </c>
       <c r="B48" t="s">
+        <v>52</v>
+      </c>
+      <c r="C48" t="s">
         <v>232</v>
-      </c>
-      <c r="C48" t="s">
-        <v>52</v>
       </c>
       <c r="D48">
         <v>1647.7024919999999</v>
@@ -2746,10 +2744,10 @@
         <v>214</v>
       </c>
       <c r="B49" t="s">
+        <v>53</v>
+      </c>
+      <c r="C49" t="s">
         <v>233</v>
-      </c>
-      <c r="C49" t="s">
-        <v>53</v>
       </c>
       <c r="D49">
         <v>4441.8900910000002</v>
@@ -2772,10 +2770,10 @@
         <v>218</v>
       </c>
       <c r="B50" t="s">
+        <v>54</v>
+      </c>
+      <c r="C50" t="s">
         <v>234</v>
-      </c>
-      <c r="C50" t="s">
-        <v>54</v>
       </c>
       <c r="D50">
         <v>3794.6566830000002</v>
@@ -2798,10 +2796,10 @@
         <v>818</v>
       </c>
       <c r="B51" t="s">
+        <v>55</v>
+      </c>
+      <c r="C51" t="s">
         <v>235</v>
-      </c>
-      <c r="C51" t="s">
-        <v>55</v>
       </c>
       <c r="D51">
         <v>2918.404137</v>
@@ -2824,10 +2822,10 @@
         <v>222</v>
       </c>
       <c r="B52" t="s">
+        <v>56</v>
+      </c>
+      <c r="C52" t="s">
         <v>236</v>
-      </c>
-      <c r="C52" t="s">
-        <v>56</v>
       </c>
       <c r="D52">
         <v>3584.004336</v>
@@ -2850,10 +2848,10 @@
         <v>226</v>
       </c>
       <c r="B53" t="s">
+        <v>57</v>
+      </c>
+      <c r="C53" t="s">
         <v>237</v>
-      </c>
-      <c r="C53" t="s">
-        <v>57</v>
       </c>
       <c r="D53">
         <v>9847.7438199999997</v>
@@ -2876,10 +2874,10 @@
         <v>232</v>
       </c>
       <c r="B54" t="s">
+        <v>58</v>
+      </c>
+      <c r="C54" t="s">
         <v>238</v>
-      </c>
-      <c r="C54" t="s">
-        <v>58</v>
       </c>
       <c r="D54">
         <v>1324.146622</v>
@@ -2902,10 +2900,10 @@
         <v>233</v>
       </c>
       <c r="B55" t="s">
+        <v>59</v>
+      </c>
+      <c r="C55" t="s">
         <v>239</v>
-      </c>
-      <c r="C55" t="s">
-        <v>59</v>
       </c>
       <c r="D55">
         <v>8254.7281700000003</v>
@@ -2928,10 +2926,10 @@
         <v>231</v>
       </c>
       <c r="B56" t="s">
+        <v>60</v>
+      </c>
+      <c r="C56" t="s">
         <v>240</v>
-      </c>
-      <c r="C56" t="s">
-        <v>60</v>
       </c>
       <c r="D56">
         <v>1029.87987</v>
@@ -2954,10 +2952,10 @@
         <v>242</v>
       </c>
       <c r="B57" t="s">
+        <v>61</v>
+      </c>
+      <c r="C57" t="s">
         <v>241</v>
-      </c>
-      <c r="C57" t="s">
-        <v>61</v>
       </c>
       <c r="D57">
         <v>2787.189417</v>
@@ -2980,10 +2978,10 @@
         <v>246</v>
       </c>
       <c r="B58" t="s">
+        <v>62</v>
+      </c>
+      <c r="C58" t="s">
         <v>242</v>
-      </c>
-      <c r="C58" t="s">
-        <v>62</v>
       </c>
       <c r="D58">
         <v>31030.032459999999</v>
@@ -3006,10 +3004,10 @@
         <v>250</v>
       </c>
       <c r="B59" t="s">
+        <v>63</v>
+      </c>
+      <c r="C59" t="s">
         <v>243</v>
-      </c>
-      <c r="C59" t="s">
-        <v>63</v>
       </c>
       <c r="D59">
         <v>33335.619509999997</v>
@@ -3032,10 +3030,10 @@
         <v>266</v>
       </c>
       <c r="B60" t="s">
+        <v>64</v>
+      </c>
+      <c r="C60" t="s">
         <v>244</v>
-      </c>
-      <c r="C60" t="s">
-        <v>64</v>
       </c>
       <c r="D60">
         <v>6909.8905340000001</v>
@@ -3058,10 +3056,10 @@
         <v>270</v>
       </c>
       <c r="B61" t="s">
+        <v>65</v>
+      </c>
+      <c r="C61" t="s">
         <v>245</v>
-      </c>
-      <c r="C61" t="s">
-        <v>65</v>
       </c>
       <c r="D61">
         <v>2148.5698600000001</v>
@@ -3084,10 +3082,10 @@
         <v>268</v>
       </c>
       <c r="B62" t="s">
+        <v>66</v>
+      </c>
+      <c r="C62" t="s">
         <v>246</v>
-      </c>
-      <c r="C62" t="s">
-        <v>66</v>
       </c>
       <c r="D62">
         <v>1385.1740259999999</v>
@@ -3110,10 +3108,10 @@
         <v>276</v>
       </c>
       <c r="B63" t="s">
+        <v>67</v>
+      </c>
+      <c r="C63" t="s">
         <v>247</v>
-      </c>
-      <c r="C63" t="s">
-        <v>67</v>
       </c>
       <c r="D63">
         <v>29803.067869999999</v>
@@ -3136,10 +3134,10 @@
         <v>288</v>
       </c>
       <c r="B64" t="s">
+        <v>68</v>
+      </c>
+      <c r="C64" t="s">
         <v>248</v>
-      </c>
-      <c r="C64" t="s">
-        <v>68</v>
       </c>
       <c r="D64">
         <v>2710.9540280000001</v>
@@ -3162,10 +3160,10 @@
         <v>300</v>
       </c>
       <c r="B65" t="s">
+        <v>69</v>
+      </c>
+      <c r="C65" t="s">
         <v>249</v>
-      </c>
-      <c r="C65" t="s">
-        <v>69</v>
       </c>
       <c r="D65">
         <v>29077.54003</v>
@@ -3188,10 +3186,10 @@
         <v>308</v>
       </c>
       <c r="B66" t="s">
+        <v>70</v>
+      </c>
+      <c r="C66" t="s">
         <v>250</v>
-      </c>
-      <c r="C66" t="s">
-        <v>70</v>
       </c>
       <c r="D66">
         <v>4883.9789280000005</v>
@@ -3214,10 +3212,10 @@
         <v>320</v>
       </c>
       <c r="B67" t="s">
+        <v>71</v>
+      </c>
+      <c r="C67" t="s">
         <v>251</v>
-      </c>
-      <c r="C67" t="s">
-        <v>71</v>
       </c>
       <c r="D67">
         <v>3906.249722</v>
@@ -3240,10 +3238,10 @@
         <v>324</v>
       </c>
       <c r="B68" t="s">
+        <v>72</v>
+      </c>
+      <c r="C68" t="s">
         <v>252</v>
-      </c>
-      <c r="C68" t="s">
-        <v>72</v>
       </c>
       <c r="D68">
         <v>1909.5328030000001</v>
@@ -3266,10 +3264,10 @@
         <v>624</v>
       </c>
       <c r="B69" t="s">
+        <v>73</v>
+      </c>
+      <c r="C69" t="s">
         <v>253</v>
-      </c>
-      <c r="C69" t="s">
-        <v>73</v>
       </c>
       <c r="D69">
         <v>1350.587417</v>
@@ -3292,10 +3290,10 @@
         <v>328</v>
       </c>
       <c r="B70" t="s">
+        <v>74</v>
+      </c>
+      <c r="C70" t="s">
         <v>254</v>
-      </c>
-      <c r="C70" t="s">
-        <v>74</v>
       </c>
       <c r="D70">
         <v>2892.34123</v>
@@ -3318,10 +3316,10 @@
         <v>332</v>
       </c>
       <c r="B71" t="s">
+        <v>75</v>
+      </c>
+      <c r="C71" t="s">
         <v>255</v>
-      </c>
-      <c r="C71" t="s">
-        <v>75</v>
       </c>
       <c r="D71">
         <v>1531.636375</v>
@@ -3344,10 +3342,10 @@
         <v>340</v>
       </c>
       <c r="B72" t="s">
+        <v>76</v>
+      </c>
+      <c r="C72" t="s">
         <v>256</v>
-      </c>
-      <c r="C72" t="s">
-        <v>76</v>
       </c>
       <c r="D72">
         <v>2591.560645</v>
@@ -3370,10 +3368,10 @@
         <v>348</v>
       </c>
       <c r="B73" t="s">
+        <v>77</v>
+      </c>
+      <c r="C73" t="s">
         <v>257</v>
-      </c>
-      <c r="C73" t="s">
-        <v>77</v>
       </c>
       <c r="D73">
         <v>8657.0286290000004</v>
@@ -3396,10 +3394,10 @@
         <v>352</v>
       </c>
       <c r="B74" t="s">
+        <v>78</v>
+      </c>
+      <c r="C74" t="s">
         <v>258</v>
-      </c>
-      <c r="C74" t="s">
-        <v>78</v>
       </c>
       <c r="D74">
         <v>36036.018799999998</v>
@@ -3422,10 +3420,10 @@
         <v>356</v>
       </c>
       <c r="B75" t="s">
+        <v>79</v>
+      </c>
+      <c r="C75" t="s">
         <v>259</v>
-      </c>
-      <c r="C75" t="s">
-        <v>79</v>
       </c>
       <c r="D75">
         <v>1586.180746</v>
@@ -3448,10 +3446,10 @@
         <v>360</v>
       </c>
       <c r="B76" t="s">
+        <v>80</v>
+      </c>
+      <c r="C76" t="s">
         <v>260</v>
-      </c>
-      <c r="C76" t="s">
-        <v>80</v>
       </c>
       <c r="D76">
         <v>1429.5266899999999</v>
@@ -3474,10 +3472,10 @@
         <v>364</v>
       </c>
       <c r="B77" t="s">
+        <v>81</v>
+      </c>
+      <c r="C77" t="s">
         <v>261</v>
-      </c>
-      <c r="C77" t="s">
-        <v>81</v>
       </c>
       <c r="D77">
         <v>4146.2617469999996</v>
@@ -3500,10 +3498,10 @@
         <v>368</v>
       </c>
       <c r="B78" t="s">
+        <v>82</v>
+      </c>
+      <c r="C78" t="s">
         <v>262</v>
-      </c>
-      <c r="C78" t="s">
-        <v>82</v>
       </c>
       <c r="D78">
         <v>2300.6822099999999</v>
@@ -3526,10 +3524,10 @@
         <v>372</v>
       </c>
       <c r="B79" t="s">
+        <v>83</v>
+      </c>
+      <c r="C79" t="s">
         <v>263</v>
-      </c>
-      <c r="C79" t="s">
-        <v>83</v>
       </c>
       <c r="D79">
         <v>34158.062749999997</v>
@@ -3552,10 +3550,10 @@
         <v>376</v>
       </c>
       <c r="B80" t="s">
+        <v>84</v>
+      </c>
+      <c r="C80" t="s">
         <v>264</v>
-      </c>
-      <c r="C80" t="s">
-        <v>84</v>
       </c>
       <c r="D80">
         <v>24895.508900000001</v>
@@ -3578,10 +3576,10 @@
         <v>380</v>
       </c>
       <c r="B81" t="s">
+        <v>85</v>
+      </c>
+      <c r="C81" t="s">
         <v>265</v>
-      </c>
-      <c r="C81" t="s">
-        <v>85</v>
       </c>
       <c r="D81">
         <v>28549.186610000001</v>
@@ -3604,10 +3602,10 @@
         <v>388</v>
       </c>
       <c r="B82" t="s">
+        <v>86</v>
+      </c>
+      <c r="C82" t="s">
         <v>266</v>
-      </c>
-      <c r="C82" t="s">
-        <v>86</v>
       </c>
       <c r="D82">
         <v>4886.4539580000001</v>
@@ -3630,10 +3628,10 @@
         <v>392</v>
       </c>
       <c r="B83" t="s">
+        <v>87</v>
+      </c>
+      <c r="C83" t="s">
         <v>267</v>
-      </c>
-      <c r="C83" t="s">
-        <v>87</v>
       </c>
       <c r="D83">
         <v>33170.215499999998</v>
@@ -3656,10 +3654,10 @@
         <v>400</v>
       </c>
       <c r="B84" t="s">
+        <v>88</v>
+      </c>
+      <c r="C84" t="s">
         <v>268</v>
-      </c>
-      <c r="C84" t="s">
-        <v>88</v>
       </c>
       <c r="D84">
         <v>3971.082977</v>
@@ -3682,10 +3680,10 @@
         <v>398</v>
       </c>
       <c r="B85" t="s">
+        <v>89</v>
+      </c>
+      <c r="C85" t="s">
         <v>269</v>
-      </c>
-      <c r="C85" t="s">
-        <v>89</v>
       </c>
       <c r="D85">
         <v>3180.9842870000002</v>
@@ -3708,10 +3706,10 @@
         <v>404</v>
       </c>
       <c r="B86" t="s">
+        <v>90</v>
+      </c>
+      <c r="C86" t="s">
         <v>270</v>
-      </c>
-      <c r="C86" t="s">
-        <v>90</v>
       </c>
       <c r="D86">
         <v>2844.553911</v>
@@ -3734,10 +3732,10 @@
         <v>414</v>
       </c>
       <c r="B87" t="s">
+        <v>91</v>
+      </c>
+      <c r="C87" t="s">
         <v>271</v>
-      </c>
-      <c r="C87" t="s">
-        <v>91</v>
       </c>
       <c r="D87">
         <v>33139.442020000002</v>
@@ -3760,10 +3758,10 @@
         <v>417</v>
       </c>
       <c r="B88" t="s">
+        <v>92</v>
+      </c>
+      <c r="C88" t="s">
         <v>272</v>
-      </c>
-      <c r="C88" t="s">
-        <v>92</v>
       </c>
       <c r="D88">
         <v>482.79030130000001</v>
@@ -3786,10 +3784,10 @@
         <v>418</v>
       </c>
       <c r="B89" t="s">
+        <v>93</v>
+      </c>
+      <c r="C89" t="s">
         <v>273</v>
-      </c>
-      <c r="C89" t="s">
-        <v>93</v>
       </c>
       <c r="D89">
         <v>1036.730249</v>
@@ -3812,10 +3810,10 @@
         <v>428</v>
       </c>
       <c r="B90" t="s">
+        <v>94</v>
+      </c>
+      <c r="C90" t="s">
         <v>274</v>
-      </c>
-      <c r="C90" t="s">
-        <v>94</v>
       </c>
       <c r="D90">
         <v>5671.2560830000002</v>
@@ -3838,10 +3836,10 @@
         <v>422</v>
       </c>
       <c r="B91" t="s">
+        <v>95</v>
+      </c>
+      <c r="C91" t="s">
         <v>275</v>
-      </c>
-      <c r="C91" t="s">
-        <v>95</v>
       </c>
       <c r="D91">
         <v>7974.6597199999997</v>
@@ -3864,10 +3862,10 @@
         <v>426</v>
       </c>
       <c r="B92" t="s">
+        <v>96</v>
+      </c>
+      <c r="C92" t="s">
         <v>276</v>
-      </c>
-      <c r="C92" t="s">
-        <v>96</v>
       </c>
       <c r="D92">
         <v>3088.4990200000002</v>
@@ -3890,10 +3888,10 @@
         <v>430</v>
       </c>
       <c r="B93" t="s">
+        <v>97</v>
+      </c>
+      <c r="C93" t="s">
         <v>277</v>
-      </c>
-      <c r="C93" t="s">
-        <v>97</v>
       </c>
       <c r="D93">
         <v>1125.193217</v>
@@ -3916,10 +3914,10 @@
         <v>434</v>
       </c>
       <c r="B94" t="s">
+        <v>98</v>
+      </c>
+      <c r="C94" t="s">
         <v>278</v>
-      </c>
-      <c r="C94" t="s">
-        <v>98</v>
       </c>
       <c r="D94">
         <v>9690.2444699999996</v>
@@ -3942,10 +3940,10 @@
         <v>440</v>
       </c>
       <c r="B95" t="s">
+        <v>99</v>
+      </c>
+      <c r="C95" t="s">
         <v>279</v>
-      </c>
-      <c r="C95" t="s">
-        <v>99</v>
       </c>
       <c r="D95">
         <v>6145.9930080000004</v>
@@ -3968,10 +3966,10 @@
         <v>442</v>
       </c>
       <c r="B96" t="s">
+        <v>100</v>
+      </c>
+      <c r="C96" t="s">
         <v>280</v>
-      </c>
-      <c r="C96" t="s">
-        <v>100</v>
       </c>
       <c r="D96">
         <v>41586.225539999999</v>
@@ -3994,10 +3992,10 @@
         <v>450</v>
       </c>
       <c r="B97" t="s">
+        <v>101</v>
+      </c>
+      <c r="C97" t="s">
         <v>281</v>
-      </c>
-      <c r="C97" t="s">
-        <v>101</v>
       </c>
       <c r="D97">
         <v>1524.5627320000001</v>
@@ -4020,10 +4018,10 @@
         <v>454</v>
       </c>
       <c r="B98" t="s">
+        <v>102</v>
+      </c>
+      <c r="C98" t="s">
         <v>282</v>
-      </c>
-      <c r="C98" t="s">
-        <v>102</v>
       </c>
       <c r="D98">
         <v>1747.4617579999999</v>
@@ -4046,10 +4044,10 @@
         <v>458</v>
       </c>
       <c r="B99" t="s">
+        <v>103</v>
+      </c>
+      <c r="C99" t="s">
         <v>283</v>
-      </c>
-      <c r="C99" t="s">
-        <v>103</v>
       </c>
       <c r="D99">
         <v>3211.7106410000001</v>
@@ -4072,10 +4070,10 @@
         <v>462</v>
       </c>
       <c r="B100" t="s">
+        <v>104</v>
+      </c>
+      <c r="C100" t="s">
         <v>284</v>
-      </c>
-      <c r="C100" t="s">
-        <v>104</v>
       </c>
       <c r="D100">
         <v>2399.3182320000001</v>
@@ -4098,10 +4096,10 @@
         <v>466</v>
       </c>
       <c r="B101" t="s">
+        <v>105</v>
+      </c>
+      <c r="C101" t="s">
         <v>285</v>
-      </c>
-      <c r="C101" t="s">
-        <v>105</v>
       </c>
       <c r="D101">
         <v>2063.9447610000002</v>
@@ -4124,10 +4122,10 @@
         <v>470</v>
       </c>
       <c r="B102" t="s">
+        <v>106</v>
+      </c>
+      <c r="C102" t="s">
         <v>286</v>
-      </c>
-      <c r="C102" t="s">
-        <v>106</v>
       </c>
       <c r="D102">
         <v>20906.509959999999</v>
@@ -4150,10 +4148,10 @@
         <v>478</v>
       </c>
       <c r="B103" t="s">
+        <v>107</v>
+      </c>
+      <c r="C103" t="s">
         <v>287</v>
-      </c>
-      <c r="C103" t="s">
-        <v>107</v>
       </c>
       <c r="D103">
         <v>2177.6893439999999</v>
@@ -4176,10 +4174,10 @@
         <v>480</v>
       </c>
       <c r="B104" t="s">
+        <v>108</v>
+      </c>
+      <c r="C104" t="s">
         <v>288</v>
-      </c>
-      <c r="C104" t="s">
-        <v>108</v>
       </c>
       <c r="D104">
         <v>5696.2677720000002</v>
@@ -4202,10 +4200,10 @@
         <v>484</v>
       </c>
       <c r="B105" t="s">
+        <v>109</v>
+      </c>
+      <c r="C105" t="s">
         <v>289</v>
-      </c>
-      <c r="C105" t="s">
-        <v>109</v>
       </c>
       <c r="D105">
         <v>6031.9367149999998</v>
@@ -4228,10 +4226,10 @@
         <v>583</v>
       </c>
       <c r="B106" t="s">
+        <v>110</v>
+      </c>
+      <c r="C106" t="s">
         <v>365</v>
-      </c>
-      <c r="C106" t="s">
-        <v>110</v>
       </c>
       <c r="D106">
         <v>1932.379668</v>
@@ -4254,10 +4252,10 @@
         <v>496</v>
       </c>
       <c r="B107" t="s">
+        <v>111</v>
+      </c>
+      <c r="C107" t="s">
         <v>290</v>
-      </c>
-      <c r="C107" t="s">
-        <v>111</v>
       </c>
       <c r="D107">
         <v>1106.7177180000001</v>
@@ -4280,10 +4278,10 @@
         <v>504</v>
       </c>
       <c r="B108" t="s">
+        <v>112</v>
+      </c>
+      <c r="C108" t="s">
         <v>292</v>
-      </c>
-      <c r="C108" t="s">
-        <v>112</v>
       </c>
       <c r="D108">
         <v>2849.6225300000001</v>
@@ -4306,10 +4304,10 @@
         <v>508</v>
       </c>
       <c r="B109" t="s">
+        <v>113</v>
+      </c>
+      <c r="C109" t="s">
         <v>293</v>
-      </c>
-      <c r="C109" t="s">
-        <v>113</v>
       </c>
       <c r="D109">
         <v>1639.7410950000001</v>
@@ -4332,10 +4330,10 @@
         <v>104</v>
       </c>
       <c r="B110" t="s">
+        <v>114</v>
+      </c>
+      <c r="C110" t="s">
         <v>294</v>
-      </c>
-      <c r="C110" t="s">
-        <v>114</v>
       </c>
       <c r="D110">
         <v>596.42109889999995</v>
@@ -4358,10 +4356,10 @@
         <v>516</v>
       </c>
       <c r="B111" t="s">
+        <v>115</v>
+      </c>
+      <c r="C111" t="s">
         <v>295</v>
-      </c>
-      <c r="C111" t="s">
-        <v>115</v>
       </c>
       <c r="D111">
         <v>5502.1059560000003</v>
@@ -4384,10 +4382,10 @@
         <v>524</v>
       </c>
       <c r="B112" t="s">
+        <v>116</v>
+      </c>
+      <c r="C112" t="s">
         <v>296</v>
-      </c>
-      <c r="C112" t="s">
-        <v>116</v>
       </c>
       <c r="D112">
         <v>1088.3832150000001</v>
@@ -4410,10 +4408,10 @@
         <v>528</v>
       </c>
       <c r="B113" t="s">
+        <v>117</v>
+      </c>
+      <c r="C113" t="s">
         <v>297</v>
-      </c>
-      <c r="C113" t="s">
-        <v>117</v>
       </c>
       <c r="D113">
         <v>31616.823609999999</v>
@@ -4436,10 +4434,10 @@
         <v>554</v>
       </c>
       <c r="B114" t="s">
+        <v>118</v>
+      </c>
+      <c r="C114" t="s">
         <v>298</v>
-      </c>
-      <c r="C114" t="s">
-        <v>118</v>
       </c>
       <c r="D114">
         <v>27227.750390000001</v>
@@ -4462,10 +4460,10 @@
         <v>558</v>
       </c>
       <c r="B115" t="s">
+        <v>119</v>
+      </c>
+      <c r="C115" t="s">
         <v>299</v>
-      </c>
-      <c r="C115" t="s">
-        <v>119</v>
       </c>
       <c r="D115">
         <v>2176.467392</v>
@@ -4488,10 +4486,10 @@
         <v>562</v>
       </c>
       <c r="B116" t="s">
+        <v>120</v>
+      </c>
+      <c r="C116" t="s">
         <v>300</v>
-      </c>
-      <c r="C116" t="s">
-        <v>120</v>
       </c>
       <c r="D116">
         <v>1474.8773169999999</v>
@@ -4514,10 +4512,10 @@
         <v>566</v>
       </c>
       <c r="B117" t="s">
+        <v>121</v>
+      </c>
+      <c r="C117" t="s">
         <v>301</v>
-      </c>
-      <c r="C117" t="s">
-        <v>121</v>
       </c>
       <c r="D117">
         <v>3292.3060869999999</v>
@@ -4540,10 +4538,10 @@
         <v>578</v>
       </c>
       <c r="B118" t="s">
+        <v>122</v>
+      </c>
+      <c r="C118" t="s">
         <v>302</v>
-      </c>
-      <c r="C118" t="s">
-        <v>122</v>
       </c>
       <c r="D118">
         <v>38803.423320000002</v>
@@ -4566,10 +4564,10 @@
         <v>512</v>
       </c>
       <c r="B119" t="s">
+        <v>123</v>
+      </c>
+      <c r="C119" t="s">
         <v>303</v>
-      </c>
-      <c r="C119" t="s">
-        <v>123</v>
       </c>
       <c r="D119">
         <v>16418.835650000001</v>
@@ -4592,10 +4590,10 @@
         <v>586</v>
       </c>
       <c r="B120" t="s">
+        <v>124</v>
+      </c>
+      <c r="C120" t="s">
         <v>304</v>
-      </c>
-      <c r="C120" t="s">
-        <v>124</v>
       </c>
       <c r="D120">
         <v>1948.9608780000001</v>
@@ -4618,10 +4616,10 @@
         <v>591</v>
       </c>
       <c r="B121" t="s">
+        <v>125</v>
+      </c>
+      <c r="C121" t="s">
         <v>305</v>
-      </c>
-      <c r="C121" t="s">
-        <v>125</v>
       </c>
       <c r="D121">
         <v>4719.319759</v>
@@ -4644,10 +4642,10 @@
         <v>598</v>
       </c>
       <c r="B122" t="s">
+        <v>126</v>
+      </c>
+      <c r="C122" t="s">
         <v>306</v>
-      </c>
-      <c r="C122" t="s">
-        <v>126</v>
       </c>
       <c r="D122">
         <v>1195.740865</v>
@@ -4670,10 +4668,10 @@
         <v>600</v>
       </c>
       <c r="B123" t="s">
+        <v>127</v>
+      </c>
+      <c r="C123" t="s">
         <v>307</v>
-      </c>
-      <c r="C123" t="s">
-        <v>127</v>
       </c>
       <c r="D123">
         <v>2608.9239729999999</v>
@@ -4696,10 +4694,10 @@
         <v>604</v>
       </c>
       <c r="B124" t="s">
+        <v>128</v>
+      </c>
+      <c r="C124" t="s">
         <v>308</v>
-      </c>
-      <c r="C124" t="s">
-        <v>128</v>
       </c>
       <c r="D124">
         <v>3787.009423</v>
@@ -4722,10 +4720,10 @@
         <v>608</v>
       </c>
       <c r="B125" t="s">
+        <v>129</v>
+      </c>
+      <c r="C125" t="s">
         <v>309</v>
-      </c>
-      <c r="C125" t="s">
-        <v>129</v>
       </c>
       <c r="D125">
         <v>1876.52367</v>
@@ -4748,10 +4746,10 @@
         <v>616</v>
       </c>
       <c r="B126" t="s">
+        <v>130</v>
+      </c>
+      <c r="C126" t="s">
         <v>310</v>
-      </c>
-      <c r="C126" t="s">
-        <v>130</v>
       </c>
       <c r="D126">
         <v>6243.9956570000004</v>
@@ -4774,10 +4772,10 @@
         <v>620</v>
       </c>
       <c r="B127" t="s">
+        <v>131</v>
+      </c>
+      <c r="C127" t="s">
         <v>311</v>
-      </c>
-      <c r="C127" t="s">
-        <v>131</v>
       </c>
       <c r="D127">
         <v>23357.211210000001</v>
@@ -4800,10 +4798,10 @@
         <v>634</v>
       </c>
       <c r="B128" t="s">
+        <v>132</v>
+      </c>
+      <c r="C128" t="s">
         <v>312</v>
-      </c>
-      <c r="C128" t="s">
-        <v>132</v>
       </c>
       <c r="D128">
         <v>52066.675309999999</v>
@@ -4826,10 +4824,10 @@
         <v>410</v>
       </c>
       <c r="B129" t="s">
+        <v>133</v>
+      </c>
+      <c r="C129" t="s">
         <v>313</v>
-      </c>
-      <c r="C129" t="s">
-        <v>133</v>
       </c>
       <c r="D129">
         <v>4987.9632769999998</v>
@@ -4852,10 +4850,10 @@
         <v>498</v>
       </c>
       <c r="B130" t="s">
+        <v>134</v>
+      </c>
+      <c r="C130" t="s">
         <v>314</v>
-      </c>
-      <c r="C130" t="s">
-        <v>134</v>
       </c>
       <c r="D130">
         <v>693.72554709999997</v>
@@ -4878,10 +4876,10 @@
         <v>499</v>
       </c>
       <c r="B131" t="s">
+        <v>135</v>
+      </c>
+      <c r="C131" t="s">
         <v>291</v>
-      </c>
-      <c r="C131" t="s">
-        <v>135</v>
       </c>
       <c r="D131">
         <v>3110.2957219999998</v>
@@ -4904,10 +4902,10 @@
         <v>688</v>
       </c>
       <c r="B132" t="s">
+        <v>136</v>
+      </c>
+      <c r="C132" t="s">
         <v>324</v>
-      </c>
-      <c r="C132" t="s">
-        <v>136</v>
       </c>
       <c r="D132">
         <v>2301.7158140000001</v>
@@ -4930,10 +4928,10 @@
         <v>642</v>
       </c>
       <c r="B133" t="s">
+        <v>137</v>
+      </c>
+      <c r="C133" t="s">
         <v>315</v>
-      </c>
-      <c r="C133" t="s">
-        <v>137</v>
       </c>
       <c r="D133">
         <v>3722.4966250000002</v>
@@ -4956,10 +4954,10 @@
         <v>643</v>
       </c>
       <c r="B134" t="s">
+        <v>138</v>
+      </c>
+      <c r="C134" t="s">
         <v>316</v>
-      </c>
-      <c r="C134" t="s">
-        <v>138</v>
       </c>
       <c r="D134">
         <v>4240.3737659999997</v>
@@ -4982,10 +4980,10 @@
         <v>646</v>
       </c>
       <c r="B135" t="s">
+        <v>139</v>
+      </c>
+      <c r="C135" t="s">
         <v>317</v>
-      </c>
-      <c r="C135" t="s">
-        <v>139</v>
       </c>
       <c r="D135">
         <v>2100.3044989999999</v>
@@ -5008,10 +5006,10 @@
         <v>662</v>
       </c>
       <c r="B136" t="s">
+        <v>140</v>
+      </c>
+      <c r="C136" t="s">
         <v>318</v>
-      </c>
-      <c r="C136" t="s">
-        <v>140</v>
       </c>
       <c r="D136">
         <v>5571.9574389999998</v>
@@ -5034,10 +5032,10 @@
         <v>670</v>
       </c>
       <c r="B137" t="s">
+        <v>141</v>
+      </c>
+      <c r="C137" t="s">
         <v>319</v>
-      </c>
-      <c r="C137" t="s">
-        <v>141</v>
       </c>
       <c r="D137">
         <v>4706.9540630000001</v>
@@ -5060,10 +5058,10 @@
         <v>678</v>
       </c>
       <c r="B138" t="s">
+        <v>142</v>
+      </c>
+      <c r="C138" t="s">
         <v>321</v>
-      </c>
-      <c r="C138" t="s">
-        <v>142</v>
       </c>
       <c r="D138">
         <v>1679.68515</v>
@@ -5086,10 +5084,10 @@
         <v>882</v>
       </c>
       <c r="B139" t="s">
+        <v>143</v>
+      </c>
+      <c r="C139" t="s">
         <v>320</v>
-      </c>
-      <c r="C139" t="s">
-        <v>143</v>
       </c>
       <c r="D139">
         <v>2343.307863</v>
@@ -5112,10 +5110,10 @@
         <v>682</v>
       </c>
       <c r="B140" t="s">
+        <v>144</v>
+      </c>
+      <c r="C140" t="s">
         <v>322</v>
-      </c>
-      <c r="C140" t="s">
-        <v>144</v>
       </c>
       <c r="D140">
         <v>18079.79391</v>
@@ -5138,10 +5136,10 @@
         <v>686</v>
       </c>
       <c r="B141" t="s">
+        <v>145</v>
+      </c>
+      <c r="C141" t="s">
         <v>323</v>
-      </c>
-      <c r="C141" t="s">
-        <v>145</v>
       </c>
       <c r="D141">
         <v>2467.4052660000002</v>
@@ -5164,10 +5162,10 @@
         <v>694</v>
       </c>
       <c r="B142" t="s">
+        <v>146</v>
+      </c>
+      <c r="C142" t="s">
         <v>325</v>
-      </c>
-      <c r="C142" t="s">
-        <v>146</v>
       </c>
       <c r="D142">
         <v>1327.0855449999999</v>
@@ -5190,10 +5188,10 @@
         <v>702</v>
       </c>
       <c r="B143" t="s">
+        <v>147</v>
+      </c>
+      <c r="C143" t="s">
         <v>326</v>
-      </c>
-      <c r="C143" t="s">
-        <v>147</v>
       </c>
       <c r="D143">
         <v>27939.151470000001</v>
@@ -5216,10 +5214,10 @@
         <v>703</v>
       </c>
       <c r="B144" t="s">
+        <v>148</v>
+      </c>
+      <c r="C144" t="s">
         <v>327</v>
-      </c>
-      <c r="C144" t="s">
-        <v>148</v>
       </c>
       <c r="D144">
         <v>6767.4414850000003</v>
@@ -5242,10 +5240,10 @@
         <v>705</v>
       </c>
       <c r="B145" t="s">
+        <v>149</v>
+      </c>
+      <c r="C145" t="s">
         <v>328</v>
-      </c>
-      <c r="C145" t="s">
-        <v>149</v>
       </c>
       <c r="D145">
         <v>22825.905900000002</v>
@@ -5268,10 +5266,10 @@
         <v>90</v>
       </c>
       <c r="B146" t="s">
+        <v>150</v>
+      </c>
+      <c r="C146" t="s">
         <v>329</v>
-      </c>
-      <c r="C146" t="s">
-        <v>150</v>
       </c>
       <c r="D146">
         <v>1427.640236</v>
@@ -5294,10 +5292,10 @@
         <v>706</v>
       </c>
       <c r="B147" t="s">
+        <v>151</v>
+      </c>
+      <c r="C147" t="s">
         <v>330</v>
-      </c>
-      <c r="C147" t="s">
-        <v>151</v>
       </c>
       <c r="D147">
         <v>1029.87987</v>
@@ -5320,10 +5318,10 @@
         <v>710</v>
       </c>
       <c r="B148" t="s">
+        <v>152</v>
+      </c>
+      <c r="C148" t="s">
         <v>331</v>
-      </c>
-      <c r="C148" t="s">
-        <v>152</v>
       </c>
       <c r="D148">
         <v>6648.3923379999997</v>
@@ -5346,10 +5344,10 @@
         <v>728</v>
       </c>
       <c r="B149" t="s">
+        <v>153</v>
+      </c>
+      <c r="C149" t="s">
         <v>332</v>
-      </c>
-      <c r="C149" t="s">
-        <v>153</v>
       </c>
       <c r="D149">
         <v>2063.6994129999998</v>
@@ -5372,10 +5370,10 @@
         <v>724</v>
       </c>
       <c r="B150" t="s">
+        <v>154</v>
+      </c>
+      <c r="C150" t="s">
         <v>333</v>
-      </c>
-      <c r="C150" t="s">
-        <v>154</v>
       </c>
       <c r="D150">
         <v>26643.357609999999</v>
@@ -5398,10 +5396,10 @@
         <v>144</v>
       </c>
       <c r="B151" t="s">
+        <v>155</v>
+      </c>
+      <c r="C151" t="s">
         <v>334</v>
-      </c>
-      <c r="C151" t="s">
-        <v>155</v>
       </c>
       <c r="D151">
         <v>1796.936854</v>
@@ -5424,10 +5422,10 @@
         <v>729</v>
       </c>
       <c r="B152" t="s">
+        <v>156</v>
+      </c>
+      <c r="C152" t="s">
         <v>335</v>
-      </c>
-      <c r="C152" t="s">
-        <v>156</v>
       </c>
       <c r="D152">
         <v>2063.6994129999998</v>
@@ -5450,10 +5448,10 @@
         <v>740</v>
       </c>
       <c r="B153" t="s">
+        <v>157</v>
+      </c>
+      <c r="C153" t="s">
         <v>336</v>
-      </c>
-      <c r="C153" t="s">
-        <v>157</v>
       </c>
       <c r="D153">
         <v>4370.1155319999998</v>
@@ -5476,10 +5474,10 @@
         <v>748</v>
       </c>
       <c r="B154" t="s">
+        <v>158</v>
+      </c>
+      <c r="C154" t="s">
         <v>337</v>
-      </c>
-      <c r="C154" t="s">
-        <v>158</v>
       </c>
       <c r="D154">
         <v>4943.2836719999996</v>
@@ -5502,10 +5500,10 @@
         <v>752</v>
       </c>
       <c r="B155" t="s">
+        <v>159</v>
+      </c>
+      <c r="C155" t="s">
         <v>338</v>
-      </c>
-      <c r="C155" t="s">
-        <v>159</v>
       </c>
       <c r="D155">
         <v>31810.672740000002</v>
@@ -5528,10 +5526,10 @@
         <v>756</v>
       </c>
       <c r="B156" t="s">
+        <v>160</v>
+      </c>
+      <c r="C156" t="s">
         <v>339</v>
-      </c>
-      <c r="C156" t="s">
-        <v>160</v>
       </c>
       <c r="D156">
         <v>34963.765489999998</v>
@@ -5554,10 +5552,10 @@
         <v>760</v>
       </c>
       <c r="B157" t="s">
+        <v>161</v>
+      </c>
+      <c r="C157" t="s">
         <v>340</v>
-      </c>
-      <c r="C157" t="s">
-        <v>161</v>
       </c>
       <c r="D157">
         <v>2624.4972760000001</v>
@@ -5580,10 +5578,10 @@
         <v>762</v>
       </c>
       <c r="B158" t="s">
+        <v>162</v>
+      </c>
+      <c r="C158" t="s">
         <v>341</v>
-      </c>
-      <c r="C158" t="s">
-        <v>162</v>
       </c>
       <c r="D158">
         <v>419.40103909999999</v>
@@ -5606,10 +5604,10 @@
         <v>764</v>
       </c>
       <c r="B159" t="s">
+        <v>163</v>
+      </c>
+      <c r="C159" t="s">
         <v>342</v>
-      </c>
-      <c r="C159" t="s">
-        <v>163</v>
       </c>
       <c r="D159">
         <v>2037.083288</v>
@@ -5632,10 +5630,10 @@
         <v>626</v>
       </c>
       <c r="B160" t="s">
+        <v>164</v>
+      </c>
+      <c r="C160" t="s">
         <v>343</v>
-      </c>
-      <c r="C160" t="s">
-        <v>164</v>
       </c>
       <c r="D160">
         <v>790.18065720000004</v>
@@ -5658,10 +5656,10 @@
         <v>768</v>
       </c>
       <c r="B161" t="s">
+        <v>165</v>
+      </c>
+      <c r="C161" t="s">
         <v>344</v>
-      </c>
-      <c r="C161" t="s">
-        <v>165</v>
       </c>
       <c r="D161">
         <v>1736.1788140000001</v>
@@ -5684,10 +5682,10 @@
         <v>776</v>
       </c>
       <c r="B162" t="s">
+        <v>166</v>
+      </c>
+      <c r="C162" t="s">
         <v>345</v>
-      </c>
-      <c r="C162" t="s">
-        <v>166</v>
       </c>
       <c r="D162">
         <v>1951.2262109999999</v>
@@ -5710,10 +5708,10 @@
         <v>780</v>
       </c>
       <c r="B163" t="s">
+        <v>167</v>
+      </c>
+      <c r="C163" t="s">
         <v>346</v>
-      </c>
-      <c r="C163" t="s">
-        <v>167</v>
       </c>
       <c r="D163">
         <v>7230.0781989999996</v>
@@ -5736,10 +5734,10 @@
         <v>788</v>
       </c>
       <c r="B164" t="s">
+        <v>168</v>
+      </c>
+      <c r="C164" t="s">
         <v>347</v>
-      </c>
-      <c r="C164" t="s">
-        <v>168</v>
       </c>
       <c r="D164">
         <v>4300.127778</v>
@@ -5762,10 +5760,10 @@
         <v>792</v>
       </c>
       <c r="B165" t="s">
+        <v>169</v>
+      </c>
+      <c r="C165" t="s">
         <v>348</v>
-      </c>
-      <c r="C165" t="s">
-        <v>169</v>
       </c>
       <c r="D165">
         <v>4240.0606280000002</v>
@@ -5788,10 +5786,10 @@
         <v>795</v>
       </c>
       <c r="B166" t="s">
+        <v>170</v>
+      </c>
+      <c r="C166" t="s">
         <v>349</v>
-      </c>
-      <c r="C166" t="s">
-        <v>170</v>
       </c>
       <c r="D166">
         <v>2925.1312440000002</v>
@@ -5814,10 +5812,10 @@
         <v>800</v>
       </c>
       <c r="B167" t="s">
+        <v>171</v>
+      </c>
+      <c r="C167" t="s">
         <v>350</v>
-      </c>
-      <c r="C167" t="s">
-        <v>171</v>
       </c>
       <c r="D167">
         <v>2493.6153960000001</v>
@@ -5840,10 +5838,10 @@
         <v>804</v>
       </c>
       <c r="B168" t="s">
+        <v>172</v>
+      </c>
+      <c r="C168" t="s">
         <v>351</v>
-      </c>
-      <c r="C168" t="s">
-        <v>172</v>
       </c>
       <c r="D168">
         <v>1590.3565860000001</v>
@@ -5866,10 +5864,10 @@
         <v>784</v>
       </c>
       <c r="B169" t="s">
+        <v>173</v>
+      </c>
+      <c r="C169" t="s">
         <v>352</v>
-      </c>
-      <c r="C169" t="s">
-        <v>173</v>
       </c>
       <c r="D169">
         <v>32616.51658</v>
@@ -5892,10 +5890,10 @@
         <v>826</v>
       </c>
       <c r="B170" t="s">
+        <v>174</v>
+      </c>
+      <c r="C170" t="s">
         <v>353</v>
-      </c>
-      <c r="C170" t="s">
-        <v>174</v>
       </c>
       <c r="D170">
         <v>30795.30213</v>
@@ -5918,10 +5916,10 @@
         <v>834</v>
       </c>
       <c r="B171" t="s">
+        <v>175</v>
+      </c>
+      <c r="C171" t="s">
         <v>354</v>
-      </c>
-      <c r="C171" t="s">
-        <v>175</v>
       </c>
       <c r="D171">
         <v>2334.1495839999998</v>
@@ -5944,10 +5942,10 @@
         <v>840</v>
       </c>
       <c r="B172" t="s">
+        <v>176</v>
+      </c>
+      <c r="C172" t="s">
         <v>355</v>
-      </c>
-      <c r="C172" t="s">
-        <v>176</v>
       </c>
       <c r="D172">
         <v>33438.211199999998</v>
@@ -5970,10 +5968,10 @@
         <v>858</v>
       </c>
       <c r="B173" t="s">
+        <v>177</v>
+      </c>
+      <c r="C173" t="s">
         <v>356</v>
-      </c>
-      <c r="C173" t="s">
-        <v>177</v>
       </c>
       <c r="D173">
         <v>5014.3105079999996</v>
@@ -5996,10 +5994,10 @@
         <v>860</v>
       </c>
       <c r="B174" t="s">
+        <v>178</v>
+      </c>
+      <c r="C174" t="s">
         <v>357</v>
-      </c>
-      <c r="C174" t="s">
-        <v>178</v>
       </c>
       <c r="D174">
         <v>524.89433740000004</v>
@@ -6022,10 +6020,10 @@
         <v>548</v>
       </c>
       <c r="B175" t="s">
+        <v>179</v>
+      </c>
+      <c r="C175" t="s">
         <v>358</v>
-      </c>
-      <c r="C175" t="s">
-        <v>179</v>
       </c>
       <c r="D175">
         <v>1690.986598</v>
@@ -6048,10 +6046,10 @@
         <v>862</v>
       </c>
       <c r="B176" t="s">
+        <v>180</v>
+      </c>
+      <c r="C176" t="s">
         <v>359</v>
-      </c>
-      <c r="C176" t="s">
-        <v>180</v>
       </c>
       <c r="D176">
         <v>5076.0987480000003</v>
@@ -6074,10 +6072,10 @@
         <v>704</v>
       </c>
       <c r="B177" t="s">
+        <v>181</v>
+      </c>
+      <c r="C177" t="s">
         <v>360</v>
-      </c>
-      <c r="C177" t="s">
-        <v>181</v>
       </c>
       <c r="D177">
         <v>1058.550874</v>
@@ -6100,10 +6098,10 @@
         <v>887</v>
       </c>
       <c r="B178" t="s">
+        <v>182</v>
+      </c>
+      <c r="C178" t="s">
         <v>361</v>
-      </c>
-      <c r="C178" t="s">
-        <v>182</v>
       </c>
       <c r="D178">
         <v>1682.67949</v>
@@ -6126,10 +6124,10 @@
         <v>894</v>
       </c>
       <c r="B179" t="s">
+        <v>183</v>
+      </c>
+      <c r="C179" t="s">
         <v>362</v>
-      </c>
-      <c r="C179" t="s">
-        <v>183</v>
       </c>
       <c r="D179">
         <v>3106.6653160000001</v>
@@ -6152,10 +6150,10 @@
         <v>716</v>
       </c>
       <c r="B180" t="s">
+        <v>184</v>
+      </c>
+      <c r="C180" t="s">
         <v>363</v>
-      </c>
-      <c r="C180" t="s">
-        <v>184</v>
       </c>
       <c r="D180">
         <v>2068.2084049999999</v>

</xml_diff>

<commit_message>
Changed intervention defaults for TB app.
</commit_message>
<xml_diff>
--- a/SourceData/humanresources/HWModData.xlsx
+++ b/SourceData/humanresources/HWModData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proj\SpectrumEngine\DefaultData\SourceData\humanresources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CB6CC9A-C75D-462F-A538-910E641DD400}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBB49640-5288-4CF7-AB8C-2AAB7C482470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="-1095" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="StaffSalariesDB" sheetId="1" r:id="rId1"/>
@@ -1487,7 +1487,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H180"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -1528,19 +1530,19 @@
         <v>186</v>
       </c>
       <c r="D2">
-        <v>970.38318130000005</v>
+        <v>1316.3779576527966</v>
       </c>
       <c r="E2">
-        <v>1265.333529</v>
+        <v>1711.2913449486355</v>
       </c>
       <c r="F2">
-        <v>1670.5213220000001</v>
+        <v>2276.9780889129452</v>
       </c>
       <c r="G2">
-        <v>2704.8210279999998</v>
+        <v>2775.0670458626519</v>
       </c>
       <c r="H2">
-        <v>4060.2142650000001</v>
+        <v>4162.6005687939778</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -1554,19 +1556,19 @@
         <v>187</v>
       </c>
       <c r="D3">
-        <v>2383.926665</v>
+        <v>8290.3640241987869</v>
       </c>
       <c r="E3">
-        <v>3108.5270209999999</v>
+        <v>10777.473231458423</v>
       </c>
       <c r="F3">
-        <v>4103.9461529999999</v>
+        <v>14029.846810182564</v>
       </c>
       <c r="G3">
-        <v>6644.8956410000001</v>
+        <v>17218.448357951329</v>
       </c>
       <c r="H3">
-        <v>9974.6710739999999</v>
+        <v>25827.672536926995</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -1580,19 +1582,19 @@
         <v>188</v>
       </c>
       <c r="D4">
-        <v>4459.8694379999997</v>
+        <v>8880.7552734767578</v>
       </c>
       <c r="E4">
-        <v>5815.4576909999996</v>
+        <v>11544.981855519785</v>
       </c>
       <c r="F4">
-        <v>7677.6959189999998</v>
+        <v>15541.321728584326</v>
       </c>
       <c r="G4">
-        <v>12431.32494</v>
+        <v>18871.604956138108</v>
       </c>
       <c r="H4">
-        <v>18660.695960000001</v>
+        <v>28307.407434207162</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -1606,19 +1608,19 @@
         <v>189</v>
       </c>
       <c r="D5">
-        <v>4069.1682799999999</v>
+        <v>4625.937787970186</v>
       </c>
       <c r="E5">
-        <v>5306.0019579999998</v>
+        <v>6013.7191243612424</v>
       </c>
       <c r="F5">
-        <v>7005.1011879999996</v>
+        <v>8095.3911289478265</v>
       </c>
       <c r="G5">
-        <v>11342.294610000001</v>
+        <v>9830.1177994366462</v>
       </c>
       <c r="H5">
-        <v>17025.949560000001</v>
+        <v>14745.176699154968</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -1632,19 +1634,19 @@
         <v>190</v>
       </c>
       <c r="D6">
-        <v>4839.4223400000001</v>
+        <v>13846.118598564874</v>
       </c>
       <c r="E6">
-        <v>6310.3766290000003</v>
+        <v>17999.954178134336</v>
       </c>
       <c r="F6">
-        <v>8331.0988510000006</v>
+        <v>23431.893012955941</v>
       </c>
       <c r="G6">
-        <v>13489.2809</v>
+        <v>28757.323243173199</v>
       </c>
       <c r="H6">
-        <v>20248.796549999999</v>
+        <v>43135.984864759805</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -1658,19 +1660,19 @@
         <v>191</v>
       </c>
       <c r="D7">
-        <v>1503.3972369999999</v>
+        <v>6464.6181647049216</v>
       </c>
       <c r="E7">
-        <v>1960.358514</v>
+        <v>8404.0036141163982</v>
       </c>
       <c r="F7">
-        <v>2588.108686</v>
+        <v>10940.123047962175</v>
       </c>
       <c r="G7">
-        <v>4190.5306469999996</v>
+        <v>13426.514649771761</v>
       </c>
       <c r="H7">
-        <v>6290.4170489999997</v>
+        <v>20139.771974657644</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -1684,19 +1686,19 @@
         <v>192</v>
       </c>
       <c r="D8">
-        <v>30820.62342</v>
+        <v>54627.520892272099</v>
       </c>
       <c r="E8">
-        <v>40188.627489999999</v>
+        <v>71015.777159953737</v>
       </c>
       <c r="F8">
-        <v>53057.915240000002</v>
+        <v>91045.868153786825</v>
       </c>
       <c r="G8">
-        <v>85908.610050000003</v>
+        <v>115324.76632812998</v>
       </c>
       <c r="H8">
-        <v>128957.6502</v>
+        <v>172987.14949219493</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -1710,19 +1712,19 @@
         <v>193</v>
       </c>
       <c r="D9">
-        <v>30610.24411</v>
+        <v>48166.10140586504</v>
       </c>
       <c r="E9">
-        <v>39914.302880000003</v>
+        <v>62615.931827624554</v>
       </c>
       <c r="F9">
-        <v>52695.745819999996</v>
+        <v>80276.835676441726</v>
       </c>
       <c r="G9">
-        <v>85322.204209999996</v>
+        <v>101683.99185682619</v>
       </c>
       <c r="H9">
-        <v>128077.39479999999</v>
+        <v>152525.98778523927</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -1736,19 +1738,19 @@
         <v>194</v>
       </c>
       <c r="D10">
-        <v>1486.842167</v>
+        <v>7030.4589572752984</v>
       </c>
       <c r="E10">
-        <v>1938.7714900000001</v>
+        <v>9139.596644457888</v>
       </c>
       <c r="F10">
-        <v>2559.609019</v>
+        <v>11897.699773850505</v>
       </c>
       <c r="G10">
-        <v>4144.3854709999996</v>
+        <v>14601.722449725619</v>
       </c>
       <c r="H10">
-        <v>6221.1483989999997</v>
+        <v>21902.583674588433</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -1762,19 +1764,19 @@
         <v>195</v>
       </c>
       <c r="D11">
-        <v>9233.1930790000006</v>
+        <v>25434.389295573001</v>
       </c>
       <c r="E11">
-        <v>12039.644759999999</v>
+        <v>33064.706084244906</v>
       </c>
       <c r="F11">
-        <v>15895.0054</v>
+        <v>42390.648825954995</v>
       </c>
       <c r="G11">
-        <v>25736.364020000001</v>
+        <v>53694.821846209663</v>
       </c>
       <c r="H11">
-        <v>38632.926630000002</v>
+        <v>80542.232769314491</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -1788,19 +1790,19 @@
         <v>196</v>
       </c>
       <c r="D12">
-        <v>21923.596539999999</v>
+        <v>24165.003052413176</v>
       </c>
       <c r="E12">
-        <v>28587.32748</v>
+        <v>31414.503968137131</v>
       </c>
       <c r="F12">
-        <v>37741.62227</v>
+        <v>40275.00508735529</v>
       </c>
       <c r="G12">
-        <v>61109.267019999999</v>
+        <v>51015.006443983366</v>
       </c>
       <c r="H12">
-        <v>91731.288339999999</v>
+        <v>76522.509665975042</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -1814,19 +1816,19 @@
         <v>197</v>
       </c>
       <c r="D13">
-        <v>1255.088741</v>
+        <v>5899.0176944673958</v>
       </c>
       <c r="E13">
-        <v>1636.5760419999999</v>
+        <v>7668.7230028076146</v>
       </c>
       <c r="F13">
-        <v>2160.6439019999998</v>
+        <v>10323.280965317943</v>
       </c>
       <c r="G13">
-        <v>3498.4019560000002</v>
+        <v>12535.412600743215</v>
       </c>
       <c r="H13">
-        <v>5251.4607720000004</v>
+        <v>18803.118901114824</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -1840,19 +1842,19 @@
         <v>198</v>
       </c>
       <c r="D14">
-        <v>6919.8844369999997</v>
+        <v>15756.72119487909</v>
       </c>
       <c r="E14">
-        <v>9023.2002819999998</v>
+        <v>20483.73755334282</v>
       </c>
       <c r="F14">
-        <v>11912.62866</v>
+        <v>26261.20199146515</v>
       </c>
       <c r="G14">
-        <v>19288.307239999998</v>
+        <v>33264.189189189186</v>
       </c>
       <c r="H14">
-        <v>28953.730899999999</v>
+        <v>49896.28378378378</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -1866,19 +1868,19 @@
         <v>199</v>
       </c>
       <c r="D15">
-        <v>2528.5908979999999</v>
+        <v>9736.6346312805472</v>
       </c>
       <c r="E15">
-        <v>3297.1623020000002</v>
+        <v>12657.625020664713</v>
       </c>
       <c r="F15">
-        <v>4352.9866259999999</v>
+        <v>16477.381683705542</v>
       </c>
       <c r="G15">
-        <v>7048.1289900000002</v>
+        <v>20222.241157274984</v>
       </c>
       <c r="H15">
-        <v>10579.965759999999</v>
+        <v>30333.36173591248</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -1892,19 +1894,19 @@
         <v>200</v>
       </c>
       <c r="D16">
-        <v>30866.694469999999</v>
+        <v>46665.357465620655</v>
       </c>
       <c r="E16">
-        <v>40248.701959999999</v>
+        <v>60664.964705306862</v>
       </c>
       <c r="F16">
-        <v>53137.226880000002</v>
+        <v>77775.595776034432</v>
       </c>
       <c r="G16">
-        <v>86037.027329999997</v>
+        <v>98515.754649643597</v>
       </c>
       <c r="H16">
-        <v>129150.41770000001</v>
+        <v>147773.63197446539</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -1918,19 +1920,19 @@
         <v>201</v>
       </c>
       <c r="D17">
-        <v>4578.8636619999997</v>
+        <v>7879.2586904309828</v>
       </c>
       <c r="E17">
-        <v>5970.6205019999998</v>
+        <v>10243.036297560278</v>
       </c>
       <c r="F17">
-        <v>7882.5452949999999</v>
+        <v>13334.130091498588</v>
       </c>
       <c r="G17">
-        <v>12763.006359999999</v>
+        <v>16364.614203202811</v>
       </c>
       <c r="H17">
-        <v>19158.583859999999</v>
+        <v>24546.921304804222</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
@@ -1944,19 +1946,19 @@
         <v>202</v>
       </c>
       <c r="D18">
-        <v>2046.6863249999999</v>
+        <v>3266.1875381158006</v>
       </c>
       <c r="E18">
-        <v>2668.781653</v>
+        <v>4246.0437995505408</v>
       </c>
       <c r="F18">
-        <v>3523.3845879999999</v>
+        <v>5715.8281917026516</v>
       </c>
       <c r="G18">
-        <v>5704.8806240000004</v>
+        <v>6940.6485184960766</v>
       </c>
       <c r="H18">
-        <v>8563.611954</v>
+        <v>10410.972777744115</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
@@ -1970,19 +1972,19 @@
         <v>203</v>
       </c>
       <c r="D19">
-        <v>1472.045478</v>
+        <v>8544.4744909844903</v>
       </c>
       <c r="E19">
-        <v>1919.4773110000001</v>
+        <v>11107.816838279839</v>
       </c>
       <c r="F19">
-        <v>2534.1364159999998</v>
+        <v>14952.83035922286</v>
       </c>
       <c r="G19">
-        <v>4103.1415619999998</v>
+        <v>18157.008293342042</v>
       </c>
       <c r="H19">
-        <v>6159.2370529999998</v>
+        <v>27235.512440013063</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
@@ -1996,19 +1998,19 @@
         <v>204</v>
       </c>
       <c r="D20">
-        <v>2311.7824679999999</v>
+        <v>8028.0552054286509</v>
       </c>
       <c r="E20">
-        <v>3014.4544190000001</v>
+        <v>10436.471767057246</v>
       </c>
       <c r="F20">
-        <v>3979.7494219999999</v>
+        <v>14049.09660950014</v>
       </c>
       <c r="G20">
-        <v>6443.8027700000002</v>
+        <v>17059.617311535883</v>
       </c>
       <c r="H20">
-        <v>9672.8100140000006</v>
+        <v>25589.425967303825</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
@@ -2022,19 +2024,19 @@
         <v>205</v>
       </c>
       <c r="D21">
-        <v>2341.9968119999999</v>
+        <v>9399.2584890345279</v>
       </c>
       <c r="E21">
-        <v>3053.8524860000002</v>
+        <v>12219.036035744886</v>
       </c>
       <c r="F21">
-        <v>4031.7636229999998</v>
+        <v>15906.437442981509</v>
       </c>
       <c r="G21">
-        <v>6528.021452</v>
+        <v>19521.536861840941</v>
       </c>
       <c r="H21">
-        <v>9799.2309089999999</v>
+        <v>29282.305292761419</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
@@ -2048,19 +2050,19 @@
         <v>206</v>
       </c>
       <c r="D22">
-        <v>6655.0979710000001</v>
+        <v>9410.4349267904072</v>
       </c>
       <c r="E22">
-        <v>8677.931321</v>
+        <v>12233.565404827528</v>
       </c>
       <c r="F22">
-        <v>11456.79694</v>
+        <v>15925.35141456838</v>
       </c>
       <c r="G22">
-        <v>18550.24828</v>
+        <v>19544.749463333923</v>
       </c>
       <c r="H22">
-        <v>27845.828570000001</v>
+        <v>29317.124195000884</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
@@ -2074,19 +2076,19 @@
         <v>207</v>
       </c>
       <c r="D23">
-        <v>4737.2754180000002</v>
+        <v>10005.820279167037</v>
       </c>
       <c r="E23">
-        <v>6177.1818999999996</v>
+        <v>13007.56636291715</v>
       </c>
       <c r="F23">
-        <v>8155.2522230000004</v>
+        <v>16932.926626282679</v>
       </c>
       <c r="G23">
-        <v>13204.5592</v>
+        <v>20781.319041346924</v>
       </c>
       <c r="H23">
-        <v>19821.40004</v>
+        <v>31171.978562020391</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
@@ -2100,19 +2102,19 @@
         <v>208</v>
       </c>
       <c r="D24">
-        <v>27933.960060000001</v>
+        <v>28304.021473464327</v>
       </c>
       <c r="E24">
-        <v>36424.55573</v>
+        <v>36795.22791550363</v>
       </c>
       <c r="F24">
-        <v>48088.504419999997</v>
+        <v>47173.369122440548</v>
       </c>
       <c r="G24">
-        <v>77862.399139999994</v>
+        <v>59752.93422175802</v>
       </c>
       <c r="H24">
-        <v>116879.46090000001</v>
+        <v>89629.401332637019</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
@@ -2126,19 +2128,19 @@
         <v>209</v>
       </c>
       <c r="D25">
-        <v>2941.2037230000001</v>
+        <v>15885.144431881274</v>
       </c>
       <c r="E25">
-        <v>3835.1898080000001</v>
+        <v>20650.687761445657</v>
       </c>
       <c r="F25">
-        <v>5063.3024429999996</v>
+        <v>26882.552115491388</v>
       </c>
       <c r="G25">
-        <v>8198.2353270000003</v>
+        <v>32992.22305083034</v>
       </c>
       <c r="H25">
-        <v>12306.393539999999</v>
+        <v>49488.334576245514</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
@@ -2152,19 +2154,19 @@
         <v>210</v>
       </c>
       <c r="D26">
-        <v>1859.510996</v>
+        <v>3288.489991696033</v>
       </c>
       <c r="E26">
-        <v>2424.7139240000001</v>
+        <v>4275.0369892048438</v>
       </c>
       <c r="F26">
-        <v>3201.1609720000001</v>
+        <v>5688.1989045553009</v>
       </c>
       <c r="G26">
-        <v>5183.1529449999998</v>
+        <v>6932.4924149267727</v>
       </c>
       <c r="H26">
-        <v>7780.445103</v>
+        <v>10398.738622390158</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
@@ -2178,19 +2180,19 @@
         <v>211</v>
       </c>
       <c r="D27">
-        <v>1526.757423</v>
+        <v>818.28387269388998</v>
       </c>
       <c r="E27">
-        <v>1990.819086</v>
+        <v>1063.7690345020569</v>
       </c>
       <c r="F27">
-        <v>2628.323406</v>
+        <v>1415.4099419569989</v>
       </c>
       <c r="G27">
-        <v>4255.644225</v>
+        <v>1725.0308667600923</v>
       </c>
       <c r="H27">
-        <v>6388.1592199999996</v>
+        <v>2587.5463001401381</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
@@ -2204,19 +2206,19 @@
         <v>212</v>
       </c>
       <c r="D28">
-        <v>938.31894690000001</v>
+        <v>3900.5640515514965</v>
       </c>
       <c r="E28">
-        <v>1223.5232920000001</v>
+        <v>5070.7332670169453</v>
       </c>
       <c r="F28">
-        <v>1615.3225219999999</v>
+        <v>6825.9870902151197</v>
       </c>
       <c r="G28">
-        <v>2615.4460089999998</v>
+        <v>8288.6986095469292</v>
       </c>
       <c r="H28">
-        <v>3926.0531780000001</v>
+        <v>12433.047914320394</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
@@ -2230,19 +2232,19 @@
         <v>213</v>
       </c>
       <c r="D29">
-        <v>2854.3906539999998</v>
+        <v>3970.2168895342193</v>
       </c>
       <c r="E29">
-        <v>3721.9896939999999</v>
+        <v>5161.2819563944859</v>
       </c>
       <c r="F29">
-        <v>4913.8531480000001</v>
+        <v>6947.8795566848839</v>
       </c>
       <c r="G29">
-        <v>7956.2548210000004</v>
+        <v>8436.7108902602158</v>
       </c>
       <c r="H29">
-        <v>11943.155940000001</v>
+        <v>12655.066335390324</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
@@ -2256,19 +2258,19 @@
         <v>214</v>
       </c>
       <c r="D30">
-        <v>29985.01153</v>
+        <v>47122.759476463973</v>
       </c>
       <c r="E30">
-        <v>39099.029329999998</v>
+        <v>61259.587319403166</v>
       </c>
       <c r="F30">
-        <v>51619.403639999997</v>
+        <v>78537.932460773285</v>
       </c>
       <c r="G30">
-        <v>83579.447060000006</v>
+        <v>99481.381116979479</v>
       </c>
       <c r="H30">
-        <v>125461.33719999999</v>
+        <v>149222.07167546923</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
@@ -2282,19 +2284,19 @@
         <v>215</v>
       </c>
       <c r="D31">
-        <v>3887.6780939999999</v>
+        <v>8155.5969027526735</v>
       </c>
       <c r="E31">
-        <v>5069.347385</v>
+        <v>10602.275973578477</v>
       </c>
       <c r="F31">
-        <v>6692.6645850000004</v>
+        <v>14272.29457981718</v>
       </c>
       <c r="G31">
-        <v>10836.413560000001</v>
+        <v>17330.643418349431</v>
       </c>
       <c r="H31">
-        <v>16266.570110000001</v>
+        <v>25995.965127524145</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
@@ -2308,19 +2310,19 @@
         <v>216</v>
       </c>
       <c r="D32">
-        <v>1654.2851069999999</v>
+        <v>1706.2087905373749</v>
       </c>
       <c r="E32">
-        <v>2157.1091219999998</v>
+        <v>2218.0714276985877</v>
       </c>
       <c r="F32">
-        <v>2847.8631919999998</v>
+        <v>2951.2800701187025</v>
       </c>
       <c r="G32">
-        <v>4611.1116000000002</v>
+        <v>3596.8725854571685</v>
       </c>
       <c r="H32">
-        <v>6921.7522710000003</v>
+        <v>5395.3088781857523</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
@@ -2334,19 +2336,19 @@
         <v>217</v>
       </c>
       <c r="D33">
-        <v>2268.0479559999999</v>
+        <v>2537.0541656389232</v>
       </c>
       <c r="E33">
-        <v>2957.4266950000001</v>
+        <v>3298.1704153306005</v>
       </c>
       <c r="F33">
-        <v>3904.4601600000001</v>
+        <v>4388.4180162402999</v>
       </c>
       <c r="G33">
-        <v>6321.898322</v>
+        <v>5348.3844572928656</v>
       </c>
       <c r="H33">
-        <v>9489.8189110000003</v>
+        <v>8022.5766859392979</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
@@ -2360,19 +2362,19 @@
         <v>218</v>
       </c>
       <c r="D34">
-        <v>5793.0180309999996</v>
+        <v>14616.546998375616</v>
       </c>
       <c r="E34">
-        <v>7553.8200690000003</v>
+        <v>19001.511097888302</v>
       </c>
       <c r="F34">
-        <v>9972.7203929999996</v>
+        <v>24360.911663959356</v>
       </c>
       <c r="G34">
-        <v>16147.30891</v>
+        <v>30857.154774348517</v>
       </c>
       <c r="H34">
-        <v>24238.769690000001</v>
+        <v>46285.73216152277</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
@@ -2386,19 +2388,19 @@
         <v>219</v>
       </c>
       <c r="D35">
-        <v>1635.254312</v>
+        <v>16402.756635353478</v>
       </c>
       <c r="E35">
-        <v>2132.29387</v>
+        <v>21323.583625959523</v>
       </c>
       <c r="F35">
-        <v>2815.1015480000001</v>
+        <v>27758.511229059732</v>
       </c>
       <c r="G35">
-        <v>4558.0656529999997</v>
+        <v>34067.26378111876</v>
       </c>
       <c r="H35">
-        <v>6842.124855</v>
+        <v>51100.895671678147</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
@@ -2412,19 +2414,19 @@
         <v>220</v>
       </c>
       <c r="D36">
-        <v>3489.6259580000001</v>
+        <v>8037.5192282835296</v>
       </c>
       <c r="E36">
-        <v>4550.3063259999999</v>
+        <v>10448.774996768589</v>
       </c>
       <c r="F36">
-        <v>6007.415094</v>
+        <v>13601.955617095206</v>
       </c>
       <c r="G36">
-        <v>9726.8933070000003</v>
+        <v>16693.309166435025</v>
       </c>
       <c r="H36">
-        <v>14601.066220000001</v>
+        <v>25039.963749652539</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
@@ -2438,19 +2440,19 @@
         <v>221</v>
       </c>
       <c r="D37">
-        <v>1953.5227609999999</v>
+        <v>3785.9300175870285</v>
       </c>
       <c r="E37">
-        <v>2547.3007950000001</v>
+        <v>4921.7090228631378</v>
       </c>
       <c r="F37">
-        <v>3363.002872</v>
+        <v>6625.3775307773003</v>
       </c>
       <c r="G37">
-        <v>5445.1989110000004</v>
+        <v>8045.1012873724358</v>
       </c>
       <c r="H37">
-        <v>8173.8030220000001</v>
+        <v>12067.651931058654</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
@@ -2464,19 +2466,19 @@
         <v>222</v>
       </c>
       <c r="D38">
-        <v>3664.4705949999998</v>
+        <v>6097.1357076796148</v>
       </c>
       <c r="E38">
-        <v>4778.295419</v>
+        <v>7926.2764199835001</v>
       </c>
       <c r="F38">
-        <v>6308.4113390000002</v>
+        <v>10669.987488439327</v>
       </c>
       <c r="G38">
-        <v>10214.25073</v>
+        <v>12956.413378819181</v>
       </c>
       <c r="H38">
-        <v>15332.639800000001</v>
+        <v>19434.620068228771</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
@@ -2490,19 +2492,19 @@
         <v>223</v>
       </c>
       <c r="D39">
-        <v>4527.536513</v>
+        <v>16385.263488714983</v>
       </c>
       <c r="E39">
-        <v>5903.6923390000002</v>
+        <v>21300.842535329481</v>
       </c>
       <c r="F39">
-        <v>7794.1852529999996</v>
+        <v>27728.907442440744</v>
       </c>
       <c r="G39">
-        <v>12619.938389999999</v>
+        <v>34030.931861177276</v>
       </c>
       <c r="H39">
-        <v>18943.824140000001</v>
+        <v>51046.397791765921</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
@@ -2516,19 +2518,19 @@
         <v>224</v>
       </c>
       <c r="D40">
-        <v>2801.7736580000001</v>
+        <v>6272.1093433641709</v>
       </c>
       <c r="E40">
-        <v>3653.379633</v>
+        <v>8153.7421463734227</v>
       </c>
       <c r="F40">
-        <v>4823.2726270000003</v>
+        <v>10976.1913508873</v>
       </c>
       <c r="G40">
-        <v>7809.5915640000003</v>
+        <v>13328.232354648862</v>
       </c>
       <c r="H40">
-        <v>11722.999320000001</v>
+        <v>19992.348531973294</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
@@ -2542,19 +2544,19 @@
         <v>225</v>
       </c>
       <c r="D41">
-        <v>16099.20571</v>
+        <v>16028.129151101373</v>
       </c>
       <c r="E41">
-        <v>20992.598760000001</v>
+        <v>20836.567896431785</v>
       </c>
       <c r="F41">
-        <v>27714.893380000001</v>
+        <v>26713.548585168952</v>
       </c>
       <c r="G41">
-        <v>44874.510370000004</v>
+        <v>33837.161541214009</v>
       </c>
       <c r="H41">
-        <v>67361.250610000003</v>
+        <v>50755.742311821006</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
@@ -2568,19 +2570,19 @@
         <v>226</v>
       </c>
       <c r="D42">
-        <v>10863.882949999999</v>
+        <v>62967.292658771403</v>
       </c>
       <c r="E42">
-        <v>14165.98682</v>
+        <v>81857.480456402831</v>
       </c>
       <c r="F42">
-        <v>18702.249240000001</v>
+        <v>106560.03373022853</v>
       </c>
       <c r="G42">
-        <v>30281.706880000002</v>
+        <v>130778.22321437139</v>
       </c>
       <c r="H42">
-        <v>45455.953260000002</v>
+        <v>196167.3348215571</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
@@ -2594,19 +2596,19 @@
         <v>227</v>
       </c>
       <c r="D43">
-        <v>24660.844959999999</v>
+        <v>42569.596875000003</v>
       </c>
       <c r="E43">
-        <v>32156.56926</v>
+        <v>55340.475937500007</v>
       </c>
       <c r="F43">
-        <v>42453.814250000003</v>
+        <v>72040.856250000012</v>
       </c>
       <c r="G43">
-        <v>68739.002590000004</v>
+        <v>88413.778125000012</v>
       </c>
       <c r="H43">
-        <v>103184.30530000001</v>
+        <v>132620.66718750002</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
@@ -2620,19 +2622,19 @@
         <v>228</v>
       </c>
       <c r="D44">
-        <v>18648.902139999998</v>
+        <v>24140.262767590011</v>
       </c>
       <c r="E44">
-        <v>24317.28168</v>
+        <v>31382.341597867016</v>
       </c>
       <c r="F44">
-        <v>32104.213329999999</v>
+        <v>40233.771279316687</v>
       </c>
       <c r="G44">
-        <v>51981.468390000002</v>
+        <v>50962.776953801134</v>
       </c>
       <c r="H44">
-        <v>78029.524780000007</v>
+        <v>76444.165430701687</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
@@ -2646,19 +2648,19 @@
         <v>229</v>
       </c>
       <c r="D45">
-        <v>113.74685839999999</v>
+        <v>0</v>
       </c>
       <c r="E45">
-        <v>148.32049499999999</v>
+        <v>0</v>
       </c>
       <c r="F45">
-        <v>195.81599919999999</v>
+        <v>0</v>
       </c>
       <c r="G45">
-        <v>317.0550566</v>
+        <v>0</v>
       </c>
       <c r="H45">
-        <v>475.93221510000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
@@ -2672,19 +2674,19 @@
         <v>230</v>
       </c>
       <c r="D46">
-        <v>1049.5852379999999</v>
+        <v>2134.8064987583034</v>
       </c>
       <c r="E46">
-        <v>1368.6092450000001</v>
+        <v>2775.2484483857947</v>
       </c>
       <c r="F46">
-        <v>1806.868207</v>
+        <v>3692.6382681224709</v>
       </c>
       <c r="G46">
-        <v>2925.5867950000002</v>
+        <v>4500.4028892742608</v>
       </c>
       <c r="H46">
-        <v>4391.6063629999999</v>
+        <v>6750.6043339113912</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
@@ -2698,19 +2700,19 @@
         <v>231</v>
       </c>
       <c r="D47">
-        <v>34176.872000000003</v>
+        <v>62341.78661848203</v>
       </c>
       <c r="E47">
-        <v>44565.016060000002</v>
+        <v>81044.322604026645</v>
       </c>
       <c r="F47">
-        <v>58835.720269999998</v>
+        <v>103902.97769747005</v>
       </c>
       <c r="G47">
-        <v>95263.730710000003</v>
+        <v>131610.4384167954</v>
       </c>
       <c r="H47">
-        <v>143000.64749999999</v>
+        <v>197415.65762519307</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
@@ -2724,19 +2726,19 @@
         <v>232</v>
       </c>
       <c r="D48">
-        <v>1647.7024919999999</v>
+        <v>7350.1235569834289</v>
       </c>
       <c r="E48">
-        <v>2148.525705</v>
+        <v>9555.1606240784586</v>
       </c>
       <c r="F48">
-        <v>2836.5311750000001</v>
+        <v>12862.716224721002</v>
       </c>
       <c r="G48">
-        <v>4592.7633889999997</v>
+        <v>15619.012558589786</v>
       </c>
       <c r="H48">
-        <v>6894.2097210000002</v>
+        <v>23428.51883788468</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
@@ -2750,19 +2752,19 @@
         <v>233</v>
       </c>
       <c r="D49">
-        <v>4441.8900910000002</v>
+        <v>11019.774530602579</v>
       </c>
       <c r="E49">
-        <v>5792.0134770000004</v>
+        <v>14325.706889783354</v>
       </c>
       <c r="F49">
-        <v>7646.7443489999996</v>
+        <v>18648.849205635135</v>
       </c>
       <c r="G49">
-        <v>12381.209769999999</v>
+        <v>22887.224025097665</v>
       </c>
       <c r="H49">
-        <v>18585.467939999999</v>
+        <v>34330.836037646506</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.3">
@@ -2776,19 +2778,19 @@
         <v>234</v>
       </c>
       <c r="D50">
-        <v>3794.6566830000002</v>
+        <v>7754.6727317074074</v>
       </c>
       <c r="E50">
-        <v>4948.051888</v>
+        <v>10081.07455121963</v>
       </c>
       <c r="F50">
-        <v>6532.5275849999998</v>
+        <v>13123.292315197152</v>
       </c>
       <c r="G50">
-        <v>10577.12808</v>
+        <v>16105.858750469231</v>
       </c>
       <c r="H50">
-        <v>15877.355970000001</v>
+        <v>24158.78812570385</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.3">
@@ -2802,19 +2804,19 @@
         <v>235</v>
       </c>
       <c r="D51">
-        <v>2918.404137</v>
+        <v>9328.1339961362501</v>
       </c>
       <c r="E51">
-        <v>3805.4602319999999</v>
+        <v>12126.574194977125</v>
       </c>
       <c r="F51">
-        <v>5024.0527990000001</v>
+        <v>16324.234493238439</v>
       </c>
       <c r="G51">
-        <v>8134.6843500000004</v>
+        <v>19822.284741789528</v>
       </c>
       <c r="H51">
-        <v>12210.99699</v>
+        <v>29733.427112684294</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
@@ -2828,19 +2830,19 @@
         <v>236</v>
       </c>
       <c r="D52">
-        <v>3584.004336</v>
+        <v>6063.6045894890021</v>
       </c>
       <c r="E52">
-        <v>4673.3712439999999</v>
+        <v>7882.6859663357027</v>
       </c>
       <c r="F52">
-        <v>6169.888121</v>
+        <v>10261.484689904466</v>
       </c>
       <c r="G52">
-        <v>9989.9611619999996</v>
+        <v>12593.640301246389</v>
       </c>
       <c r="H52">
-        <v>14995.9581</v>
+        <v>18890.460451869585</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.3">
@@ -2854,19 +2856,19 @@
         <v>237</v>
       </c>
       <c r="D53">
-        <v>9847.7438199999997</v>
+        <v>9627.9104672315189</v>
       </c>
       <c r="E53">
-        <v>12840.98971</v>
+        <v>12516.283607400976</v>
       </c>
       <c r="F53">
-        <v>16952.958729999998</v>
+        <v>16293.386944545649</v>
       </c>
       <c r="G53">
-        <v>27449.3469</v>
+        <v>19996.429431942386</v>
       </c>
       <c r="H53">
-        <v>41204.289920000003</v>
+        <v>29994.644147913583</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
@@ -2880,19 +2882,19 @@
         <v>238</v>
       </c>
       <c r="D54">
-        <v>1324.146622</v>
+        <v>2382.8000000000002</v>
       </c>
       <c r="E54">
-        <v>1726.624235</v>
+        <v>3097.6400000000003</v>
       </c>
       <c r="F54">
-        <v>2279.5275179999999</v>
+        <v>4121.6000000000004</v>
       </c>
       <c r="G54">
-        <v>3690.8921089999999</v>
+        <v>5023.2</v>
       </c>
       <c r="H54">
-        <v>5540.4082689999996</v>
+        <v>7534.7999999999993</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
@@ -2906,19 +2908,19 @@
         <v>239</v>
       </c>
       <c r="D55">
-        <v>8254.7281700000003</v>
+        <v>25149.331097893824</v>
       </c>
       <c r="E55">
-        <v>10763.77304</v>
+        <v>32694.130427261975</v>
       </c>
       <c r="F55">
-        <v>14210.571330000001</v>
+        <v>41915.551829823038</v>
       </c>
       <c r="G55">
-        <v>23009.016199999998</v>
+        <v>53093.032317775847</v>
       </c>
       <c r="H55">
-        <v>34538.89733</v>
+        <v>79639.548476663767</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
@@ -2932,19 +2934,19 @@
         <v>240</v>
       </c>
       <c r="D56">
-        <v>1029.87987</v>
+        <v>3422.5025810888442</v>
       </c>
       <c r="E56">
-        <v>1342.9143819999999</v>
+        <v>4449.2533554154979</v>
       </c>
       <c r="F56">
-        <v>1772.9452799999999</v>
+        <v>5920.004464586109</v>
       </c>
       <c r="G56">
-        <v>2870.6605610000001</v>
+        <v>7215.0054412143199</v>
       </c>
       <c r="H56">
-        <v>4309.1564420000004</v>
+        <v>10822.508161821479</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.3">
@@ -2958,19 +2960,19 @@
         <v>241</v>
       </c>
       <c r="D57">
-        <v>2787.189417</v>
+        <v>6052.8667438849989</v>
       </c>
       <c r="E57">
-        <v>3634.3624759999998</v>
+        <v>7868.7267670504998</v>
       </c>
       <c r="F57">
-        <v>4798.1657569999998</v>
+        <v>10243.312951189999</v>
       </c>
       <c r="G57">
-        <v>7768.9398279999996</v>
+        <v>12571.338621914998</v>
       </c>
       <c r="H57">
-        <v>11661.97689</v>
+        <v>18857.007932872501</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.3">
@@ -2984,19 +2986,19 @@
         <v>242</v>
       </c>
       <c r="D58">
-        <v>31030.032459999999</v>
+        <v>69627.970979560181</v>
       </c>
       <c r="E58">
-        <v>40461.68692</v>
+        <v>90516.36227342824</v>
       </c>
       <c r="F58">
-        <v>53418.414340000003</v>
+        <v>117831.95088848646</v>
       </c>
       <c r="G58">
-        <v>86492.311400000006</v>
+        <v>144611.93972677883</v>
       </c>
       <c r="H58">
-        <v>129833.8459</v>
+        <v>216917.90959016827</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.3">
@@ -3010,19 +3012,19 @@
         <v>243</v>
       </c>
       <c r="D59">
-        <v>33335.619509999997</v>
+        <v>39304.177568966777</v>
       </c>
       <c r="E59">
-        <v>43468.062819999999</v>
+        <v>51095.430839656816</v>
       </c>
       <c r="F59">
-        <v>57387.498319999999</v>
+        <v>65506.962614944627</v>
       </c>
       <c r="G59">
-        <v>92918.845239999995</v>
+        <v>82975.485978929864</v>
       </c>
       <c r="H59">
-        <v>139480.7335</v>
+        <v>124463.22896839479</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.3">
@@ -3036,19 +3038,19 @@
         <v>244</v>
       </c>
       <c r="D60">
-        <v>6909.8905340000001</v>
+        <v>11226.536287566472</v>
       </c>
       <c r="E60">
-        <v>9010.1687079999992</v>
+        <v>14594.497173836415</v>
       </c>
       <c r="F60">
-        <v>11895.42409</v>
+        <v>18998.753717420186</v>
       </c>
       <c r="G60">
-        <v>19260.450489999999</v>
+        <v>23316.652289561134</v>
       </c>
       <c r="H60">
-        <v>28911.915059999999</v>
+        <v>34974.978434341705</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.3">
@@ -3062,19 +3064,19 @@
         <v>245</v>
       </c>
       <c r="D61">
-        <v>2148.5698600000001</v>
+        <v>2856.9603668621517</v>
       </c>
       <c r="E61">
-        <v>2801.6329380000002</v>
+        <v>3714.0484769207974</v>
       </c>
       <c r="F61">
-        <v>3698.777795</v>
+        <v>4941.7692832210196</v>
       </c>
       <c r="G61">
-        <v>5988.86816</v>
+        <v>6022.7813139256168</v>
       </c>
       <c r="H61">
-        <v>8989.906422</v>
+        <v>9034.1719708884248</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.3">
@@ -3088,19 +3090,19 @@
         <v>246</v>
       </c>
       <c r="D62">
-        <v>1385.1740259999999</v>
+        <v>6530.2566987967994</v>
       </c>
       <c r="E62">
-        <v>1806.201069</v>
+        <v>8489.3337084358391</v>
       </c>
       <c r="F62">
-        <v>2384.586616</v>
+        <v>11051.203644117661</v>
       </c>
       <c r="G62">
-        <v>3860.9983219999999</v>
+        <v>13562.840835962583</v>
       </c>
       <c r="H62">
-        <v>5795.7551709999998</v>
+        <v>20344.261253943878</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.3">
@@ -3114,19 +3116,19 @@
         <v>247</v>
       </c>
       <c r="D63">
-        <v>29803.067869999999</v>
+        <v>46284.075328897932</v>
       </c>
       <c r="E63">
-        <v>38861.783439999999</v>
+        <v>60169.297927567321</v>
       </c>
       <c r="F63">
-        <v>51306.186370000003</v>
+        <v>77140.125548163225</v>
       </c>
       <c r="G63">
-        <v>83072.301980000004</v>
+        <v>97710.825694340077</v>
       </c>
       <c r="H63">
-        <v>124700.0604</v>
+        <v>146566.2385415101</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.3">
@@ -3140,19 +3142,19 @@
         <v>248</v>
       </c>
       <c r="D64">
-        <v>2710.9540280000001</v>
+        <v>5813.006190840505</v>
       </c>
       <c r="E64">
-        <v>3534.9551529999999</v>
+        <v>7556.9080480926577</v>
       </c>
       <c r="F64">
-        <v>4666.9260089999998</v>
+        <v>10172.760833970886</v>
       </c>
       <c r="G64">
-        <v>7556.4432710000001</v>
+        <v>12352.638155536073</v>
       </c>
       <c r="H64">
-        <v>11342.997719999999</v>
+        <v>18528.957233304111</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.3">
@@ -3166,19 +3168,19 @@
         <v>249</v>
       </c>
       <c r="D65">
-        <v>29077.54003</v>
+        <v>18279.614231898551</v>
       </c>
       <c r="E65">
-        <v>37915.729639999998</v>
+        <v>23763.498501468115</v>
       </c>
       <c r="F65">
-        <v>50057.1852</v>
+        <v>30466.023719830915</v>
       </c>
       <c r="G65">
-        <v>81049.984419999993</v>
+        <v>38590.296711785821</v>
       </c>
       <c r="H65">
-        <v>121664.3539</v>
+        <v>57885.445067678731</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.3">
@@ -3192,19 +3194,19 @@
         <v>250</v>
       </c>
       <c r="D66">
-        <v>4883.9789280000005</v>
+        <v>11713.666639916539</v>
       </c>
       <c r="E66">
-        <v>6368.4763009999997</v>
+        <v>15227.766631891502</v>
       </c>
       <c r="F66">
-        <v>8407.8033240000004</v>
+        <v>19823.128159858759</v>
       </c>
       <c r="G66">
-        <v>13613.476780000001</v>
+        <v>24328.38455982666</v>
       </c>
       <c r="H66">
-        <v>20435.227340000001</v>
+        <v>36492.576839739995</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.3">
@@ -3218,19 +3220,19 @@
         <v>251</v>
       </c>
       <c r="D67">
-        <v>3906.249722</v>
+        <v>6538.3208212932104</v>
       </c>
       <c r="E67">
-        <v>5093.563905</v>
+        <v>8499.8170676811733</v>
       </c>
       <c r="F67">
-        <v>6724.6357690000004</v>
+        <v>11064.850620650048</v>
       </c>
       <c r="G67">
-        <v>10888.179630000001</v>
+        <v>13579.589398070513</v>
       </c>
       <c r="H67">
-        <v>16344.276309999999</v>
+        <v>20369.384097105773</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.3">
@@ -3244,19 +3246,19 @@
         <v>252</v>
       </c>
       <c r="D68">
-        <v>1909.5328030000001</v>
+        <v>2854.0223987009826</v>
       </c>
       <c r="E68">
-        <v>2489.939981</v>
+        <v>3710.2291183112775</v>
       </c>
       <c r="F68">
-        <v>3287.2738559999998</v>
+        <v>4994.53919772672</v>
       </c>
       <c r="G68">
-        <v>5322.582437</v>
+        <v>6064.797597239588</v>
       </c>
       <c r="H68">
-        <v>7989.7430960000002</v>
+        <v>9097.1963958593824</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.3">
@@ -3270,19 +3272,19 @@
         <v>253</v>
       </c>
       <c r="D69">
-        <v>1350.587417</v>
+        <v>2941.9388386449873</v>
       </c>
       <c r="E69">
-        <v>1761.1017750000001</v>
+        <v>3824.5204902384835</v>
       </c>
       <c r="F69">
-        <v>2325.0455299999999</v>
+        <v>5088.7590722507884</v>
       </c>
       <c r="G69">
-        <v>3764.5924989999999</v>
+        <v>6201.925119305648</v>
       </c>
       <c r="H69">
-        <v>5651.0401270000002</v>
+        <v>9302.887678958472</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.3">
@@ -3296,19 +3298,19 @@
         <v>254</v>
       </c>
       <c r="D70">
-        <v>2892.34123</v>
+        <v>8995.1811338031202</v>
       </c>
       <c r="E70">
-        <v>3771.4754400000002</v>
+        <v>11693.735473944058</v>
       </c>
       <c r="F70">
-        <v>4979.1853259999998</v>
+        <v>14991.968556338536</v>
       </c>
       <c r="G70">
-        <v>8062.0372770000004</v>
+        <v>18989.82683802881</v>
       </c>
       <c r="H70">
-        <v>12101.94627</v>
+        <v>28484.740257043213</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.3">
@@ -3322,19 +3324,19 @@
         <v>255</v>
       </c>
       <c r="D71">
-        <v>1531.636375</v>
+        <v>4376.9813386868318</v>
       </c>
       <c r="E71">
-        <v>1997.1810069999999</v>
+        <v>5690.0757402928821</v>
       </c>
       <c r="F71">
-        <v>2636.7225560000002</v>
+        <v>7659.717342701957</v>
       </c>
       <c r="G71">
-        <v>4269.2436909999997</v>
+        <v>9301.0853447095178</v>
       </c>
       <c r="H71">
-        <v>6408.5734149999998</v>
+        <v>13951.628017064277</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.3">
@@ -3348,19 +3350,19 @@
         <v>256</v>
       </c>
       <c r="D72">
-        <v>2591.560645</v>
+        <v>6652.1343693017252</v>
       </c>
       <c r="E72">
-        <v>3379.2718580000001</v>
+        <v>8647.7746800922432</v>
       </c>
       <c r="F72">
-        <v>4461.3894790000004</v>
+        <v>11641.235146278021</v>
       </c>
       <c r="G72">
-        <v>7223.649238</v>
+        <v>14135.785534766166</v>
       </c>
       <c r="H72">
-        <v>10843.439689999999</v>
+        <v>21203.678302149248</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.3">
@@ -3374,19 +3376,19 @@
         <v>257</v>
       </c>
       <c r="D73">
-        <v>8657.0286290000004</v>
+        <v>16877.742250818505</v>
       </c>
       <c r="E73">
-        <v>11288.353709999999</v>
+        <v>21941.064926064057</v>
       </c>
       <c r="F73">
-        <v>14903.134340000001</v>
+        <v>28129.570418030838</v>
       </c>
       <c r="G73">
-        <v>24130.378110000001</v>
+        <v>35630.789196172394</v>
       </c>
       <c r="H73">
-        <v>36222.176769999998</v>
+        <v>53446.183794258592</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.3">
@@ -3400,19 +3402,19 @@
         <v>258</v>
       </c>
       <c r="D74">
-        <v>36036.018799999998</v>
+        <v>61839.219780492567</v>
       </c>
       <c r="E74">
-        <v>46989.255089999999</v>
+        <v>80390.985714640352</v>
       </c>
       <c r="F74">
-        <v>62036.254269999998</v>
+        <v>103065.36630082096</v>
       </c>
       <c r="G74">
-        <v>100445.8685</v>
+        <v>130549.46398103987</v>
       </c>
       <c r="H74">
-        <v>150779.5687</v>
+        <v>195824.19597155976</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.3">
@@ -3426,19 +3428,19 @@
         <v>259</v>
       </c>
       <c r="D75">
-        <v>1586.180746</v>
+        <v>5371.5051412503663</v>
       </c>
       <c r="E75">
-        <v>2068.3042740000001</v>
+        <v>6982.9566836254762</v>
       </c>
       <c r="F75">
-        <v>2730.621067</v>
+        <v>9400.1339971881425</v>
       </c>
       <c r="G75">
-        <v>4421.2792639999998</v>
+        <v>11414.448425157028</v>
       </c>
       <c r="H75">
-        <v>6636.7944310000003</v>
+        <v>17121.672637735541</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.3">
@@ -3452,19 +3454,19 @@
         <v>260</v>
       </c>
       <c r="D76">
-        <v>1429.5266899999999</v>
+        <v>5634.4807774587807</v>
       </c>
       <c r="E76">
-        <v>1864.0348329999999</v>
+        <v>7324.8250106964151</v>
       </c>
       <c r="F76">
-        <v>2460.9400300000002</v>
+        <v>9535.2751618533221</v>
       </c>
       <c r="G76">
-        <v>3984.6257900000001</v>
+        <v>11702.383153183622</v>
       </c>
       <c r="H76">
-        <v>5981.332703</v>
+        <v>17553.574729775435</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.3">
@@ -3478,19 +3480,19 @@
         <v>261</v>
       </c>
       <c r="D77">
-        <v>4146.2617469999996</v>
+        <v>9802.0807315069906</v>
       </c>
       <c r="E77">
-        <v>5406.5281729999997</v>
+        <v>12742.704950959089</v>
       </c>
       <c r="F77">
-        <v>7137.8181210000002</v>
+        <v>17153.641280137235</v>
       </c>
       <c r="G77">
-        <v>11557.18295</v>
+        <v>20829.421554452354</v>
       </c>
       <c r="H77">
-        <v>17348.519029999999</v>
+        <v>31244.132331678531</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.3">
@@ -3504,19 +3506,19 @@
         <v>262</v>
       </c>
       <c r="D78">
-        <v>2300.6822099999999</v>
+        <v>6202.0859455716009</v>
       </c>
       <c r="E78">
-        <v>2999.9802100000002</v>
+        <v>8062.7117292430812</v>
       </c>
       <c r="F78">
-        <v>3960.6402520000001</v>
+        <v>10495.837754044247</v>
       </c>
       <c r="G78">
-        <v>6412.8621970000004</v>
+        <v>12881.255425417939</v>
       </c>
       <c r="H78">
-        <v>9626.3650350000007</v>
+        <v>19321.883138126912</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.3">
@@ -3530,19 +3532,19 @@
         <v>263</v>
       </c>
       <c r="D79">
-        <v>34158.062749999997</v>
+        <v>91801.618424230561</v>
       </c>
       <c r="E79">
-        <v>44540.489690000002</v>
+        <v>119342.10395149974</v>
       </c>
       <c r="F79">
-        <v>58803.34001</v>
+        <v>153002.69737371762</v>
       </c>
       <c r="G79">
-        <v>95211.302280000004</v>
+        <v>193803.41667337561</v>
       </c>
       <c r="H79">
-        <v>142921.94699999999</v>
+        <v>290705.12501006341</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.3">
@@ -3556,19 +3558,19 @@
         <v>264</v>
       </c>
       <c r="D80">
-        <v>24895.508900000001</v>
+        <v>46916.564365089762</v>
       </c>
       <c r="E80">
-        <v>32462.559880000001</v>
+        <v>60991.533674616701</v>
       </c>
       <c r="F80">
-        <v>42857.789839999998</v>
+        <v>78194.273941816267</v>
       </c>
       <c r="G80">
-        <v>69393.098800000007</v>
+        <v>99046.080326300609</v>
       </c>
       <c r="H80">
-        <v>104166.171</v>
+        <v>148569.1204894509</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.3">
@@ -3582,19 +3584,19 @@
         <v>265</v>
       </c>
       <c r="D81">
-        <v>28549.186610000001</v>
+        <v>32804.332503825302</v>
       </c>
       <c r="E81">
-        <v>37226.781889999998</v>
+        <v>42645.632254972901</v>
       </c>
       <c r="F81">
-        <v>49147.621149999999</v>
+        <v>54673.887506375504</v>
       </c>
       <c r="G81">
-        <v>79577.265719999996</v>
+        <v>69253.590841408964</v>
       </c>
       <c r="H81">
-        <v>119453.6519</v>
+        <v>103880.38626211345</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.3">
@@ -3608,19 +3610,19 @@
         <v>266</v>
       </c>
       <c r="D82">
-        <v>4886.4539580000001</v>
+        <v>6738.6553235561341</v>
       </c>
       <c r="E82">
-        <v>6371.703622</v>
+        <v>8760.2519206229754</v>
       </c>
       <c r="F82">
-        <v>8412.0641039999991</v>
+        <v>11403.878239864229</v>
       </c>
       <c r="G82">
-        <v>13620.375609999999</v>
+        <v>13995.668748924279</v>
       </c>
       <c r="H82">
-        <v>20445.583190000001</v>
+        <v>20993.503123386421</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.3">
@@ -3634,19 +3636,19 @@
         <v>267</v>
       </c>
       <c r="D83">
-        <v>33170.215499999998</v>
+        <v>35844.414091036102</v>
       </c>
       <c r="E83">
-        <v>43252.383849999998</v>
+        <v>46597.738318346943</v>
       </c>
       <c r="F83">
-        <v>57102.754180000004</v>
+        <v>59740.690151726842</v>
       </c>
       <c r="G83">
-        <v>92457.802360000001</v>
+        <v>75671.540858853987</v>
       </c>
       <c r="H83">
-        <v>138788.66070000001</v>
+        <v>113507.31128828098</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.3">
@@ -3660,19 +3662,19 @@
         <v>268</v>
       </c>
       <c r="D84">
-        <v>3971.082977</v>
+        <v>9966.6190902333219</v>
       </c>
       <c r="E84">
-        <v>5178.1033859999998</v>
+        <v>12956.60481730332</v>
       </c>
       <c r="F84">
-        <v>6836.2466629999999</v>
+        <v>17441.583407908314</v>
       </c>
       <c r="G84">
-        <v>11068.89417</v>
+        <v>21179.065566745809</v>
       </c>
       <c r="H84">
-        <v>16615.547399999999</v>
+        <v>31768.598350118711</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.3">
@@ -3686,19 +3688,19 @@
         <v>269</v>
       </c>
       <c r="D85">
-        <v>3180.9842870000002</v>
+        <v>13485.926730167719</v>
       </c>
       <c r="E85">
-        <v>4147.8522620000003</v>
+        <v>17531.704749218035</v>
       </c>
       <c r="F85">
-        <v>5476.0863330000002</v>
+        <v>22822.337543360754</v>
       </c>
       <c r="G85">
-        <v>8866.5934809999999</v>
+        <v>28009.232439579107</v>
       </c>
       <c r="H85">
-        <v>13309.66779</v>
+        <v>42013.848659368668</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.3">
@@ -3712,19 +3714,19 @@
         <v>270</v>
       </c>
       <c r="D86">
-        <v>2844.553911</v>
+        <v>4967.1867091660315</v>
       </c>
       <c r="E86">
-        <v>3709.1630479999999</v>
+        <v>6457.3427219158411</v>
       </c>
       <c r="F86">
-        <v>4896.9191270000001</v>
+        <v>8692.5767410405551</v>
       </c>
       <c r="G86">
-        <v>7928.8361370000002</v>
+        <v>10555.271756977816</v>
       </c>
       <c r="H86">
-        <v>11901.997670000001</v>
+        <v>15832.907635466725</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.3">
@@ -3738,19 +3740,19 @@
         <v>271</v>
       </c>
       <c r="D87">
-        <v>33139.442020000002</v>
+        <v>29092.356813958962</v>
       </c>
       <c r="E87">
-        <v>43212.256690000002</v>
+        <v>37820.063858146656</v>
       </c>
       <c r="F87">
-        <v>57049.777410000002</v>
+        <v>48487.261356598268</v>
       </c>
       <c r="G87">
-        <v>92372.025150000001</v>
+        <v>61417.197718357806</v>
       </c>
       <c r="H87">
-        <v>138659.90030000001</v>
+        <v>92125.796577536705</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.3">
@@ -3764,19 +3766,19 @@
         <v>272</v>
       </c>
       <c r="D88">
-        <v>482.79030130000001</v>
+        <v>3277.2199295828909</v>
       </c>
       <c r="E88">
-        <v>629.53559740000003</v>
+        <v>4260.3859084577589</v>
       </c>
       <c r="F88">
-        <v>831.12682500000005</v>
+        <v>5735.1348767700601</v>
       </c>
       <c r="G88">
-        <v>1345.717222</v>
+        <v>6964.0923503636432</v>
       </c>
       <c r="H88">
-        <v>2020.0598130000001</v>
+        <v>10446.138525545464</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.3">
@@ -3790,19 +3792,19 @@
         <v>273</v>
       </c>
       <c r="D89">
-        <v>1036.730249</v>
+        <v>6085.4962419256935</v>
       </c>
       <c r="E89">
-        <v>1351.8469500000001</v>
+        <v>7911.1451145034025</v>
       </c>
       <c r="F89">
-        <v>1784.7382560000001</v>
+        <v>10649.618423369964</v>
       </c>
       <c r="G89">
-        <v>2889.7551309999999</v>
+        <v>12931.679514092099</v>
       </c>
       <c r="H89">
-        <v>4337.8193540000002</v>
+        <v>19397.51927113815</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.3">
@@ -3816,19 +3818,19 @@
         <v>274</v>
       </c>
       <c r="D90">
-        <v>5671.2560830000002</v>
+        <v>18837.358413676979</v>
       </c>
       <c r="E90">
-        <v>7395.0482780000002</v>
+        <v>24488.565937780073</v>
       </c>
       <c r="F90">
-        <v>9763.1063630000008</v>
+        <v>31395.597356128295</v>
       </c>
       <c r="G90">
-        <v>15807.9128</v>
+        <v>39767.756651095842</v>
       </c>
       <c r="H90">
-        <v>23729.30126</v>
+        <v>59651.634976643756</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.3">
@@ -3842,19 +3844,19 @@
         <v>275</v>
       </c>
       <c r="D91">
-        <v>7974.6597199999997</v>
+        <v>9926.7517803843002</v>
       </c>
       <c r="E91">
-        <v>10398.5771</v>
+        <v>12904.777314499592</v>
       </c>
       <c r="F91">
-        <v>13728.431570000001</v>
+        <v>17371.815615672527</v>
       </c>
       <c r="G91">
-        <v>22228.360629999999</v>
+        <v>21094.347533316639</v>
       </c>
       <c r="H91">
-        <v>33367.053110000001</v>
+        <v>31641.521299974956</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.3">
@@ -3868,19 +3870,19 @@
         <v>276</v>
       </c>
       <c r="D92">
-        <v>3088.4990200000002</v>
+        <v>2470.8148539088629</v>
       </c>
       <c r="E92">
-        <v>4027.2558709999998</v>
+        <v>3212.0593100815222</v>
       </c>
       <c r="F92">
-        <v>5316.8723099999997</v>
+        <v>4323.9259943405104</v>
       </c>
       <c r="G92">
-        <v>8608.8024359999999</v>
+        <v>5250.481564556334</v>
       </c>
       <c r="H92">
-        <v>12922.69695</v>
+        <v>7875.722346834501</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.3">
@@ -3894,19 +3896,19 @@
         <v>277</v>
       </c>
       <c r="D93">
-        <v>1125.193217</v>
+        <v>2499.9537876418913</v>
       </c>
       <c r="E93">
-        <v>1467.198455</v>
+        <v>3249.9399239344584</v>
       </c>
       <c r="F93">
-        <v>1937.0278639999999</v>
+        <v>4324.2443894346225</v>
       </c>
       <c r="G93">
-        <v>3136.3345250000002</v>
+        <v>5270.1728496234455</v>
       </c>
       <c r="H93">
-        <v>4707.9603580000003</v>
+        <v>7905.2592744351687</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.3">
@@ -3920,19 +3922,19 @@
         <v>278</v>
       </c>
       <c r="D94">
-        <v>9690.2444699999996</v>
+        <v>7681.6367201146304</v>
       </c>
       <c r="E94">
-        <v>12635.618039999999</v>
+        <v>9986.1277361490193</v>
       </c>
       <c r="F94">
-        <v>16681.822520000002</v>
+        <v>12999.69291096322</v>
       </c>
       <c r="G94">
-        <v>27010.33727</v>
+        <v>15954.16857254577</v>
       </c>
       <c r="H94">
-        <v>40545.291369999999</v>
+        <v>23931.252858818658</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.3">
@@ -3946,19 +3948,19 @@
         <v>279</v>
       </c>
       <c r="D95">
-        <v>6145.9930080000004</v>
+        <v>21464.654129420942</v>
       </c>
       <c r="E95">
-        <v>8014.0826550000002</v>
+        <v>27904.050368247226</v>
       </c>
       <c r="F95">
-        <v>10580.36924</v>
+        <v>35774.423549034902</v>
       </c>
       <c r="G95">
-        <v>17131.182239999998</v>
+        <v>45314.269828777535</v>
       </c>
       <c r="H95">
-        <v>25715.664659999999</v>
+        <v>67971.404743166306</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.3">
@@ -3972,19 +3974,19 @@
         <v>280</v>
       </c>
       <c r="D96">
-        <v>41586.225539999999</v>
+        <v>120340.61499238691</v>
       </c>
       <c r="E96">
-        <v>54226.460789999997</v>
+        <v>156442.799490103</v>
       </c>
       <c r="F96">
-        <v>71590.973370000007</v>
+        <v>200567.69165397817</v>
       </c>
       <c r="G96">
-        <v>115916.37149999999</v>
+        <v>254052.40942837234</v>
       </c>
       <c r="H96">
-        <v>174002.38320000001</v>
+        <v>381078.61414255848</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.3">
@@ -3998,19 +4000,19 @@
         <v>281</v>
       </c>
       <c r="D97">
-        <v>1524.5627320000001</v>
+        <v>1862.4027004061741</v>
       </c>
       <c r="E97">
-        <v>1987.957314</v>
+        <v>2421.1235105280266</v>
       </c>
       <c r="F97">
-        <v>2624.5452319999999</v>
+        <v>3221.4533196214907</v>
       </c>
       <c r="G97">
-        <v>4249.5268020000003</v>
+        <v>3926.1462332886913</v>
       </c>
       <c r="H97">
-        <v>6378.9763389999998</v>
+        <v>5889.2193499330369</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.3">
@@ -4024,19 +4026,19 @@
         <v>282</v>
       </c>
       <c r="D98">
-        <v>1747.4617579999999</v>
+        <v>2344.3560127640571</v>
       </c>
       <c r="E98">
-        <v>2278.6070439999999</v>
+        <v>3047.6628165932748</v>
       </c>
       <c r="F98">
-        <v>3008.267437</v>
+        <v>4055.1022923486398</v>
       </c>
       <c r="G98">
-        <v>4870.8297910000001</v>
+        <v>4942.1559187999046</v>
       </c>
       <c r="H98">
-        <v>7311.6159600000001</v>
+        <v>7413.233878199856</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.3">
@@ -4050,19 +4052,19 @@
         <v>283</v>
       </c>
       <c r="D99">
-        <v>3211.7106410000001</v>
+        <v>14475.009838664528</v>
       </c>
       <c r="E99">
-        <v>4187.9179670000003</v>
+        <v>18817.512790263889</v>
       </c>
       <c r="F99">
-        <v>5528.9819630000002</v>
+        <v>24496.17049620151</v>
       </c>
       <c r="G99">
-        <v>8952.2393269999993</v>
+        <v>30063.481972610942</v>
       </c>
       <c r="H99">
-        <v>13438.23101</v>
+        <v>45095.22295891642</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.3">
@@ -4076,19 +4078,19 @@
         <v>284</v>
       </c>
       <c r="D100">
-        <v>2399.3182320000001</v>
+        <v>13099.212789515554</v>
       </c>
       <c r="E100">
-        <v>3128.5968929999999</v>
+        <v>17028.976626370222</v>
       </c>
       <c r="F100">
-        <v>4130.4428429999998</v>
+        <v>22167.898566872478</v>
       </c>
       <c r="G100">
-        <v>6687.7976989999997</v>
+        <v>27206.057332070766</v>
       </c>
       <c r="H100">
-        <v>10039.071470000001</v>
+        <v>40809.085998106159</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.3">
@@ -4102,19 +4104,19 @@
         <v>285</v>
       </c>
       <c r="D101">
-        <v>2063.9447610000002</v>
+        <v>3261.587328314266</v>
       </c>
       <c r="E101">
-        <v>2691.2858329999999</v>
+        <v>4240.0635268085462</v>
       </c>
       <c r="F101">
-        <v>3553.0951049999999</v>
+        <v>5641.6645678949462</v>
       </c>
       <c r="G101">
-        <v>5752.9863439999999</v>
+        <v>6875.7786921219658</v>
       </c>
       <c r="H101">
-        <v>8635.8235820000009</v>
+        <v>10313.668038182948</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.3">
@@ -4128,19 +4130,19 @@
         <v>286</v>
       </c>
       <c r="D102">
-        <v>20906.509959999999</v>
+        <v>31393.162145394828</v>
       </c>
       <c r="E102">
-        <v>27261.094929999999</v>
+        <v>40811.110789013284</v>
       </c>
       <c r="F102">
-        <v>35990.700720000001</v>
+        <v>52321.936908991382</v>
       </c>
       <c r="G102">
-        <v>58274.26614</v>
+        <v>66274.453418055753</v>
       </c>
       <c r="H102">
-        <v>87475.660740000007</v>
+        <v>99411.680127083615</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.3">
@@ -4154,19 +4156,19 @@
         <v>287</v>
       </c>
       <c r="D103">
-        <v>2177.6893439999999</v>
+        <v>4796.1456063740625</v>
       </c>
       <c r="E103">
-        <v>2839.6033600000001</v>
+        <v>6234.9892882862814</v>
       </c>
       <c r="F103">
-        <v>3748.9071859999999</v>
+        <v>8393.2548111546093</v>
       </c>
       <c r="G103">
-        <v>6070.0350570000001</v>
+        <v>10191.809413544883</v>
       </c>
       <c r="H103">
-        <v>9111.7462739999992</v>
+        <v>15287.714120317323</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.3">
@@ -4180,19 +4182,19 @@
         <v>288</v>
       </c>
       <c r="D104">
-        <v>5696.2677720000002</v>
+        <v>11789.674234665717</v>
       </c>
       <c r="E104">
-        <v>7427.6623310000004</v>
+        <v>15326.576505065434</v>
       </c>
       <c r="F104">
-        <v>9806.1641560000007</v>
+        <v>19951.756397126599</v>
       </c>
       <c r="G104">
-        <v>15877.629730000001</v>
+        <v>24486.246487382643</v>
       </c>
       <c r="H104">
-        <v>23833.953539999999</v>
+        <v>36729.369731073966</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.3">
@@ -4206,19 +4208,19 @@
         <v>289</v>
       </c>
       <c r="D105">
-        <v>6031.9367149999998</v>
+        <v>13466.894821358101</v>
       </c>
       <c r="E105">
-        <v>7865.3586729999997</v>
+        <v>17506.963267765532</v>
       </c>
       <c r="F105">
-        <v>10384.020549999999</v>
+        <v>22790.12969768294</v>
       </c>
       <c r="G105">
-        <v>16813.26468</v>
+        <v>27969.704628974516</v>
       </c>
       <c r="H105">
-        <v>25238.437730000001</v>
+        <v>41954.556943461779</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.3">
@@ -4232,19 +4234,19 @@
         <v>365</v>
       </c>
       <c r="D106">
-        <v>1932.379668</v>
+        <v>8613.0238396195564</v>
       </c>
       <c r="E106">
-        <v>2519.7312080000002</v>
+        <v>11196.930991505424</v>
       </c>
       <c r="F106">
-        <v>3326.6048930000002</v>
+        <v>15072.791719334224</v>
       </c>
       <c r="G106">
-        <v>5386.2652019999996</v>
+        <v>18302.675659191555</v>
       </c>
       <c r="H106">
-        <v>8085.3374690000001</v>
+        <v>27454.013488787336</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.3">
@@ -4258,19 +4260,19 @@
         <v>290</v>
       </c>
       <c r="D107">
-        <v>1106.7177180000001</v>
+        <v>10958.736312700372</v>
       </c>
       <c r="E107">
-        <v>1443.1072819999999</v>
+        <v>14246.357206510485</v>
       </c>
       <c r="F107">
-        <v>1905.222164</v>
+        <v>19177.788547225653</v>
       </c>
       <c r="G107">
-        <v>3084.8363949999998</v>
+        <v>23287.314664488291</v>
       </c>
       <c r="H107">
-        <v>4630.6563740000001</v>
+        <v>34930.971996732434</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.3">
@@ -4284,19 +4286,19 @@
         <v>292</v>
       </c>
       <c r="D108">
-        <v>2849.6225300000001</v>
+        <v>9042.0597656249993</v>
       </c>
       <c r="E108">
-        <v>3715.7722859999999</v>
+        <v>11754.677695312501</v>
       </c>
       <c r="F108">
-        <v>4905.6447889999999</v>
+        <v>15823.604589843751</v>
       </c>
       <c r="G108">
-        <v>7942.9642729999996</v>
+        <v>19214.377001953122</v>
       </c>
       <c r="H108">
-        <v>11923.205459999999</v>
+        <v>28821.565502929687</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.3">
@@ -4310,19 +4312,19 @@
         <v>293</v>
       </c>
       <c r="D109">
-        <v>1639.7410950000001</v>
+        <v>1864.9398124294944</v>
       </c>
       <c r="E109">
-        <v>2138.1444219999998</v>
+        <v>2424.4217561583428</v>
       </c>
       <c r="F109">
-        <v>2822.8255749999998</v>
+        <v>3225.8418377158823</v>
       </c>
       <c r="G109">
-        <v>4570.5719959999997</v>
+        <v>3931.4947397162314</v>
       </c>
       <c r="H109">
-        <v>6860.8981610000001</v>
+        <v>5897.2421095743466</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.3">
@@ -4336,19 +4338,19 @@
         <v>294</v>
       </c>
       <c r="D110">
-        <v>596.42109889999995</v>
+        <v>2956.0671979388289</v>
       </c>
       <c r="E110">
-        <v>777.7047546</v>
+        <v>3842.8873573204778</v>
       </c>
       <c r="F110">
-        <v>1026.743025</v>
+        <v>5173.1175963929509</v>
       </c>
       <c r="G110">
-        <v>1662.448774</v>
+        <v>6281.6427956200114</v>
       </c>
       <c r="H110">
-        <v>2495.5064139999999</v>
+        <v>9422.464193430018</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.3">
@@ -4362,19 +4364,19 @@
         <v>295</v>
       </c>
       <c r="D111">
-        <v>5502.1059560000003</v>
+        <v>6394.9456421243431</v>
       </c>
       <c r="E111">
-        <v>7174.484555</v>
+        <v>8313.4293347616458</v>
       </c>
       <c r="F111">
-        <v>9471.9132549999995</v>
+        <v>10822.215702056581</v>
       </c>
       <c r="G111">
-        <v>15336.428099999999</v>
+        <v>13281.810179796714</v>
       </c>
       <c r="H111">
-        <v>23021.55429</v>
+        <v>19922.715269695072</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.3">
@@ -4388,19 +4390,19 @@
         <v>296</v>
       </c>
       <c r="D112">
-        <v>1088.3832150000001</v>
+        <v>2950.5460923899</v>
       </c>
       <c r="E112">
-        <v>1419.1999619999999</v>
+        <v>3835.70992010687</v>
       </c>
       <c r="F112">
-        <v>1873.6591920000001</v>
+        <v>5163.4556616823247</v>
       </c>
       <c r="G112">
-        <v>3033.731276</v>
+        <v>6269.9104463285366</v>
       </c>
       <c r="H112">
-        <v>4553.9423399999996</v>
+        <v>9404.865669492805</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.3">
@@ -4414,19 +4416,19 @@
         <v>297</v>
       </c>
       <c r="D113">
-        <v>31616.823609999999</v>
+        <v>52855.083492432728</v>
       </c>
       <c r="E113">
-        <v>41226.834690000003</v>
+        <v>68711.608540162561</v>
       </c>
       <c r="F113">
-        <v>54428.579360000003</v>
+        <v>88091.805820721216</v>
       </c>
       <c r="G113">
-        <v>88127.917929999996</v>
+        <v>111582.9540395802</v>
       </c>
       <c r="H113">
-        <v>132289.05929999999</v>
+        <v>167374.43105937028</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.3">
@@ -4440,19 +4442,19 @@
         <v>298</v>
       </c>
       <c r="D114">
-        <v>27227.750390000001</v>
+        <v>44996.778605323008</v>
       </c>
       <c r="E114">
-        <v>35503.691899999998</v>
+        <v>58495.812186919917</v>
       </c>
       <c r="F114">
-        <v>46872.759610000001</v>
+        <v>74994.631008871671</v>
       </c>
       <c r="G114">
-        <v>75893.928530000005</v>
+        <v>94993.199277904117</v>
       </c>
       <c r="H114">
-        <v>113924.5843</v>
+        <v>142489.79891685618</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.3">
@@ -4466,19 +4468,19 @@
         <v>299</v>
       </c>
       <c r="D115">
-        <v>2176.467392</v>
+        <v>4955.8301912059933</v>
       </c>
       <c r="E115">
-        <v>2838.009994</v>
+        <v>6442.5792485677921</v>
       </c>
       <c r="F115">
-        <v>3746.8035890000001</v>
+        <v>8672.7028346104889</v>
       </c>
       <c r="G115">
-        <v>6066.6290220000001</v>
+        <v>10531.139156312734</v>
       </c>
       <c r="H115">
-        <v>9106.6334650000008</v>
+        <v>15796.708734469103</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.3">
@@ -4492,19 +4494,19 @@
         <v>300</v>
       </c>
       <c r="D116">
-        <v>1474.8773169999999</v>
+        <v>2185.3291305851285</v>
       </c>
       <c r="E116">
-        <v>1923.1698940000001</v>
+        <v>2840.9278697606674</v>
       </c>
       <c r="F116">
-        <v>2539.0114469999999</v>
+        <v>3780.0287664175194</v>
       </c>
       <c r="G116">
-        <v>4111.0349569999998</v>
+        <v>4606.9100590713515</v>
       </c>
       <c r="H116">
-        <v>6171.0858500000004</v>
+        <v>6910.3650886070272</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.3">
@@ -4518,19 +4520,19 @@
         <v>301</v>
       </c>
       <c r="D117">
-        <v>3292.3060869999999</v>
+        <v>4957.8585848427338</v>
       </c>
       <c r="E117">
-        <v>4293.0105960000001</v>
+        <v>6445.2161602955539</v>
       </c>
       <c r="F117">
-        <v>5667.727578</v>
+        <v>8676.2525234747845</v>
       </c>
       <c r="G117">
-        <v>9176.8889930000005</v>
+        <v>10535.449492790809</v>
       </c>
       <c r="H117">
-        <v>13775.453240000001</v>
+        <v>15803.174239186214</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.3">
@@ -4544,19 +4546,19 @@
         <v>302</v>
       </c>
       <c r="D118">
-        <v>38803.423320000002</v>
+        <v>81589.85192064532</v>
       </c>
       <c r="E118">
-        <v>50597.819000000003</v>
+        <v>106066.80749683894</v>
       </c>
       <c r="F118">
-        <v>66800.360190000007</v>
+        <v>135983.08653440888</v>
       </c>
       <c r="G118">
-        <v>108159.66039999999</v>
+        <v>172245.24294358457</v>
       </c>
       <c r="H118">
-        <v>162358.7629</v>
+        <v>258367.86441537683</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.3">
@@ -4570,19 +4572,19 @@
         <v>303</v>
       </c>
       <c r="D119">
-        <v>16418.835650000001</v>
+        <v>17558.519817047996</v>
       </c>
       <c r="E119">
-        <v>21409.381010000001</v>
+        <v>22826.0757621624</v>
       </c>
       <c r="F119">
-        <v>28265.13852</v>
+        <v>29264.199695079995</v>
       </c>
       <c r="G119">
-        <v>45765.438620000001</v>
+        <v>37067.986280434656</v>
       </c>
       <c r="H119">
-        <v>68698.625450000007</v>
+        <v>55601.97942065198</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.3">
@@ -4596,19 +4598,19 @@
         <v>304</v>
       </c>
       <c r="D120">
-        <v>1948.9608780000001</v>
+        <v>3614.6599033420089</v>
       </c>
       <c r="E120">
-        <v>2541.352316</v>
+        <v>4699.0578743446113</v>
       </c>
       <c r="F120">
-        <v>3355.149559</v>
+        <v>6325.6548308485162</v>
       </c>
       <c r="G120">
-        <v>5432.4832370000004</v>
+        <v>7681.1522946017685</v>
       </c>
       <c r="H120">
-        <v>8154.7154879999998</v>
+        <v>11521.728441902653</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.3">
@@ -4622,19 +4624,19 @@
         <v>305</v>
       </c>
       <c r="D121">
-        <v>4719.319759</v>
+        <v>13942.160821204492</v>
       </c>
       <c r="E121">
-        <v>6153.7685739999997</v>
+        <v>18124.809067565842</v>
       </c>
       <c r="F121">
-        <v>8124.3414320000002</v>
+        <v>23236.934702007486</v>
       </c>
       <c r="G121">
-        <v>13154.510060000001</v>
+        <v>29433.450622542812</v>
       </c>
       <c r="H121">
-        <v>19746.271140000001</v>
+        <v>44150.175933814215</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.3">
@@ -4648,19 +4650,19 @@
         <v>306</v>
       </c>
       <c r="D122">
-        <v>1195.740865</v>
+        <v>6299.0498645126881</v>
       </c>
       <c r="E122">
-        <v>1559.1892330000001</v>
+        <v>8188.7648238664951</v>
       </c>
       <c r="F122">
-        <v>2058.4761250000001</v>
+        <v>11023.337262897205</v>
       </c>
       <c r="G122">
-        <v>3332.9772170000001</v>
+        <v>13385.480962089461</v>
       </c>
       <c r="H122">
-        <v>5003.141243</v>
+        <v>20078.221443134193</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.3">
@@ -4674,19 +4676,19 @@
         <v>307</v>
       </c>
       <c r="D123">
-        <v>2608.9239729999999</v>
+        <v>7747.2743321171483</v>
       </c>
       <c r="E123">
-        <v>3401.9128129999999</v>
+        <v>10071.456631752293</v>
       </c>
       <c r="F123">
-        <v>4491.2805669999998</v>
+        <v>13110.77194665979</v>
       </c>
       <c r="G123">
-        <v>7272.0473300000003</v>
+        <v>16090.492843627922</v>
       </c>
       <c r="H123">
-        <v>10916.090190000001</v>
+        <v>24135.739265441887</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.3">
@@ -4700,19 +4702,19 @@
         <v>308</v>
       </c>
       <c r="D124">
-        <v>3787.009423</v>
+        <v>8626.1033925192496</v>
       </c>
       <c r="E124">
-        <v>4938.0802249999997</v>
+        <v>11213.934410275026</v>
       </c>
       <c r="F124">
-        <v>6519.3627749999996</v>
+        <v>14598.021125801808</v>
       </c>
       <c r="G124">
-        <v>10555.8123</v>
+        <v>17915.753199847673</v>
       </c>
       <c r="H124">
-        <v>15845.3588</v>
+        <v>26873.629799771516</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.3">
@@ -4726,19 +4728,19 @@
         <v>309</v>
       </c>
       <c r="D125">
-        <v>1876.52367</v>
+        <v>8305.2945160617965</v>
       </c>
       <c r="E125">
-        <v>2446.8976419999999</v>
+        <v>10796.882870880338</v>
       </c>
       <c r="F125">
-        <v>3230.4484080000002</v>
+        <v>14534.265403108146</v>
       </c>
       <c r="G125">
-        <v>5230.5736340000003</v>
+        <v>17648.750846631319</v>
       </c>
       <c r="H125">
-        <v>7851.6284299999998</v>
+        <v>26473.126269946977</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.3">
@@ -4752,19 +4754,19 @@
         <v>310</v>
       </c>
       <c r="D126">
-        <v>6243.9956570000004</v>
+        <v>16245.25149970448</v>
       </c>
       <c r="E126">
-        <v>8141.87345</v>
+        <v>21118.826949615825</v>
       </c>
       <c r="F126">
-        <v>10749.081480000001</v>
+        <v>27075.419166174132</v>
       </c>
       <c r="G126">
-        <v>17404.352299999999</v>
+        <v>34295.530943820566</v>
       </c>
       <c r="H126">
-        <v>26125.720979999998</v>
+        <v>51443.296415730845</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.3">
@@ -4778,19 +4780,19 @@
         <v>311</v>
       </c>
       <c r="D127">
-        <v>23357.211210000001</v>
+        <v>22195.049838711817</v>
       </c>
       <c r="E127">
-        <v>30456.69284</v>
+        <v>28853.564790325363</v>
       </c>
       <c r="F127">
-        <v>40209.59979</v>
+        <v>36991.749731186355</v>
       </c>
       <c r="G127">
-        <v>65105.287550000001</v>
+        <v>46856.216326169386</v>
       </c>
       <c r="H127">
-        <v>97729.725720000002</v>
+        <v>70284.324489254068</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.3">
@@ -4804,19 +4806,19 @@
         <v>312</v>
       </c>
       <c r="D128">
-        <v>52066.675309999999</v>
+        <v>60172.867550404371</v>
       </c>
       <c r="E128">
-        <v>67892.468959999998</v>
+        <v>78224.727815525694</v>
       </c>
       <c r="F128">
-        <v>89633.139729999995</v>
+        <v>100288.11258400728</v>
       </c>
       <c r="G128">
-        <v>145129.30660000001</v>
+        <v>127031.60927307588</v>
       </c>
       <c r="H128">
-        <v>217854.00020000001</v>
+        <v>190547.4139096138</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.3">
@@ -4830,19 +4832,19 @@
         <v>313</v>
       </c>
       <c r="D129">
-        <v>4987.9632769999998</v>
+        <v>31628.03784073293</v>
       </c>
       <c r="E129">
-        <v>6504.0669470000003</v>
+        <v>41116.449192952816</v>
       </c>
       <c r="F129">
-        <v>8586.8130949999995</v>
+        <v>52713.396401221551</v>
       </c>
       <c r="G129">
-        <v>13903.32007</v>
+        <v>66770.30210821396</v>
       </c>
       <c r="H129">
-        <v>20870.311890000001</v>
+        <v>100155.45316232093</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.3">
@@ -4856,19 +4858,19 @@
         <v>314</v>
       </c>
       <c r="D130">
-        <v>693.72554709999997</v>
+        <v>6857.1683013567153</v>
       </c>
       <c r="E130">
-        <v>904.58512840000003</v>
+        <v>8914.3187917637297</v>
       </c>
       <c r="F130">
-        <v>1194.2533020000001</v>
+        <v>11604.438663834442</v>
       </c>
       <c r="G130">
-        <v>1933.672681</v>
+        <v>14241.811087433178</v>
       </c>
       <c r="H130">
-        <v>2902.641365</v>
+        <v>21362.716631149771</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.3">
@@ -4882,19 +4884,19 @@
         <v>291</v>
       </c>
       <c r="D131">
-        <v>3110.2957219999998</v>
+        <v>13121.470310944595</v>
       </c>
       <c r="E131">
-        <v>4055.6777350000002</v>
+        <v>17057.911404227973</v>
       </c>
       <c r="F131">
-        <v>5354.3954830000002</v>
+        <v>22205.565141598545</v>
       </c>
       <c r="G131">
-        <v>8669.5580009999994</v>
+        <v>27252.284491961851</v>
       </c>
       <c r="H131">
-        <v>13013.897300000001</v>
+        <v>40878.426737942777</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.3">
@@ -4908,19 +4910,19 @@
         <v>324</v>
       </c>
       <c r="D132">
-        <v>2301.7158140000001</v>
+        <v>12398.987726750667</v>
       </c>
       <c r="E132">
-        <v>3001.3279809999999</v>
+        <v>16118.684044775868</v>
       </c>
       <c r="F132">
-        <v>3962.419609</v>
+        <v>20982.902306808821</v>
       </c>
       <c r="G132">
-        <v>6415.7432399999998</v>
+        <v>25751.743740174465</v>
       </c>
       <c r="H132">
-        <v>9630.6897750000007</v>
+        <v>38627.615610261702</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.3">
@@ -4934,19 +4936,19 @@
         <v>315</v>
       </c>
       <c r="D133">
-        <v>3722.4966250000002</v>
+        <v>13451.962471810175</v>
       </c>
       <c r="E133">
-        <v>4853.9586040000004</v>
+        <v>17487.551213353228</v>
       </c>
       <c r="F133">
-        <v>6408.3035490000002</v>
+        <v>22419.937453016959</v>
       </c>
       <c r="G133">
-        <v>10375.99099</v>
+        <v>28398.587440488147</v>
       </c>
       <c r="H133">
-        <v>15575.428540000001</v>
+        <v>42597.881160732213</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.3">
@@ -4960,19 +4962,19 @@
         <v>316</v>
       </c>
       <c r="D134">
-        <v>4240.3737659999997</v>
+        <v>16291.666015625</v>
       </c>
       <c r="E134">
-        <v>5529.2457709999999</v>
+        <v>21179.165820312501</v>
       </c>
       <c r="F134">
-        <v>7299.832609</v>
+        <v>27570.511718750004</v>
       </c>
       <c r="G134">
-        <v>11819.50837</v>
+        <v>33836.537109375</v>
       </c>
       <c r="H134">
-        <v>17742.296429999999</v>
+        <v>50754.805664062507</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.3">
@@ -4986,19 +4988,19 @@
         <v>317</v>
       </c>
       <c r="D135">
-        <v>2100.3044989999999</v>
+        <v>3038.3341607901093</v>
       </c>
       <c r="E135">
-        <v>2738.6972030000002</v>
+        <v>3949.8344090271426</v>
       </c>
       <c r="F135">
-        <v>3615.6886450000002</v>
+        <v>5255.4969267720808</v>
       </c>
       <c r="G135">
-        <v>5854.3345399999998</v>
+        <v>6405.1368795034732</v>
       </c>
       <c r="H135">
-        <v>8787.9576359999992</v>
+        <v>9607.7053192552103</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.3">
@@ -5012,19 +5014,19 @@
         <v>318</v>
       </c>
       <c r="D136">
-        <v>5571.9574389999998</v>
+        <v>14191.095203725246</v>
       </c>
       <c r="E136">
-        <v>7265.5675680000004</v>
+        <v>18448.423764842821</v>
       </c>
       <c r="F136">
-        <v>9592.1630640000003</v>
+        <v>24015.699575535033</v>
       </c>
       <c r="G136">
-        <v>15531.13032</v>
+        <v>29473.813115429359</v>
       </c>
       <c r="H136">
-        <v>23313.822329999999</v>
+        <v>44210.719673144042</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.3">
@@ -5038,19 +5040,19 @@
         <v>319</v>
       </c>
       <c r="D137">
-        <v>4706.9540630000001</v>
+        <v>10868.083511184383</v>
       </c>
       <c r="E137">
-        <v>6137.6442950000001</v>
+        <v>14128.508564539698</v>
       </c>
       <c r="F137">
-        <v>8103.0538020000004</v>
+        <v>18392.141326619723</v>
       </c>
       <c r="G137">
-        <v>13120.042240000001</v>
+        <v>22572.173446306024</v>
       </c>
       <c r="H137">
-        <v>19694.5314</v>
+        <v>33858.260169459041</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.3">
@@ -5064,19 +5066,19 @@
         <v>321</v>
       </c>
       <c r="D138">
-        <v>1679.68515</v>
+        <v>5641.0864823312104</v>
       </c>
       <c r="E138">
-        <v>2190.2295709999999</v>
+        <v>7333.4124270305747</v>
       </c>
       <c r="F138">
-        <v>2891.5895409999998</v>
+        <v>9871.9013440796189</v>
       </c>
       <c r="G138">
-        <v>4681.9110250000003</v>
+        <v>11987.308774953823</v>
       </c>
       <c r="H138">
-        <v>7028.0294819999999</v>
+        <v>17980.963162430733</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.3">
@@ -5090,19 +5092,19 @@
         <v>320</v>
       </c>
       <c r="D139">
-        <v>2343.307863</v>
+        <v>9258.4553809550107</v>
       </c>
       <c r="E139">
-        <v>3055.5620349999999</v>
+        <v>12035.991995241517</v>
       </c>
       <c r="F139">
-        <v>4034.0206069999999</v>
+        <v>16202.296916671272</v>
       </c>
       <c r="G139">
-        <v>6531.6758419999996</v>
+        <v>19674.217684529398</v>
       </c>
       <c r="H139">
-        <v>9804.7165229999991</v>
+        <v>29511.326526794099</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.3">
@@ -5116,19 +5118,19 @@
         <v>322</v>
       </c>
       <c r="D140">
-        <v>18079.79391</v>
+        <v>21884.056696068597</v>
       </c>
       <c r="E140">
-        <v>23575.191610000002</v>
+        <v>28449.273704889179</v>
       </c>
       <c r="F140">
-        <v>31124.489600000001</v>
+        <v>36473.427826780993</v>
       </c>
       <c r="G140">
-        <v>50395.150800000003</v>
+        <v>46199.675247255924</v>
       </c>
       <c r="H140">
-        <v>75648.299100000004</v>
+        <v>69299.512870883875</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.3">
@@ -5142,19 +5144,19 @@
         <v>323</v>
       </c>
       <c r="D141">
-        <v>2467.4052660000002</v>
+        <v>3920.5442853685704</v>
       </c>
       <c r="E141">
-        <v>3217.379148</v>
+        <v>5096.7075709791416</v>
       </c>
       <c r="F141">
-        <v>4247.6551399999998</v>
+        <v>6860.952499394999</v>
       </c>
       <c r="G141">
-        <v>6877.5817399999996</v>
+        <v>8331.1566064082126</v>
       </c>
       <c r="H141">
-        <v>10323.956819999999</v>
+        <v>12496.734909612318</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.3">
@@ -5168,19 +5170,19 @@
         <v>325</v>
       </c>
       <c r="D142">
-        <v>1327.0855449999999</v>
+        <v>1867.0987641996664</v>
       </c>
       <c r="E142">
-        <v>1730.456451</v>
+        <v>2427.2283934595666</v>
       </c>
       <c r="F142">
-        <v>2284.5868959999998</v>
+        <v>3229.5762407778016</v>
       </c>
       <c r="G142">
-        <v>3699.0839879999999</v>
+        <v>3936.0460434479451</v>
       </c>
       <c r="H142">
-        <v>5552.7051220000003</v>
+        <v>5904.0690651719178</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.3">
@@ -5194,19 +5196,19 @@
         <v>326</v>
       </c>
       <c r="D143">
-        <v>27939.151470000001</v>
+        <v>69939.08031357819</v>
       </c>
       <c r="E143">
-        <v>36431.325080000002</v>
+        <v>90920.804407651653</v>
       </c>
       <c r="F143">
-        <v>48097.441460000002</v>
+        <v>116565.13385596364</v>
       </c>
       <c r="G143">
-        <v>77876.869529999996</v>
+        <v>147649.16955088725</v>
       </c>
       <c r="H143">
-        <v>116901.1825</v>
+        <v>221473.75432633088</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.3">
@@ -5220,19 +5222,19 @@
         <v>327</v>
       </c>
       <c r="D144">
-        <v>6767.4414850000003</v>
+        <v>19591.333803722326</v>
       </c>
       <c r="E144">
-        <v>8824.4219219999995</v>
+        <v>25468.733944839027</v>
       </c>
       <c r="F144">
-        <v>11650.19707</v>
+        <v>32652.223006203876</v>
       </c>
       <c r="G144">
-        <v>18863.39169</v>
+        <v>41359.482474524906</v>
       </c>
       <c r="H144">
-        <v>28315.889009999999</v>
+        <v>62039.223711787359</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.3">
@@ -5246,19 +5248,19 @@
         <v>328</v>
       </c>
       <c r="D145">
-        <v>22825.905900000002</v>
+        <v>26397.958230903878</v>
       </c>
       <c r="E145">
-        <v>29763.895980000001</v>
+        <v>34317.345700175043</v>
       </c>
       <c r="F145">
-        <v>39294.95405</v>
+        <v>43996.597051506462</v>
       </c>
       <c r="G145">
-        <v>63624.340850000001</v>
+        <v>55729.022931908177</v>
       </c>
       <c r="H145">
-        <v>95506.672569999995</v>
+        <v>83593.53439786227</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.3">
@@ -5272,19 +5274,19 @@
         <v>329</v>
       </c>
       <c r="D146">
-        <v>1427.640236</v>
+        <v>5358.0886895443937</v>
       </c>
       <c r="E146">
-        <v>1861.5749860000001</v>
+        <v>6965.5152964077124</v>
       </c>
       <c r="F146">
-        <v>2457.6924869999998</v>
+        <v>9376.6552067026896</v>
       </c>
       <c r="G146">
-        <v>3979.3675370000001</v>
+        <v>11385.938465281835</v>
       </c>
       <c r="H146">
-        <v>5973.4395249999998</v>
+        <v>17078.907697922754</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.3">
@@ -5298,19 +5300,19 @@
         <v>330</v>
       </c>
       <c r="D147">
-        <v>1029.87987</v>
+        <v>2133.1376094957996</v>
       </c>
       <c r="E147">
-        <v>1342.9143819999999</v>
+        <v>2773.0788923445398</v>
       </c>
       <c r="F147">
-        <v>1772.9452799999999</v>
+        <v>3689.7515407494911</v>
       </c>
       <c r="G147">
-        <v>2870.6605610000001</v>
+        <v>4496.8846902884416</v>
       </c>
       <c r="H147">
-        <v>4309.1564420000004</v>
+        <v>6745.3270354326623</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.3">
@@ -5324,19 +5326,19 @@
         <v>331</v>
       </c>
       <c r="D148">
-        <v>6648.3923379999997</v>
+        <v>9195.6965803536696</v>
       </c>
       <c r="E148">
-        <v>8669.1874950000001</v>
+        <v>11954.40555445977</v>
       </c>
       <c r="F148">
-        <v>11445.25315</v>
+        <v>15561.948059060056</v>
       </c>
       <c r="G148">
-        <v>18531.55717</v>
+        <v>19098.754436119161</v>
       </c>
       <c r="H148">
-        <v>27817.7713</v>
+        <v>28648.131654178742</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.3">
@@ -5350,19 +5352,19 @@
         <v>332</v>
       </c>
       <c r="D149">
-        <v>2063.6994129999998</v>
+        <v>3966.4</v>
       </c>
       <c r="E149">
-        <v>2690.9659109999998</v>
+        <v>5156.3200000000006</v>
       </c>
       <c r="F149">
-        <v>3552.6727369999999</v>
+        <v>6860.8</v>
       </c>
       <c r="G149">
-        <v>5752.3024679999999</v>
+        <v>8361.6</v>
       </c>
       <c r="H149">
-        <v>8634.7970129999994</v>
+        <v>12542.4</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.3">
@@ -5376,19 +5378,19 @@
         <v>333</v>
       </c>
       <c r="D150">
-        <v>26643.357609999999</v>
+        <v>27439.93885759174</v>
       </c>
       <c r="E150">
-        <v>34741.671499999997</v>
+        <v>35671.920514869264</v>
       </c>
       <c r="F150">
-        <v>45866.723420000002</v>
+        <v>45733.231429319567</v>
       </c>
       <c r="G150">
-        <v>74265.007180000001</v>
+        <v>57928.759810471442</v>
       </c>
       <c r="H150">
-        <v>111479.406</v>
+        <v>86893.139715707162</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.3">
@@ -5402,19 +5404,19 @@
         <v>334</v>
       </c>
       <c r="D151">
-        <v>1796.936854</v>
+        <v>9591.7727880300245</v>
       </c>
       <c r="E151">
-        <v>2343.1202170000001</v>
+        <v>12469.304624439033</v>
       </c>
       <c r="F151">
-        <v>3093.4391559999999</v>
+        <v>16785.602379052543</v>
       </c>
       <c r="G151">
-        <v>5008.7353970000004</v>
+        <v>20382.5171745638</v>
       </c>
       <c r="H151">
-        <v>7518.6264430000001</v>
+        <v>30573.775761845704</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.3">
@@ -5428,19 +5430,19 @@
         <v>335</v>
       </c>
       <c r="D152">
-        <v>2063.6994129999998</v>
+        <v>2773.9151123046877</v>
       </c>
       <c r="E152">
-        <v>2690.9659109999998</v>
+        <v>3606.0896459960941</v>
       </c>
       <c r="F152">
-        <v>3552.6727369999999</v>
+        <v>4798.1234375000004</v>
       </c>
       <c r="G152">
-        <v>5752.3024679999999</v>
+        <v>5847.7129394531248</v>
       </c>
       <c r="H152">
-        <v>8634.7970129999994</v>
+        <v>8771.5694091796868</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.3">
@@ -5454,19 +5456,19 @@
         <v>336</v>
       </c>
       <c r="D153">
-        <v>4370.1155319999998</v>
+        <v>6534.9433406279486</v>
       </c>
       <c r="E153">
-        <v>5698.4228649999995</v>
+        <v>8495.426342816334</v>
       </c>
       <c r="F153">
-        <v>7523.1839520000003</v>
+        <v>11059.134884139605</v>
       </c>
       <c r="G153">
-        <v>12181.147209999999</v>
+        <v>13572.574630534969</v>
       </c>
       <c r="H153">
-        <v>18285.1535</v>
+        <v>20358.861945802459</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.3">
@@ -5480,19 +5482,19 @@
         <v>337</v>
       </c>
       <c r="D154">
-        <v>4943.2836719999996</v>
+        <v>9764.577157223177</v>
       </c>
       <c r="E154">
-        <v>6445.8068670000002</v>
+        <v>12693.950304390131</v>
       </c>
       <c r="F154">
-        <v>8509.8968480000003</v>
+        <v>17088.01002514056</v>
       </c>
       <c r="G154">
-        <v>13778.781290000001</v>
+        <v>20749.726459099253</v>
       </c>
       <c r="H154">
-        <v>20683.366389999999</v>
+        <v>31124.589688648877</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.3">
@@ -5506,19 +5508,19 @@
         <v>338</v>
       </c>
       <c r="D155">
-        <v>31810.672740000002</v>
+        <v>55275.91278898219</v>
       </c>
       <c r="E155">
-        <v>41479.604729999999</v>
+        <v>71858.686625676855</v>
       </c>
       <c r="F155">
-        <v>54762.291949999999</v>
+        <v>92126.521314970305</v>
       </c>
       <c r="G155">
-        <v>88668.247959999993</v>
+        <v>116693.59366562906</v>
       </c>
       <c r="H155">
-        <v>133100.1502</v>
+        <v>175040.39049844356</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.3">
@@ -5532,19 +5534,19 @@
         <v>339</v>
       </c>
       <c r="D156">
-        <v>34963.765489999998</v>
+        <v>84101.791006704865</v>
       </c>
       <c r="E156">
-        <v>45591.087760000002</v>
+        <v>109332.32830871634</v>
       </c>
       <c r="F156">
-        <v>60190.362829999998</v>
+        <v>140169.65167784144</v>
       </c>
       <c r="G156">
-        <v>97457.097309999997</v>
+        <v>177548.22545859916</v>
       </c>
       <c r="H156">
-        <v>146293.11610000001</v>
+        <v>266322.33818789868</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.3">
@@ -5558,19 +5560,19 @@
         <v>340</v>
       </c>
       <c r="D157">
-        <v>2624.4972760000001</v>
+        <v>1556.3040090960999</v>
       </c>
       <c r="E157">
-        <v>3422.2196589999999</v>
+        <v>2023.1952118249299</v>
       </c>
       <c r="F157">
-        <v>4518.090115</v>
+        <v>2691.9853130310917</v>
       </c>
       <c r="G157">
-        <v>7315.4559529999997</v>
+        <v>3280.8571002566428</v>
       </c>
       <c r="H157">
-        <v>10981.251</v>
+        <v>4921.2856503849644</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.3">
@@ -5584,19 +5586,19 @@
         <v>341</v>
       </c>
       <c r="D158">
-        <v>419.40103909999999</v>
+        <v>2200.060720948612</v>
       </c>
       <c r="E158">
-        <v>546.87901350000004</v>
+        <v>2860.078937233196</v>
       </c>
       <c r="F158">
-        <v>722.00177410000003</v>
+        <v>3850.1062616600716</v>
       </c>
       <c r="G158">
-        <v>1169.0276289999999</v>
+        <v>4675.1290320158005</v>
       </c>
       <c r="H158">
-        <v>1754.8305809999999</v>
+        <v>7012.6935480237016</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.3">
@@ -5610,19 +5612,19 @@
         <v>342</v>
       </c>
       <c r="D159">
-        <v>2037.083288</v>
+        <v>9179.1670190534333</v>
       </c>
       <c r="E159">
-        <v>2656.2597489999998</v>
+        <v>11932.917124769463</v>
       </c>
       <c r="F159">
-        <v>3506.8528940000001</v>
+        <v>15533.974955321195</v>
       </c>
       <c r="G159">
-        <v>5678.1133669999999</v>
+        <v>19064.423808803283</v>
       </c>
       <c r="H159">
-        <v>8523.4315490000008</v>
+        <v>28596.635713204931</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.3">
@@ -5636,19 +5638,19 @@
         <v>343</v>
       </c>
       <c r="D160">
-        <v>790.18065720000004</v>
+        <v>6580.6819678683842</v>
       </c>
       <c r="E160">
-        <v>1030.3580059999999</v>
+        <v>8554.8865582289</v>
       </c>
       <c r="F160">
-        <v>1360.3014370000001</v>
+        <v>11516.193443769673</v>
       </c>
       <c r="G160">
-        <v>2202.5291649999999</v>
+        <v>13983.949181720316</v>
       </c>
       <c r="H160">
-        <v>3306.2225699999999</v>
+        <v>20975.923772580474</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.3">
@@ -5662,19 +5664,19 @@
         <v>344</v>
       </c>
       <c r="D161">
-        <v>1736.1788140000001</v>
+        <v>3613.6648775796766</v>
       </c>
       <c r="E161">
-        <v>2263.8946219999998</v>
+        <v>4697.7643408535796</v>
       </c>
       <c r="F161">
-        <v>2988.8437720000002</v>
+        <v>6250.6635720297108</v>
       </c>
       <c r="G161">
-        <v>4839.380005</v>
+        <v>7617.9962284112098</v>
       </c>
       <c r="H161">
-        <v>7264.4065989999999</v>
+        <v>11426.994342616814</v>
       </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.3">
@@ -5688,19 +5690,19 @@
         <v>345</v>
       </c>
       <c r="D162">
-        <v>1951.2262109999999</v>
+        <v>5753.7629395807107</v>
       </c>
       <c r="E162">
-        <v>2544.3062030000001</v>
+        <v>7479.8918214549249</v>
       </c>
       <c r="F162">
-        <v>3359.0493459999998</v>
+        <v>9737.1372823673573</v>
       </c>
       <c r="G162">
-        <v>5438.797568</v>
+        <v>11950.123028359938</v>
       </c>
       <c r="H162">
-        <v>8164.1939480000001</v>
+        <v>17925.184542539911</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.3">
@@ -5714,19 +5716,19 @@
         <v>346</v>
       </c>
       <c r="D163">
-        <v>7230.0781989999996</v>
+        <v>14450.671836834594</v>
       </c>
       <c r="E163">
-        <v>9427.6781989999999</v>
+        <v>18785.873387884974</v>
       </c>
       <c r="F163">
-        <v>12446.629360000001</v>
+        <v>24084.453061390988</v>
       </c>
       <c r="G163">
-        <v>20152.93332</v>
+        <v>30506.97387776192</v>
       </c>
       <c r="H163">
-        <v>30251.623490000002</v>
+        <v>45760.460816642873</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.3">
@@ -5740,19 +5742,19 @@
         <v>347</v>
       </c>
       <c r="D164">
-        <v>4300.127778</v>
+        <v>9137.2418615241731</v>
       </c>
       <c r="E164">
-        <v>5607.1621619999996</v>
+        <v>11878.414419981427</v>
       </c>
       <c r="F164">
-        <v>7402.699552</v>
+        <v>15990.173257667306</v>
       </c>
       <c r="G164">
-        <v>11986.06516</v>
+        <v>19416.638955738868</v>
       </c>
       <c r="H164">
-        <v>17992.315279999999</v>
+        <v>29124.958433608303</v>
       </c>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.3">
@@ -5766,19 +5768,19 @@
         <v>348</v>
       </c>
       <c r="D165">
-        <v>4240.0606280000002</v>
+        <v>12666.177070201571</v>
       </c>
       <c r="E165">
-        <v>5528.8374540000004</v>
+        <v>16466.030191262042</v>
       </c>
       <c r="F165">
-        <v>7299.2935399999997</v>
+        <v>21435.068888033427</v>
       </c>
       <c r="G165">
-        <v>11818.63553</v>
+        <v>26306.675453495573</v>
       </c>
       <c r="H165">
-        <v>17740.986219999999</v>
+        <v>39460.013180243361</v>
       </c>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.3">
@@ -5792,19 +5794,19 @@
         <v>349</v>
       </c>
       <c r="D166">
-        <v>2925.1312440000002</v>
+        <v>10250.889864693712</v>
       </c>
       <c r="E166">
-        <v>3814.2320589999999</v>
+        <v>13326.156824101829</v>
       </c>
       <c r="F166">
-        <v>5035.6335589999999</v>
+        <v>17347.659771020131</v>
       </c>
       <c r="G166">
-        <v>8153.435313</v>
+        <v>21290.30971897925</v>
       </c>
       <c r="H166">
-        <v>12239.144109999999</v>
+        <v>31935.46457846888</v>
       </c>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.3">
@@ -5818,19 +5820,19 @@
         <v>350</v>
       </c>
       <c r="D167">
-        <v>2493.6153960000001</v>
+        <v>3268.8231938881495</v>
       </c>
       <c r="E167">
-        <v>3251.5559109999999</v>
+        <v>4249.470152054595</v>
       </c>
       <c r="F167">
-        <v>4292.7760580000004</v>
+        <v>5654.1806596984206</v>
       </c>
       <c r="G167">
-        <v>6950.6391789999998</v>
+        <v>6891.0326790074496</v>
       </c>
       <c r="H167">
-        <v>10433.623540000001</v>
+        <v>10336.549018511174</v>
       </c>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.3">
@@ -5844,19 +5846,19 @@
         <v>351</v>
       </c>
       <c r="D168">
-        <v>1590.3565860000001</v>
+        <v>11586.8296875</v>
       </c>
       <c r="E168">
-        <v>2073.74937</v>
+        <v>15062.87859375</v>
       </c>
       <c r="F168">
-        <v>2737.8098030000001</v>
+        <v>20276.951953125001</v>
       </c>
       <c r="G168">
-        <v>4432.9188910000003</v>
+        <v>24622.013085937499</v>
       </c>
       <c r="H168">
-        <v>6654.2667060000003</v>
+        <v>36933.019628906244</v>
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.3">
@@ -5870,19 +5872,19 @@
         <v>352</v>
       </c>
       <c r="D169">
-        <v>32616.51658</v>
+        <v>39899.106046184643</v>
       </c>
       <c r="E169">
-        <v>42530.386780000001</v>
+        <v>51868.837860040047</v>
       </c>
       <c r="F169">
-        <v>56149.557670000002</v>
+        <v>66498.510076974402</v>
       </c>
       <c r="G169">
-        <v>90914.436279999994</v>
+        <v>84231.446097500913</v>
       </c>
       <c r="H169">
-        <v>136471.90969999999</v>
+        <v>126347.16914625136</v>
       </c>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.3">
@@ -5896,19 +5898,19 @@
         <v>353</v>
       </c>
       <c r="D170">
-        <v>30795.30213</v>
+        <v>42182.783152569929</v>
       </c>
       <c r="E170">
-        <v>40155.609729999996</v>
+        <v>54837.618098340914</v>
       </c>
       <c r="F170">
-        <v>53014.32447</v>
+        <v>70304.638587616544</v>
       </c>
       <c r="G170">
-        <v>85838.030140000003</v>
+        <v>89052.542210980959</v>
       </c>
       <c r="H170">
-        <v>128851.7025</v>
+        <v>133578.81331647141</v>
       </c>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.3">
@@ -5922,19 +5924,19 @@
         <v>354</v>
       </c>
       <c r="D171">
-        <v>2334.1495839999998</v>
+        <v>2750.476757812512</v>
       </c>
       <c r="E171">
-        <v>3043.6200739999999</v>
+        <v>3575.6197851562656</v>
       </c>
       <c r="F171">
-        <v>4018.2545660000001</v>
+        <v>4813.3343261718965</v>
       </c>
       <c r="G171">
-        <v>6506.1482910000004</v>
+        <v>5844.7631103515878</v>
       </c>
       <c r="H171">
-        <v>9766.397046</v>
+        <v>8767.1446655273812</v>
       </c>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.3">
@@ -5948,19 +5950,19 @@
         <v>355</v>
       </c>
       <c r="D172">
-        <v>33438.211199999998</v>
+        <v>63000</v>
       </c>
       <c r="E172">
-        <v>43601.837500000001</v>
+        <v>81900.000000000015</v>
       </c>
       <c r="F172">
-        <v>57564.110610000003</v>
+        <v>105000</v>
       </c>
       <c r="G172">
-        <v>93204.806649999999</v>
+        <v>133000</v>
       </c>
       <c r="H172">
-        <v>139909.9909</v>
+        <v>199499.99999999997</v>
       </c>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.3">
@@ -5974,19 +5976,19 @@
         <v>356</v>
       </c>
       <c r="D173">
-        <v>5014.3105079999996</v>
+        <v>16131.59579951653</v>
       </c>
       <c r="E173">
-        <v>6538.4224839999997</v>
+        <v>20971.074539371493</v>
       </c>
       <c r="F173">
-        <v>8632.1700349999992</v>
+        <v>26885.992999194219</v>
       </c>
       <c r="G173">
-        <v>13976.75966</v>
+        <v>34055.591132312671</v>
       </c>
       <c r="H173">
-        <v>20980.55226</v>
+        <v>51083.386698469003</v>
       </c>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.3">
@@ -6000,19 +6002,19 @@
         <v>357</v>
       </c>
       <c r="D174">
-        <v>524.89433740000004</v>
+        <v>4784.2187468929515</v>
       </c>
       <c r="E174">
-        <v>684.43725849999998</v>
+        <v>6219.4843709608376</v>
       </c>
       <c r="F174">
-        <v>903.60921280000002</v>
+        <v>8372.382807062666</v>
       </c>
       <c r="G174">
-        <v>1463.0769250000001</v>
+        <v>10166.464837147521</v>
       </c>
       <c r="H174">
-        <v>2196.2287860000001</v>
+        <v>15249.697255721283</v>
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.3">
@@ -6026,19 +6028,19 @@
         <v>358</v>
       </c>
       <c r="D175">
-        <v>1690.986598</v>
+        <v>7306.9767367669619</v>
       </c>
       <c r="E175">
-        <v>2204.9661209999999</v>
+        <v>9499.0697577970514</v>
       </c>
       <c r="F175">
-        <v>2911.0450609999998</v>
+        <v>12787.209289342183</v>
       </c>
       <c r="G175">
-        <v>4713.4123879999997</v>
+        <v>15527.325565629793</v>
       </c>
       <c r="H175">
-        <v>7075.3162650000004</v>
+        <v>23290.988348444687</v>
       </c>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.3">
@@ -6052,19 +6054,19 @@
         <v>359</v>
       </c>
       <c r="D176">
-        <v>5076.0987480000003</v>
+        <v>38400</v>
       </c>
       <c r="E176">
-        <v>6618.991411</v>
+        <v>49920</v>
       </c>
       <c r="F176">
-        <v>8738.5389149999992</v>
+        <v>67200</v>
       </c>
       <c r="G176">
-        <v>14148.98661</v>
+        <v>81600</v>
       </c>
       <c r="H176">
-        <v>21239.082600000002</v>
+        <v>122399.99999999999</v>
       </c>
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.3">
@@ -6078,19 +6080,19 @@
         <v>360</v>
       </c>
       <c r="D177">
-        <v>1058.550874</v>
+        <v>9015.5733619412276</v>
       </c>
       <c r="E177">
-        <v>1380.300009</v>
+        <v>11720.245370523597</v>
       </c>
       <c r="F177">
-        <v>1822.302612</v>
+        <v>15777.253383397148</v>
       </c>
       <c r="G177">
-        <v>2950.5773800000002</v>
+        <v>19158.093394125106</v>
       </c>
       <c r="H177">
-        <v>4429.1197979999997</v>
+        <v>28737.140091187663</v>
       </c>
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.3">
@@ -6104,19 +6106,19 @@
         <v>361</v>
       </c>
       <c r="D178">
-        <v>1682.67949</v>
+        <v>2011.4588900444035</v>
       </c>
       <c r="E178">
-        <v>2194.134047</v>
+        <v>2614.8965570577247</v>
       </c>
       <c r="F178">
-        <v>2896.7443170000001</v>
+        <v>3479.2802422389682</v>
       </c>
       <c r="G178">
-        <v>4690.2573689999999</v>
+        <v>4240.3727952287418</v>
       </c>
       <c r="H178">
-        <v>7040.5582020000002</v>
+        <v>6360.5591928431131</v>
       </c>
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.3">
@@ -6130,19 +6132,19 @@
         <v>362</v>
       </c>
       <c r="D179">
-        <v>3106.6653160000001</v>
+        <v>2723.3122901997745</v>
       </c>
       <c r="E179">
-        <v>4050.9438570000002</v>
+        <v>3540.3059772597071</v>
       </c>
       <c r="F179">
-        <v>5348.1457129999999</v>
+        <v>4765.7965078496063</v>
       </c>
       <c r="G179">
-        <v>8659.4386990000003</v>
+        <v>5787.0386166745211</v>
       </c>
       <c r="H179">
-        <v>12998.707179999999</v>
+        <v>8680.5579250117808</v>
       </c>
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.3">
@@ -6156,19 +6158,19 @@
         <v>363</v>
       </c>
       <c r="D180">
-        <v>2068.2084049999999</v>
+        <v>4257.4089861668463</v>
       </c>
       <c r="E180">
-        <v>2696.845421</v>
+        <v>5534.6316820169013</v>
       </c>
       <c r="F180">
-        <v>3560.4349969999998</v>
+        <v>7450.4657257919825</v>
       </c>
       <c r="G180">
-        <v>5764.8707139999997</v>
+        <v>9046.9940956045484</v>
       </c>
       <c r="H180">
-        <v>8653.6632420000005</v>
+        <v>13570.491143406824</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Health Workforce: Added Kiribati data.
</commit_message>
<xml_diff>
--- a/SourceData/humanresources/HWModData.xlsx
+++ b/SourceData/humanresources/HWModData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proj\SpectrumEngine\DefaultData\SourceData\humanresources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBB49640-5288-4CF7-AB8C-2AAB7C482470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EDEE44F-A377-41D9-9E82-BA78DB72D9D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25320" yWindow="-1095" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="StaffSalariesDB" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="368">
   <si>
     <t>&lt;Country Name&gt;</t>
   </si>
@@ -1134,6 +1134,12 @@
   </si>
   <si>
     <t>MICR</t>
+  </si>
+  <si>
+    <t>Kiribati</t>
+  </si>
+  <si>
+    <t>KIR</t>
   </si>
 </sst>
 </file>
@@ -1485,10 +1491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H180"/>
+  <dimension ref="A1:H181"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="J82" sqref="J82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3731,2445 +3737,2471 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87">
-        <v>414</v>
+        <v>296</v>
       </c>
       <c r="B87" t="s">
-        <v>91</v>
+        <v>366</v>
       </c>
       <c r="C87" t="s">
-        <v>271</v>
+        <v>367</v>
       </c>
       <c r="D87">
-        <v>29092.356813958962</v>
+        <v>4238.7462939999996</v>
       </c>
       <c r="E87">
-        <v>37820.063858146656</v>
+        <v>5510.370183</v>
       </c>
       <c r="F87">
-        <v>48487.261356598268</v>
+        <v>7417.8060150000001</v>
       </c>
       <c r="G87">
-        <v>61417.197718357806</v>
+        <v>9007.3358759999992</v>
       </c>
       <c r="H87">
-        <v>92125.796577536705</v>
+        <v>13511.00381</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="B88" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C88" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D88">
-        <v>3277.2199295828909</v>
+        <v>29092.356813958962</v>
       </c>
       <c r="E88">
-        <v>4260.3859084577589</v>
+        <v>37820.063858146656</v>
       </c>
       <c r="F88">
-        <v>5735.1348767700601</v>
+        <v>48487.261356598268</v>
       </c>
       <c r="G88">
-        <v>6964.0923503636432</v>
+        <v>61417.197718357806</v>
       </c>
       <c r="H88">
-        <v>10446.138525545464</v>
+        <v>92125.796577536705</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B89" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C89" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D89">
-        <v>6085.4962419256935</v>
+        <v>3277.2199295828909</v>
       </c>
       <c r="E89">
-        <v>7911.1451145034025</v>
+        <v>4260.3859084577589</v>
       </c>
       <c r="F89">
-        <v>10649.618423369964</v>
+        <v>5735.1348767700601</v>
       </c>
       <c r="G89">
-        <v>12931.679514092099</v>
+        <v>6964.0923503636432</v>
       </c>
       <c r="H89">
-        <v>19397.51927113815</v>
+        <v>10446.138525545464</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90">
-        <v>428</v>
+        <v>418</v>
       </c>
       <c r="B90" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C90" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D90">
-        <v>18837.358413676979</v>
+        <v>6085.4962419256935</v>
       </c>
       <c r="E90">
-        <v>24488.565937780073</v>
+        <v>7911.1451145034025</v>
       </c>
       <c r="F90">
-        <v>31395.597356128295</v>
+        <v>10649.618423369964</v>
       </c>
       <c r="G90">
-        <v>39767.756651095842</v>
+        <v>12931.679514092099</v>
       </c>
       <c r="H90">
-        <v>59651.634976643756</v>
+        <v>19397.51927113815</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91">
-        <v>422</v>
+        <v>428</v>
       </c>
       <c r="B91" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C91" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D91">
-        <v>9926.7517803843002</v>
+        <v>18837.358413676979</v>
       </c>
       <c r="E91">
-        <v>12904.777314499592</v>
+        <v>24488.565937780073</v>
       </c>
       <c r="F91">
-        <v>17371.815615672527</v>
+        <v>31395.597356128295</v>
       </c>
       <c r="G91">
-        <v>21094.347533316639</v>
+        <v>39767.756651095842</v>
       </c>
       <c r="H91">
-        <v>31641.521299974956</v>
+        <v>59651.634976643756</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="B92" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C92" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D92">
-        <v>2470.8148539088629</v>
+        <v>9926.7517803843002</v>
       </c>
       <c r="E92">
-        <v>3212.0593100815222</v>
+        <v>12904.777314499592</v>
       </c>
       <c r="F92">
-        <v>4323.9259943405104</v>
+        <v>17371.815615672527</v>
       </c>
       <c r="G92">
-        <v>5250.481564556334</v>
+        <v>21094.347533316639</v>
       </c>
       <c r="H92">
-        <v>7875.722346834501</v>
+        <v>31641.521299974956</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="B93" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C93" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D93">
-        <v>2499.9537876418913</v>
+        <v>2470.8148539088629</v>
       </c>
       <c r="E93">
-        <v>3249.9399239344584</v>
+        <v>3212.0593100815222</v>
       </c>
       <c r="F93">
-        <v>4324.2443894346225</v>
+        <v>4323.9259943405104</v>
       </c>
       <c r="G93">
-        <v>5270.1728496234455</v>
+        <v>5250.481564556334</v>
       </c>
       <c r="H93">
-        <v>7905.2592744351687</v>
+        <v>7875.722346834501</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="B94" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C94" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D94">
-        <v>7681.6367201146304</v>
+        <v>2499.9537876418913</v>
       </c>
       <c r="E94">
-        <v>9986.1277361490193</v>
+        <v>3249.9399239344584</v>
       </c>
       <c r="F94">
-        <v>12999.69291096322</v>
+        <v>4324.2443894346225</v>
       </c>
       <c r="G94">
-        <v>15954.16857254577</v>
+        <v>5270.1728496234455</v>
       </c>
       <c r="H94">
-        <v>23931.252858818658</v>
+        <v>7905.2592744351687</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95">
-        <v>440</v>
+        <v>434</v>
       </c>
       <c r="B95" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C95" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D95">
-        <v>21464.654129420942</v>
+        <v>7681.6367201146304</v>
       </c>
       <c r="E95">
-        <v>27904.050368247226</v>
+        <v>9986.1277361490193</v>
       </c>
       <c r="F95">
-        <v>35774.423549034902</v>
+        <v>12999.69291096322</v>
       </c>
       <c r="G95">
-        <v>45314.269828777535</v>
+        <v>15954.16857254577</v>
       </c>
       <c r="H95">
-        <v>67971.404743166306</v>
+        <v>23931.252858818658</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B96" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C96" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D96">
-        <v>120340.61499238691</v>
+        <v>21464.654129420942</v>
       </c>
       <c r="E96">
-        <v>156442.799490103</v>
+        <v>27904.050368247226</v>
       </c>
       <c r="F96">
-        <v>200567.69165397817</v>
+        <v>35774.423549034902</v>
       </c>
       <c r="G96">
-        <v>254052.40942837234</v>
+        <v>45314.269828777535</v>
       </c>
       <c r="H96">
-        <v>381078.61414255848</v>
+        <v>67971.404743166306</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97">
-        <v>450</v>
+        <v>442</v>
       </c>
       <c r="B97" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C97" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D97">
-        <v>1862.4027004061741</v>
+        <v>120340.61499238691</v>
       </c>
       <c r="E97">
-        <v>2421.1235105280266</v>
+        <v>156442.799490103</v>
       </c>
       <c r="F97">
-        <v>3221.4533196214907</v>
+        <v>200567.69165397817</v>
       </c>
       <c r="G97">
-        <v>3926.1462332886913</v>
+        <v>254052.40942837234</v>
       </c>
       <c r="H97">
-        <v>5889.2193499330369</v>
+        <v>381078.61414255848</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="B98" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C98" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D98">
-        <v>2344.3560127640571</v>
+        <v>1862.4027004061741</v>
       </c>
       <c r="E98">
-        <v>3047.6628165932748</v>
+        <v>2421.1235105280266</v>
       </c>
       <c r="F98">
-        <v>4055.1022923486398</v>
+        <v>3221.4533196214907</v>
       </c>
       <c r="G98">
-        <v>4942.1559187999046</v>
+        <v>3926.1462332886913</v>
       </c>
       <c r="H98">
-        <v>7413.233878199856</v>
+        <v>5889.2193499330369</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A99">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="B99" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C99" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D99">
-        <v>14475.009838664528</v>
+        <v>2344.3560127640571</v>
       </c>
       <c r="E99">
-        <v>18817.512790263889</v>
+        <v>3047.6628165932748</v>
       </c>
       <c r="F99">
-        <v>24496.17049620151</v>
+        <v>4055.1022923486398</v>
       </c>
       <c r="G99">
-        <v>30063.481972610942</v>
+        <v>4942.1559187999046</v>
       </c>
       <c r="H99">
-        <v>45095.22295891642</v>
+        <v>7413.233878199856</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A100">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="B100" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C100" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D100">
-        <v>13099.212789515554</v>
+        <v>14475.009838664528</v>
       </c>
       <c r="E100">
-        <v>17028.976626370222</v>
+        <v>18817.512790263889</v>
       </c>
       <c r="F100">
-        <v>22167.898566872478</v>
+        <v>24496.17049620151</v>
       </c>
       <c r="G100">
-        <v>27206.057332070766</v>
+        <v>30063.481972610942</v>
       </c>
       <c r="H100">
-        <v>40809.085998106159</v>
+        <v>45095.22295891642</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A101">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="B101" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C101" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D101">
-        <v>3261.587328314266</v>
+        <v>13099.212789515554</v>
       </c>
       <c r="E101">
-        <v>4240.0635268085462</v>
+        <v>17028.976626370222</v>
       </c>
       <c r="F101">
-        <v>5641.6645678949462</v>
+        <v>22167.898566872478</v>
       </c>
       <c r="G101">
-        <v>6875.7786921219658</v>
+        <v>27206.057332070766</v>
       </c>
       <c r="H101">
-        <v>10313.668038182948</v>
+        <v>40809.085998106159</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A102">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="B102" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C102" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D102">
-        <v>31393.162145394828</v>
+        <v>3261.587328314266</v>
       </c>
       <c r="E102">
-        <v>40811.110789013284</v>
+        <v>4240.0635268085462</v>
       </c>
       <c r="F102">
-        <v>52321.936908991382</v>
+        <v>5641.6645678949462</v>
       </c>
       <c r="G102">
-        <v>66274.453418055753</v>
+        <v>6875.7786921219658</v>
       </c>
       <c r="H102">
-        <v>99411.680127083615</v>
+        <v>10313.668038182948</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A103">
-        <v>478</v>
+        <v>470</v>
       </c>
       <c r="B103" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C103" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D103">
-        <v>4796.1456063740625</v>
+        <v>31393.162145394828</v>
       </c>
       <c r="E103">
-        <v>6234.9892882862814</v>
+        <v>40811.110789013284</v>
       </c>
       <c r="F103">
-        <v>8393.2548111546093</v>
+        <v>52321.936908991382</v>
       </c>
       <c r="G103">
-        <v>10191.809413544883</v>
+        <v>66274.453418055753</v>
       </c>
       <c r="H103">
-        <v>15287.714120317323</v>
+        <v>99411.680127083615</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A104">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B104" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C104" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D104">
-        <v>11789.674234665717</v>
+        <v>4796.1456063740625</v>
       </c>
       <c r="E104">
-        <v>15326.576505065434</v>
+        <v>6234.9892882862814</v>
       </c>
       <c r="F104">
-        <v>19951.756397126599</v>
+        <v>8393.2548111546093</v>
       </c>
       <c r="G104">
-        <v>24486.246487382643</v>
+        <v>10191.809413544883</v>
       </c>
       <c r="H104">
-        <v>36729.369731073966</v>
+        <v>15287.714120317323</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A105">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="B105" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C105" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D105">
-        <v>13466.894821358101</v>
+        <v>11789.674234665717</v>
       </c>
       <c r="E105">
-        <v>17506.963267765532</v>
+        <v>15326.576505065434</v>
       </c>
       <c r="F105">
-        <v>22790.12969768294</v>
+        <v>19951.756397126599</v>
       </c>
       <c r="G105">
-        <v>27969.704628974516</v>
+        <v>24486.246487382643</v>
       </c>
       <c r="H105">
-        <v>41954.556943461779</v>
+        <v>36729.369731073966</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A106">
-        <v>583</v>
+        <v>484</v>
       </c>
       <c r="B106" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C106" t="s">
-        <v>365</v>
+        <v>289</v>
       </c>
       <c r="D106">
-        <v>8613.0238396195564</v>
+        <v>13466.894821358101</v>
       </c>
       <c r="E106">
-        <v>11196.930991505424</v>
+        <v>17506.963267765532</v>
       </c>
       <c r="F106">
-        <v>15072.791719334224</v>
+        <v>22790.12969768294</v>
       </c>
       <c r="G106">
-        <v>18302.675659191555</v>
+        <v>27969.704628974516</v>
       </c>
       <c r="H106">
-        <v>27454.013488787336</v>
+        <v>41954.556943461779</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A107">
-        <v>496</v>
+        <v>583</v>
       </c>
       <c r="B107" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C107" t="s">
-        <v>290</v>
+        <v>365</v>
       </c>
       <c r="D107">
-        <v>10958.736312700372</v>
+        <v>8613.0238396195564</v>
       </c>
       <c r="E107">
-        <v>14246.357206510485</v>
+        <v>11196.930991505424</v>
       </c>
       <c r="F107">
-        <v>19177.788547225653</v>
+        <v>15072.791719334224</v>
       </c>
       <c r="G107">
-        <v>23287.314664488291</v>
+        <v>18302.675659191555</v>
       </c>
       <c r="H107">
-        <v>34930.971996732434</v>
+        <v>27454.013488787336</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A108">
-        <v>504</v>
+        <v>496</v>
       </c>
       <c r="B108" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C108" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D108">
-        <v>9042.0597656249993</v>
+        <v>10958.736312700372</v>
       </c>
       <c r="E108">
-        <v>11754.677695312501</v>
+        <v>14246.357206510485</v>
       </c>
       <c r="F108">
-        <v>15823.604589843751</v>
+        <v>19177.788547225653</v>
       </c>
       <c r="G108">
-        <v>19214.377001953122</v>
+        <v>23287.314664488291</v>
       </c>
       <c r="H108">
-        <v>28821.565502929687</v>
+        <v>34930.971996732434</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A109">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="B109" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C109" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D109">
-        <v>1864.9398124294944</v>
+        <v>9042.0597656249993</v>
       </c>
       <c r="E109">
-        <v>2424.4217561583428</v>
+        <v>11754.677695312501</v>
       </c>
       <c r="F109">
-        <v>3225.8418377158823</v>
+        <v>15823.604589843751</v>
       </c>
       <c r="G109">
-        <v>3931.4947397162314</v>
+        <v>19214.377001953122</v>
       </c>
       <c r="H109">
-        <v>5897.2421095743466</v>
+        <v>28821.565502929687</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A110">
-        <v>104</v>
+        <v>508</v>
       </c>
       <c r="B110" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C110" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D110">
-        <v>2956.0671979388289</v>
+        <v>1864.9398124294944</v>
       </c>
       <c r="E110">
-        <v>3842.8873573204778</v>
+        <v>2424.4217561583428</v>
       </c>
       <c r="F110">
-        <v>5173.1175963929509</v>
+        <v>3225.8418377158823</v>
       </c>
       <c r="G110">
-        <v>6281.6427956200114</v>
+        <v>3931.4947397162314</v>
       </c>
       <c r="H110">
-        <v>9422.464193430018</v>
+        <v>5897.2421095743466</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A111">
-        <v>516</v>
+        <v>104</v>
       </c>
       <c r="B111" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C111" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D111">
-        <v>6394.9456421243431</v>
+        <v>2956.0671979388289</v>
       </c>
       <c r="E111">
-        <v>8313.4293347616458</v>
+        <v>3842.8873573204778</v>
       </c>
       <c r="F111">
-        <v>10822.215702056581</v>
+        <v>5173.1175963929509</v>
       </c>
       <c r="G111">
-        <v>13281.810179796714</v>
+        <v>6281.6427956200114</v>
       </c>
       <c r="H111">
-        <v>19922.715269695072</v>
+        <v>9422.464193430018</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A112">
-        <v>524</v>
+        <v>516</v>
       </c>
       <c r="B112" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C112" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D112">
-        <v>2950.5460923899</v>
+        <v>6394.9456421243431</v>
       </c>
       <c r="E112">
-        <v>3835.70992010687</v>
+        <v>8313.4293347616458</v>
       </c>
       <c r="F112">
-        <v>5163.4556616823247</v>
+        <v>10822.215702056581</v>
       </c>
       <c r="G112">
-        <v>6269.9104463285366</v>
+        <v>13281.810179796714</v>
       </c>
       <c r="H112">
-        <v>9404.865669492805</v>
+        <v>19922.715269695072</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A113">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="B113" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C113" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D113">
-        <v>52855.083492432728</v>
+        <v>2950.5460923899</v>
       </c>
       <c r="E113">
-        <v>68711.608540162561</v>
+        <v>3835.70992010687</v>
       </c>
       <c r="F113">
-        <v>88091.805820721216</v>
+        <v>5163.4556616823247</v>
       </c>
       <c r="G113">
-        <v>111582.9540395802</v>
+        <v>6269.9104463285366</v>
       </c>
       <c r="H113">
-        <v>167374.43105937028</v>
+        <v>9404.865669492805</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A114">
-        <v>554</v>
+        <v>528</v>
       </c>
       <c r="B114" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C114" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D114">
-        <v>44996.778605323008</v>
+        <v>52855.083492432728</v>
       </c>
       <c r="E114">
-        <v>58495.812186919917</v>
+        <v>68711.608540162561</v>
       </c>
       <c r="F114">
-        <v>74994.631008871671</v>
+        <v>88091.805820721216</v>
       </c>
       <c r="G114">
-        <v>94993.199277904117</v>
+        <v>111582.9540395802</v>
       </c>
       <c r="H114">
-        <v>142489.79891685618</v>
+        <v>167374.43105937028</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A115">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="B115" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C115" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D115">
-        <v>4955.8301912059933</v>
+        <v>44996.778605323008</v>
       </c>
       <c r="E115">
-        <v>6442.5792485677921</v>
+        <v>58495.812186919917</v>
       </c>
       <c r="F115">
-        <v>8672.7028346104889</v>
+        <v>74994.631008871671</v>
       </c>
       <c r="G115">
-        <v>10531.139156312734</v>
+        <v>94993.199277904117</v>
       </c>
       <c r="H115">
-        <v>15796.708734469103</v>
+        <v>142489.79891685618</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A116">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="B116" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C116" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D116">
-        <v>2185.3291305851285</v>
+        <v>4955.8301912059933</v>
       </c>
       <c r="E116">
-        <v>2840.9278697606674</v>
+        <v>6442.5792485677921</v>
       </c>
       <c r="F116">
-        <v>3780.0287664175194</v>
+        <v>8672.7028346104889</v>
       </c>
       <c r="G116">
-        <v>4606.9100590713515</v>
+        <v>10531.139156312734</v>
       </c>
       <c r="H116">
-        <v>6910.3650886070272</v>
+        <v>15796.708734469103</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A117">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="B117" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C117" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D117">
-        <v>4957.8585848427338</v>
+        <v>2185.3291305851285</v>
       </c>
       <c r="E117">
-        <v>6445.2161602955539</v>
+        <v>2840.9278697606674</v>
       </c>
       <c r="F117">
-        <v>8676.2525234747845</v>
+        <v>3780.0287664175194</v>
       </c>
       <c r="G117">
-        <v>10535.449492790809</v>
+        <v>4606.9100590713515</v>
       </c>
       <c r="H117">
-        <v>15803.174239186214</v>
+        <v>6910.3650886070272</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A118">
-        <v>578</v>
+        <v>566</v>
       </c>
       <c r="B118" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C118" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D118">
-        <v>81589.85192064532</v>
+        <v>4957.8585848427338</v>
       </c>
       <c r="E118">
-        <v>106066.80749683894</v>
+        <v>6445.2161602955539</v>
       </c>
       <c r="F118">
-        <v>135983.08653440888</v>
+        <v>8676.2525234747845</v>
       </c>
       <c r="G118">
-        <v>172245.24294358457</v>
+        <v>10535.449492790809</v>
       </c>
       <c r="H118">
-        <v>258367.86441537683</v>
+        <v>15803.174239186214</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A119">
-        <v>512</v>
+        <v>578</v>
       </c>
       <c r="B119" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C119" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D119">
-        <v>17558.519817047996</v>
+        <v>81589.85192064532</v>
       </c>
       <c r="E119">
-        <v>22826.0757621624</v>
+        <v>106066.80749683894</v>
       </c>
       <c r="F119">
-        <v>29264.199695079995</v>
+        <v>135983.08653440888</v>
       </c>
       <c r="G119">
-        <v>37067.986280434656</v>
+        <v>172245.24294358457</v>
       </c>
       <c r="H119">
-        <v>55601.97942065198</v>
+        <v>258367.86441537683</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A120">
-        <v>586</v>
+        <v>512</v>
       </c>
       <c r="B120" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C120" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D120">
-        <v>3614.6599033420089</v>
+        <v>17558.519817047996</v>
       </c>
       <c r="E120">
-        <v>4699.0578743446113</v>
+        <v>22826.0757621624</v>
       </c>
       <c r="F120">
-        <v>6325.6548308485162</v>
+        <v>29264.199695079995</v>
       </c>
       <c r="G120">
-        <v>7681.1522946017685</v>
+        <v>37067.986280434656</v>
       </c>
       <c r="H120">
-        <v>11521.728441902653</v>
+        <v>55601.97942065198</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A121">
-        <v>591</v>
+        <v>586</v>
       </c>
       <c r="B121" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C121" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D121">
-        <v>13942.160821204492</v>
+        <v>3614.6599033420089</v>
       </c>
       <c r="E121">
-        <v>18124.809067565842</v>
+        <v>4699.0578743446113</v>
       </c>
       <c r="F121">
-        <v>23236.934702007486</v>
+        <v>6325.6548308485162</v>
       </c>
       <c r="G121">
-        <v>29433.450622542812</v>
+        <v>7681.1522946017685</v>
       </c>
       <c r="H121">
-        <v>44150.175933814215</v>
+        <v>11521.728441902653</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A122">
-        <v>598</v>
+        <v>591</v>
       </c>
       <c r="B122" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C122" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D122">
-        <v>6299.0498645126881</v>
+        <v>13942.160821204492</v>
       </c>
       <c r="E122">
-        <v>8188.7648238664951</v>
+        <v>18124.809067565842</v>
       </c>
       <c r="F122">
-        <v>11023.337262897205</v>
+        <v>23236.934702007486</v>
       </c>
       <c r="G122">
-        <v>13385.480962089461</v>
+        <v>29433.450622542812</v>
       </c>
       <c r="H122">
-        <v>20078.221443134193</v>
+        <v>44150.175933814215</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A123">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="B123" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C123" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D123">
-        <v>7747.2743321171483</v>
+        <v>6299.0498645126881</v>
       </c>
       <c r="E123">
-        <v>10071.456631752293</v>
+        <v>8188.7648238664951</v>
       </c>
       <c r="F123">
-        <v>13110.77194665979</v>
+        <v>11023.337262897205</v>
       </c>
       <c r="G123">
-        <v>16090.492843627922</v>
+        <v>13385.480962089461</v>
       </c>
       <c r="H123">
-        <v>24135.739265441887</v>
+        <v>20078.221443134193</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A124">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="B124" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C124" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D124">
-        <v>8626.1033925192496</v>
+        <v>7747.2743321171483</v>
       </c>
       <c r="E124">
-        <v>11213.934410275026</v>
+        <v>10071.456631752293</v>
       </c>
       <c r="F124">
-        <v>14598.021125801808</v>
+        <v>13110.77194665979</v>
       </c>
       <c r="G124">
-        <v>17915.753199847673</v>
+        <v>16090.492843627922</v>
       </c>
       <c r="H124">
-        <v>26873.629799771516</v>
+        <v>24135.739265441887</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A125">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="B125" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C125" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D125">
-        <v>8305.2945160617965</v>
+        <v>8626.1033925192496</v>
       </c>
       <c r="E125">
-        <v>10796.882870880338</v>
+        <v>11213.934410275026</v>
       </c>
       <c r="F125">
-        <v>14534.265403108146</v>
+        <v>14598.021125801808</v>
       </c>
       <c r="G125">
-        <v>17648.750846631319</v>
+        <v>17915.753199847673</v>
       </c>
       <c r="H125">
-        <v>26473.126269946977</v>
+        <v>26873.629799771516</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A126">
-        <v>616</v>
+        <v>608</v>
       </c>
       <c r="B126" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C126" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D126">
-        <v>16245.25149970448</v>
+        <v>8305.2945160617965</v>
       </c>
       <c r="E126">
-        <v>21118.826949615825</v>
+        <v>10796.882870880338</v>
       </c>
       <c r="F126">
-        <v>27075.419166174132</v>
+        <v>14534.265403108146</v>
       </c>
       <c r="G126">
-        <v>34295.530943820566</v>
+        <v>17648.750846631319</v>
       </c>
       <c r="H126">
-        <v>51443.296415730845</v>
+        <v>26473.126269946977</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A127">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="B127" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C127" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D127">
-        <v>22195.049838711817</v>
+        <v>16245.25149970448</v>
       </c>
       <c r="E127">
-        <v>28853.564790325363</v>
+        <v>21118.826949615825</v>
       </c>
       <c r="F127">
-        <v>36991.749731186355</v>
+        <v>27075.419166174132</v>
       </c>
       <c r="G127">
-        <v>46856.216326169386</v>
+        <v>34295.530943820566</v>
       </c>
       <c r="H127">
-        <v>70284.324489254068</v>
+        <v>51443.296415730845</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A128">
-        <v>634</v>
+        <v>620</v>
       </c>
       <c r="B128" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C128" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D128">
-        <v>60172.867550404371</v>
+        <v>22195.049838711817</v>
       </c>
       <c r="E128">
-        <v>78224.727815525694</v>
+        <v>28853.564790325363</v>
       </c>
       <c r="F128">
-        <v>100288.11258400728</v>
+        <v>36991.749731186355</v>
       </c>
       <c r="G128">
-        <v>127031.60927307588</v>
+        <v>46856.216326169386</v>
       </c>
       <c r="H128">
-        <v>190547.4139096138</v>
+        <v>70284.324489254068</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A129">
-        <v>410</v>
+        <v>634</v>
       </c>
       <c r="B129" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C129" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D129">
-        <v>31628.03784073293</v>
+        <v>60172.867550404371</v>
       </c>
       <c r="E129">
-        <v>41116.449192952816</v>
+        <v>78224.727815525694</v>
       </c>
       <c r="F129">
-        <v>52713.396401221551</v>
+        <v>100288.11258400728</v>
       </c>
       <c r="G129">
-        <v>66770.30210821396</v>
+        <v>127031.60927307588</v>
       </c>
       <c r="H129">
-        <v>100155.45316232093</v>
+        <v>190547.4139096138</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A130">
-        <v>498</v>
+        <v>410</v>
       </c>
       <c r="B130" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C130" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D130">
-        <v>6857.1683013567153</v>
+        <v>31628.03784073293</v>
       </c>
       <c r="E130">
-        <v>8914.3187917637297</v>
+        <v>41116.449192952816</v>
       </c>
       <c r="F130">
-        <v>11604.438663834442</v>
+        <v>52713.396401221551</v>
       </c>
       <c r="G130">
-        <v>14241.811087433178</v>
+        <v>66770.30210821396</v>
       </c>
       <c r="H130">
-        <v>21362.716631149771</v>
+        <v>100155.45316232093</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A131">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B131" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C131" t="s">
-        <v>291</v>
+        <v>314</v>
       </c>
       <c r="D131">
-        <v>13121.470310944595</v>
+        <v>6857.1683013567153</v>
       </c>
       <c r="E131">
-        <v>17057.911404227973</v>
+        <v>8914.3187917637297</v>
       </c>
       <c r="F131">
-        <v>22205.565141598545</v>
+        <v>11604.438663834442</v>
       </c>
       <c r="G131">
-        <v>27252.284491961851</v>
+        <v>14241.811087433178</v>
       </c>
       <c r="H131">
-        <v>40878.426737942777</v>
+        <v>21362.716631149771</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A132">
-        <v>688</v>
+        <v>499</v>
       </c>
       <c r="B132" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C132" t="s">
-        <v>324</v>
+        <v>291</v>
       </c>
       <c r="D132">
-        <v>12398.987726750667</v>
+        <v>13121.470310944595</v>
       </c>
       <c r="E132">
-        <v>16118.684044775868</v>
+        <v>17057.911404227973</v>
       </c>
       <c r="F132">
-        <v>20982.902306808821</v>
+        <v>22205.565141598545</v>
       </c>
       <c r="G132">
-        <v>25751.743740174465</v>
+        <v>27252.284491961851</v>
       </c>
       <c r="H132">
-        <v>38627.615610261702</v>
+        <v>40878.426737942777</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A133">
-        <v>642</v>
+        <v>688</v>
       </c>
       <c r="B133" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C133" t="s">
-        <v>315</v>
+        <v>324</v>
       </c>
       <c r="D133">
-        <v>13451.962471810175</v>
+        <v>12398.987726750667</v>
       </c>
       <c r="E133">
-        <v>17487.551213353228</v>
+        <v>16118.684044775868</v>
       </c>
       <c r="F133">
-        <v>22419.937453016959</v>
+        <v>20982.902306808821</v>
       </c>
       <c r="G133">
-        <v>28398.587440488147</v>
+        <v>25751.743740174465</v>
       </c>
       <c r="H133">
-        <v>42597.881160732213</v>
+        <v>38627.615610261702</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A134">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B134" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C134" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D134">
-        <v>16291.666015625</v>
+        <v>13451.962471810175</v>
       </c>
       <c r="E134">
-        <v>21179.165820312501</v>
+        <v>17487.551213353228</v>
       </c>
       <c r="F134">
-        <v>27570.511718750004</v>
+        <v>22419.937453016959</v>
       </c>
       <c r="G134">
-        <v>33836.537109375</v>
+        <v>28398.587440488147</v>
       </c>
       <c r="H134">
-        <v>50754.805664062507</v>
+        <v>42597.881160732213</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A135">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="B135" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C135" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D135">
-        <v>3038.3341607901093</v>
+        <v>16291.666015625</v>
       </c>
       <c r="E135">
-        <v>3949.8344090271426</v>
+        <v>21179.165820312501</v>
       </c>
       <c r="F135">
-        <v>5255.4969267720808</v>
+        <v>27570.511718750004</v>
       </c>
       <c r="G135">
-        <v>6405.1368795034732</v>
+        <v>33836.537109375</v>
       </c>
       <c r="H135">
-        <v>9607.7053192552103</v>
+        <v>50754.805664062507</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A136">
-        <v>662</v>
+        <v>646</v>
       </c>
       <c r="B136" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C136" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D136">
-        <v>14191.095203725246</v>
+        <v>3038.3341607901093</v>
       </c>
       <c r="E136">
-        <v>18448.423764842821</v>
+        <v>3949.8344090271426</v>
       </c>
       <c r="F136">
-        <v>24015.699575535033</v>
+        <v>5255.4969267720808</v>
       </c>
       <c r="G136">
-        <v>29473.813115429359</v>
+        <v>6405.1368795034732</v>
       </c>
       <c r="H136">
-        <v>44210.719673144042</v>
+        <v>9607.7053192552103</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A137">
-        <v>670</v>
+        <v>662</v>
       </c>
       <c r="B137" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C137" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D137">
-        <v>10868.083511184383</v>
+        <v>14191.095203725246</v>
       </c>
       <c r="E137">
-        <v>14128.508564539698</v>
+        <v>18448.423764842821</v>
       </c>
       <c r="F137">
-        <v>18392.141326619723</v>
+        <v>24015.699575535033</v>
       </c>
       <c r="G137">
-        <v>22572.173446306024</v>
+        <v>29473.813115429359</v>
       </c>
       <c r="H137">
-        <v>33858.260169459041</v>
+        <v>44210.719673144042</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A138">
-        <v>678</v>
+        <v>670</v>
       </c>
       <c r="B138" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C138" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D138">
-        <v>5641.0864823312104</v>
+        <v>10868.083511184383</v>
       </c>
       <c r="E138">
-        <v>7333.4124270305747</v>
+        <v>14128.508564539698</v>
       </c>
       <c r="F138">
-        <v>9871.9013440796189</v>
+        <v>18392.141326619723</v>
       </c>
       <c r="G138">
-        <v>11987.308774953823</v>
+        <v>22572.173446306024</v>
       </c>
       <c r="H138">
-        <v>17980.963162430733</v>
+        <v>33858.260169459041</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A139">
-        <v>882</v>
+        <v>678</v>
       </c>
       <c r="B139" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C139" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D139">
-        <v>9258.4553809550107</v>
+        <v>5641.0864823312104</v>
       </c>
       <c r="E139">
-        <v>12035.991995241517</v>
+        <v>7333.4124270305747</v>
       </c>
       <c r="F139">
-        <v>16202.296916671272</v>
+        <v>9871.9013440796189</v>
       </c>
       <c r="G139">
-        <v>19674.217684529398</v>
+        <v>11987.308774953823</v>
       </c>
       <c r="H139">
-        <v>29511.326526794099</v>
+        <v>17980.963162430733</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A140">
-        <v>682</v>
+        <v>882</v>
       </c>
       <c r="B140" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C140" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D140">
-        <v>21884.056696068597</v>
+        <v>9258.4553809550107</v>
       </c>
       <c r="E140">
-        <v>28449.273704889179</v>
+        <v>12035.991995241517</v>
       </c>
       <c r="F140">
-        <v>36473.427826780993</v>
+        <v>16202.296916671272</v>
       </c>
       <c r="G140">
-        <v>46199.675247255924</v>
+        <v>19674.217684529398</v>
       </c>
       <c r="H140">
-        <v>69299.512870883875</v>
+        <v>29511.326526794099</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A141">
-        <v>686</v>
+        <v>682</v>
       </c>
       <c r="B141" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C141" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D141">
-        <v>3920.5442853685704</v>
+        <v>21884.056696068597</v>
       </c>
       <c r="E141">
-        <v>5096.7075709791416</v>
+        <v>28449.273704889179</v>
       </c>
       <c r="F141">
-        <v>6860.952499394999</v>
+        <v>36473.427826780993</v>
       </c>
       <c r="G141">
-        <v>8331.1566064082126</v>
+        <v>46199.675247255924</v>
       </c>
       <c r="H141">
-        <v>12496.734909612318</v>
+        <v>69299.512870883875</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A142">
-        <v>694</v>
+        <v>686</v>
       </c>
       <c r="B142" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C142" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D142">
-        <v>1867.0987641996664</v>
+        <v>3920.5442853685704</v>
       </c>
       <c r="E142">
-        <v>2427.2283934595666</v>
+        <v>5096.7075709791416</v>
       </c>
       <c r="F142">
-        <v>3229.5762407778016</v>
+        <v>6860.952499394999</v>
       </c>
       <c r="G142">
-        <v>3936.0460434479451</v>
+        <v>8331.1566064082126</v>
       </c>
       <c r="H142">
-        <v>5904.0690651719178</v>
+        <v>12496.734909612318</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A143">
-        <v>702</v>
+        <v>694</v>
       </c>
       <c r="B143" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C143" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D143">
-        <v>69939.08031357819</v>
+        <v>1867.0987641996664</v>
       </c>
       <c r="E143">
-        <v>90920.804407651653</v>
+        <v>2427.2283934595666</v>
       </c>
       <c r="F143">
-        <v>116565.13385596364</v>
+        <v>3229.5762407778016</v>
       </c>
       <c r="G143">
-        <v>147649.16955088725</v>
+        <v>3936.0460434479451</v>
       </c>
       <c r="H143">
-        <v>221473.75432633088</v>
+        <v>5904.0690651719178</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A144">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="B144" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C144" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D144">
-        <v>19591.333803722326</v>
+        <v>69939.08031357819</v>
       </c>
       <c r="E144">
-        <v>25468.733944839027</v>
+        <v>90920.804407651653</v>
       </c>
       <c r="F144">
-        <v>32652.223006203876</v>
+        <v>116565.13385596364</v>
       </c>
       <c r="G144">
-        <v>41359.482474524906</v>
+        <v>147649.16955088725</v>
       </c>
       <c r="H144">
-        <v>62039.223711787359</v>
+        <v>221473.75432633088</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A145">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="B145" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C145" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D145">
-        <v>26397.958230903878</v>
+        <v>19591.333803722326</v>
       </c>
       <c r="E145">
-        <v>34317.345700175043</v>
+        <v>25468.733944839027</v>
       </c>
       <c r="F145">
-        <v>43996.597051506462</v>
+        <v>32652.223006203876</v>
       </c>
       <c r="G145">
-        <v>55729.022931908177</v>
+        <v>41359.482474524906</v>
       </c>
       <c r="H145">
-        <v>83593.53439786227</v>
+        <v>62039.223711787359</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A146">
-        <v>90</v>
+        <v>705</v>
       </c>
       <c r="B146" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C146" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D146">
-        <v>5358.0886895443937</v>
+        <v>26397.958230903878</v>
       </c>
       <c r="E146">
-        <v>6965.5152964077124</v>
+        <v>34317.345700175043</v>
       </c>
       <c r="F146">
-        <v>9376.6552067026896</v>
+        <v>43996.597051506462</v>
       </c>
       <c r="G146">
-        <v>11385.938465281835</v>
+        <v>55729.022931908177</v>
       </c>
       <c r="H146">
-        <v>17078.907697922754</v>
+        <v>83593.53439786227</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A147">
-        <v>706</v>
+        <v>90</v>
       </c>
       <c r="B147" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C147" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D147">
-        <v>2133.1376094957996</v>
+        <v>5358.0886895443937</v>
       </c>
       <c r="E147">
-        <v>2773.0788923445398</v>
+        <v>6965.5152964077124</v>
       </c>
       <c r="F147">
-        <v>3689.7515407494911</v>
+        <v>9376.6552067026896</v>
       </c>
       <c r="G147">
-        <v>4496.8846902884416</v>
+        <v>11385.938465281835</v>
       </c>
       <c r="H147">
-        <v>6745.3270354326623</v>
+        <v>17078.907697922754</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A148">
-        <v>710</v>
+        <v>706</v>
       </c>
       <c r="B148" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C148" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D148">
-        <v>9195.6965803536696</v>
+        <v>2133.1376094957996</v>
       </c>
       <c r="E148">
-        <v>11954.40555445977</v>
+        <v>2773.0788923445398</v>
       </c>
       <c r="F148">
-        <v>15561.948059060056</v>
+        <v>3689.7515407494911</v>
       </c>
       <c r="G148">
-        <v>19098.754436119161</v>
+        <v>4496.8846902884416</v>
       </c>
       <c r="H148">
-        <v>28648.131654178742</v>
+        <v>6745.3270354326623</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A149">
-        <v>728</v>
+        <v>710</v>
       </c>
       <c r="B149" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C149" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D149">
-        <v>3966.4</v>
+        <v>9195.6965803536696</v>
       </c>
       <c r="E149">
-        <v>5156.3200000000006</v>
+        <v>11954.40555445977</v>
       </c>
       <c r="F149">
-        <v>6860.8</v>
+        <v>15561.948059060056</v>
       </c>
       <c r="G149">
-        <v>8361.6</v>
+        <v>19098.754436119161</v>
       </c>
       <c r="H149">
-        <v>12542.4</v>
+        <v>28648.131654178742</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A150">
-        <v>724</v>
+        <v>728</v>
       </c>
       <c r="B150" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C150" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D150">
-        <v>27439.93885759174</v>
+        <v>3966.4</v>
       </c>
       <c r="E150">
-        <v>35671.920514869264</v>
+        <v>5156.3200000000006</v>
       </c>
       <c r="F150">
-        <v>45733.231429319567</v>
+        <v>6860.8</v>
       </c>
       <c r="G150">
-        <v>57928.759810471442</v>
+        <v>8361.6</v>
       </c>
       <c r="H150">
-        <v>86893.139715707162</v>
+        <v>12542.4</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A151">
-        <v>144</v>
+        <v>724</v>
       </c>
       <c r="B151" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C151" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D151">
-        <v>9591.7727880300245</v>
+        <v>27439.93885759174</v>
       </c>
       <c r="E151">
-        <v>12469.304624439033</v>
+        <v>35671.920514869264</v>
       </c>
       <c r="F151">
-        <v>16785.602379052543</v>
+        <v>45733.231429319567</v>
       </c>
       <c r="G151">
-        <v>20382.5171745638</v>
+        <v>57928.759810471442</v>
       </c>
       <c r="H151">
-        <v>30573.775761845704</v>
+        <v>86893.139715707162</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A152">
-        <v>729</v>
+        <v>144</v>
       </c>
       <c r="B152" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C152" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D152">
-        <v>2773.9151123046877</v>
+        <v>9591.7727880300245</v>
       </c>
       <c r="E152">
-        <v>3606.0896459960941</v>
+        <v>12469.304624439033</v>
       </c>
       <c r="F152">
-        <v>4798.1234375000004</v>
+        <v>16785.602379052543</v>
       </c>
       <c r="G152">
-        <v>5847.7129394531248</v>
+        <v>20382.5171745638</v>
       </c>
       <c r="H152">
-        <v>8771.5694091796868</v>
+        <v>30573.775761845704</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A153">
-        <v>740</v>
+        <v>729</v>
       </c>
       <c r="B153" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C153" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D153">
-        <v>6534.9433406279486</v>
+        <v>2773.9151123046877</v>
       </c>
       <c r="E153">
-        <v>8495.426342816334</v>
+        <v>3606.0896459960941</v>
       </c>
       <c r="F153">
-        <v>11059.134884139605</v>
+        <v>4798.1234375000004</v>
       </c>
       <c r="G153">
-        <v>13572.574630534969</v>
+        <v>5847.7129394531248</v>
       </c>
       <c r="H153">
-        <v>20358.861945802459</v>
+        <v>8771.5694091796868</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A154">
-        <v>748</v>
+        <v>740</v>
       </c>
       <c r="B154" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C154" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D154">
-        <v>9764.577157223177</v>
+        <v>6534.9433406279486</v>
       </c>
       <c r="E154">
-        <v>12693.950304390131</v>
+        <v>8495.426342816334</v>
       </c>
       <c r="F154">
-        <v>17088.01002514056</v>
+        <v>11059.134884139605</v>
       </c>
       <c r="G154">
-        <v>20749.726459099253</v>
+        <v>13572.574630534969</v>
       </c>
       <c r="H154">
-        <v>31124.589688648877</v>
+        <v>20358.861945802459</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A155">
-        <v>752</v>
+        <v>748</v>
       </c>
       <c r="B155" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C155" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D155">
-        <v>55275.91278898219</v>
+        <v>9764.577157223177</v>
       </c>
       <c r="E155">
-        <v>71858.686625676855</v>
+        <v>12693.950304390131</v>
       </c>
       <c r="F155">
-        <v>92126.521314970305</v>
+        <v>17088.01002514056</v>
       </c>
       <c r="G155">
-        <v>116693.59366562906</v>
+        <v>20749.726459099253</v>
       </c>
       <c r="H155">
-        <v>175040.39049844356</v>
+        <v>31124.589688648877</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A156">
-        <v>756</v>
+        <v>752</v>
       </c>
       <c r="B156" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C156" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D156">
-        <v>84101.791006704865</v>
+        <v>55275.91278898219</v>
       </c>
       <c r="E156">
-        <v>109332.32830871634</v>
+        <v>71858.686625676855</v>
       </c>
       <c r="F156">
-        <v>140169.65167784144</v>
+        <v>92126.521314970305</v>
       </c>
       <c r="G156">
-        <v>177548.22545859916</v>
+        <v>116693.59366562906</v>
       </c>
       <c r="H156">
-        <v>266322.33818789868</v>
+        <v>175040.39049844356</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A157">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="B157" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C157" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D157">
-        <v>1556.3040090960999</v>
+        <v>84101.791006704865</v>
       </c>
       <c r="E157">
-        <v>2023.1952118249299</v>
+        <v>109332.32830871634</v>
       </c>
       <c r="F157">
-        <v>2691.9853130310917</v>
+        <v>140169.65167784144</v>
       </c>
       <c r="G157">
-        <v>3280.8571002566428</v>
+        <v>177548.22545859916</v>
       </c>
       <c r="H157">
-        <v>4921.2856503849644</v>
+        <v>266322.33818789868</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A158">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="B158" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C158" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D158">
-        <v>2200.060720948612</v>
+        <v>1556.3040090960999</v>
       </c>
       <c r="E158">
-        <v>2860.078937233196</v>
+        <v>2023.1952118249299</v>
       </c>
       <c r="F158">
-        <v>3850.1062616600716</v>
+        <v>2691.9853130310917</v>
       </c>
       <c r="G158">
-        <v>4675.1290320158005</v>
+        <v>3280.8571002566428</v>
       </c>
       <c r="H158">
-        <v>7012.6935480237016</v>
+        <v>4921.2856503849644</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A159">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="B159" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C159" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D159">
-        <v>9179.1670190534333</v>
+        <v>2200.060720948612</v>
       </c>
       <c r="E159">
-        <v>11932.917124769463</v>
+        <v>2860.078937233196</v>
       </c>
       <c r="F159">
-        <v>15533.974955321195</v>
+        <v>3850.1062616600716</v>
       </c>
       <c r="G159">
-        <v>19064.423808803283</v>
+        <v>4675.1290320158005</v>
       </c>
       <c r="H159">
-        <v>28596.635713204931</v>
+        <v>7012.6935480237016</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A160">
-        <v>626</v>
+        <v>764</v>
       </c>
       <c r="B160" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C160" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D160">
-        <v>6580.6819678683842</v>
+        <v>9179.1670190534333</v>
       </c>
       <c r="E160">
-        <v>8554.8865582289</v>
+        <v>11932.917124769463</v>
       </c>
       <c r="F160">
-        <v>11516.193443769673</v>
+        <v>15533.974955321195</v>
       </c>
       <c r="G160">
-        <v>13983.949181720316</v>
+        <v>19064.423808803283</v>
       </c>
       <c r="H160">
-        <v>20975.923772580474</v>
+        <v>28596.635713204931</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A161">
-        <v>768</v>
+        <v>626</v>
       </c>
       <c r="B161" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C161" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D161">
-        <v>3613.6648775796766</v>
+        <v>6580.6819678683842</v>
       </c>
       <c r="E161">
-        <v>4697.7643408535796</v>
+        <v>8554.8865582289</v>
       </c>
       <c r="F161">
-        <v>6250.6635720297108</v>
+        <v>11516.193443769673</v>
       </c>
       <c r="G161">
-        <v>7617.9962284112098</v>
+        <v>13983.949181720316</v>
       </c>
       <c r="H161">
-        <v>11426.994342616814</v>
+        <v>20975.923772580474</v>
       </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A162">
-        <v>776</v>
+        <v>768</v>
       </c>
       <c r="B162" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C162" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D162">
-        <v>5753.7629395807107</v>
+        <v>3613.6648775796766</v>
       </c>
       <c r="E162">
-        <v>7479.8918214549249</v>
+        <v>4697.7643408535796</v>
       </c>
       <c r="F162">
-        <v>9737.1372823673573</v>
+        <v>6250.6635720297108</v>
       </c>
       <c r="G162">
-        <v>11950.123028359938</v>
+        <v>7617.9962284112098</v>
       </c>
       <c r="H162">
-        <v>17925.184542539911</v>
+        <v>11426.994342616814</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A163">
-        <v>780</v>
+        <v>776</v>
       </c>
       <c r="B163" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C163" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D163">
-        <v>14450.671836834594</v>
+        <v>5753.7629395807107</v>
       </c>
       <c r="E163">
-        <v>18785.873387884974</v>
+        <v>7479.8918214549249</v>
       </c>
       <c r="F163">
-        <v>24084.453061390988</v>
+        <v>9737.1372823673573</v>
       </c>
       <c r="G163">
-        <v>30506.97387776192</v>
+        <v>11950.123028359938</v>
       </c>
       <c r="H163">
-        <v>45760.460816642873</v>
+        <v>17925.184542539911</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A164">
-        <v>788</v>
+        <v>780</v>
       </c>
       <c r="B164" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C164" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D164">
-        <v>9137.2418615241731</v>
+        <v>14450.671836834594</v>
       </c>
       <c r="E164">
-        <v>11878.414419981427</v>
+        <v>18785.873387884974</v>
       </c>
       <c r="F164">
-        <v>15990.173257667306</v>
+        <v>24084.453061390988</v>
       </c>
       <c r="G164">
-        <v>19416.638955738868</v>
+        <v>30506.97387776192</v>
       </c>
       <c r="H164">
-        <v>29124.958433608303</v>
+        <v>45760.460816642873</v>
       </c>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A165">
-        <v>792</v>
+        <v>788</v>
       </c>
       <c r="B165" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C165" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D165">
-        <v>12666.177070201571</v>
+        <v>9137.2418615241731</v>
       </c>
       <c r="E165">
-        <v>16466.030191262042</v>
+        <v>11878.414419981427</v>
       </c>
       <c r="F165">
-        <v>21435.068888033427</v>
+        <v>15990.173257667306</v>
       </c>
       <c r="G165">
-        <v>26306.675453495573</v>
+        <v>19416.638955738868</v>
       </c>
       <c r="H165">
-        <v>39460.013180243361</v>
+        <v>29124.958433608303</v>
       </c>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A166">
-        <v>795</v>
+        <v>792</v>
       </c>
       <c r="B166" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C166" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D166">
-        <v>10250.889864693712</v>
+        <v>12666.177070201571</v>
       </c>
       <c r="E166">
-        <v>13326.156824101829</v>
+        <v>16466.030191262042</v>
       </c>
       <c r="F166">
-        <v>17347.659771020131</v>
+        <v>21435.068888033427</v>
       </c>
       <c r="G166">
-        <v>21290.30971897925</v>
+        <v>26306.675453495573</v>
       </c>
       <c r="H166">
-        <v>31935.46457846888</v>
+        <v>39460.013180243361</v>
       </c>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A167">
-        <v>800</v>
+        <v>795</v>
       </c>
       <c r="B167" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C167" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D167">
-        <v>3268.8231938881495</v>
+        <v>10250.889864693712</v>
       </c>
       <c r="E167">
-        <v>4249.470152054595</v>
+        <v>13326.156824101829</v>
       </c>
       <c r="F167">
-        <v>5654.1806596984206</v>
+        <v>17347.659771020131</v>
       </c>
       <c r="G167">
-        <v>6891.0326790074496</v>
+        <v>21290.30971897925</v>
       </c>
       <c r="H167">
-        <v>10336.549018511174</v>
+        <v>31935.46457846888</v>
       </c>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A168">
-        <v>804</v>
+        <v>800</v>
       </c>
       <c r="B168" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C168" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D168">
-        <v>11586.8296875</v>
+        <v>3268.8231938881495</v>
       </c>
       <c r="E168">
-        <v>15062.87859375</v>
+        <v>4249.470152054595</v>
       </c>
       <c r="F168">
-        <v>20276.951953125001</v>
+        <v>5654.1806596984206</v>
       </c>
       <c r="G168">
-        <v>24622.013085937499</v>
+        <v>6891.0326790074496</v>
       </c>
       <c r="H168">
-        <v>36933.019628906244</v>
+        <v>10336.549018511174</v>
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A169">
-        <v>784</v>
+        <v>804</v>
       </c>
       <c r="B169" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C169" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D169">
-        <v>39899.106046184643</v>
+        <v>11586.8296875</v>
       </c>
       <c r="E169">
-        <v>51868.837860040047</v>
+        <v>15062.87859375</v>
       </c>
       <c r="F169">
-        <v>66498.510076974402</v>
+        <v>20276.951953125001</v>
       </c>
       <c r="G169">
-        <v>84231.446097500913</v>
+        <v>24622.013085937499</v>
       </c>
       <c r="H169">
-        <v>126347.16914625136</v>
+        <v>36933.019628906244</v>
       </c>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A170">
-        <v>826</v>
+        <v>784</v>
       </c>
       <c r="B170" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C170" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D170">
-        <v>42182.783152569929</v>
+        <v>39899.106046184643</v>
       </c>
       <c r="E170">
-        <v>54837.618098340914</v>
+        <v>51868.837860040047</v>
       </c>
       <c r="F170">
-        <v>70304.638587616544</v>
+        <v>66498.510076974402</v>
       </c>
       <c r="G170">
-        <v>89052.542210980959</v>
+        <v>84231.446097500913</v>
       </c>
       <c r="H170">
-        <v>133578.81331647141</v>
+        <v>126347.16914625136</v>
       </c>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A171">
-        <v>834</v>
+        <v>826</v>
       </c>
       <c r="B171" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C171" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D171">
-        <v>2750.476757812512</v>
+        <v>42182.783152569929</v>
       </c>
       <c r="E171">
-        <v>3575.6197851562656</v>
+        <v>54837.618098340914</v>
       </c>
       <c r="F171">
-        <v>4813.3343261718965</v>
+        <v>70304.638587616544</v>
       </c>
       <c r="G171">
-        <v>5844.7631103515878</v>
+        <v>89052.542210980959</v>
       </c>
       <c r="H171">
-        <v>8767.1446655273812</v>
+        <v>133578.81331647141</v>
       </c>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A172">
-        <v>840</v>
+        <v>834</v>
       </c>
       <c r="B172" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C172" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D172">
-        <v>63000</v>
+        <v>2750.476757812512</v>
       </c>
       <c r="E172">
-        <v>81900.000000000015</v>
+        <v>3575.6197851562656</v>
       </c>
       <c r="F172">
-        <v>105000</v>
+        <v>4813.3343261718965</v>
       </c>
       <c r="G172">
-        <v>133000</v>
+        <v>5844.7631103515878</v>
       </c>
       <c r="H172">
-        <v>199499.99999999997</v>
+        <v>8767.1446655273812</v>
       </c>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A173">
-        <v>858</v>
+        <v>840</v>
       </c>
       <c r="B173" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C173" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D173">
-        <v>16131.59579951653</v>
+        <v>63000</v>
       </c>
       <c r="E173">
-        <v>20971.074539371493</v>
+        <v>81900.000000000015</v>
       </c>
       <c r="F173">
-        <v>26885.992999194219</v>
+        <v>105000</v>
       </c>
       <c r="G173">
-        <v>34055.591132312671</v>
+        <v>133000</v>
       </c>
       <c r="H173">
-        <v>51083.386698469003</v>
+        <v>199499.99999999997</v>
       </c>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A174">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="B174" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C174" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D174">
-        <v>4784.2187468929515</v>
+        <v>16131.59579951653</v>
       </c>
       <c r="E174">
-        <v>6219.4843709608376</v>
+        <v>20971.074539371493</v>
       </c>
       <c r="F174">
-        <v>8372.382807062666</v>
+        <v>26885.992999194219</v>
       </c>
       <c r="G174">
-        <v>10166.464837147521</v>
+        <v>34055.591132312671</v>
       </c>
       <c r="H174">
-        <v>15249.697255721283</v>
+        <v>51083.386698469003</v>
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A175">
-        <v>548</v>
+        <v>860</v>
       </c>
       <c r="B175" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C175" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D175">
-        <v>7306.9767367669619</v>
+        <v>4784.2187468929515</v>
       </c>
       <c r="E175">
-        <v>9499.0697577970514</v>
+        <v>6219.4843709608376</v>
       </c>
       <c r="F175">
-        <v>12787.209289342183</v>
+        <v>8372.382807062666</v>
       </c>
       <c r="G175">
-        <v>15527.325565629793</v>
+        <v>10166.464837147521</v>
       </c>
       <c r="H175">
-        <v>23290.988348444687</v>
+        <v>15249.697255721283</v>
       </c>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A176">
-        <v>862</v>
+        <v>548</v>
       </c>
       <c r="B176" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C176" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D176">
-        <v>38400</v>
+        <v>7306.9767367669619</v>
       </c>
       <c r="E176">
-        <v>49920</v>
+        <v>9499.0697577970514</v>
       </c>
       <c r="F176">
-        <v>67200</v>
+        <v>12787.209289342183</v>
       </c>
       <c r="G176">
-        <v>81600</v>
+        <v>15527.325565629793</v>
       </c>
       <c r="H176">
-        <v>122399.99999999999</v>
+        <v>23290.988348444687</v>
       </c>
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A177">
-        <v>704</v>
+        <v>862</v>
       </c>
       <c r="B177" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C177" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D177">
-        <v>9015.5733619412276</v>
+        <v>38400</v>
       </c>
       <c r="E177">
-        <v>11720.245370523597</v>
+        <v>49920</v>
       </c>
       <c r="F177">
-        <v>15777.253383397148</v>
+        <v>67200</v>
       </c>
       <c r="G177">
-        <v>19158.093394125106</v>
+        <v>81600</v>
       </c>
       <c r="H177">
-        <v>28737.140091187663</v>
+        <v>122399.99999999999</v>
       </c>
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A178">
-        <v>887</v>
+        <v>704</v>
       </c>
       <c r="B178" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C178" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D178">
-        <v>2011.4588900444035</v>
+        <v>9015.5733619412276</v>
       </c>
       <c r="E178">
-        <v>2614.8965570577247</v>
+        <v>11720.245370523597</v>
       </c>
       <c r="F178">
-        <v>3479.2802422389682</v>
+        <v>15777.253383397148</v>
       </c>
       <c r="G178">
-        <v>4240.3727952287418</v>
+        <v>19158.093394125106</v>
       </c>
       <c r="H178">
-        <v>6360.5591928431131</v>
+        <v>28737.140091187663</v>
       </c>
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A179">
-        <v>894</v>
+        <v>887</v>
       </c>
       <c r="B179" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C179" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D179">
-        <v>2723.3122901997745</v>
+        <v>2011.4588900444035</v>
       </c>
       <c r="E179">
-        <v>3540.3059772597071</v>
+        <v>2614.8965570577247</v>
       </c>
       <c r="F179">
-        <v>4765.7965078496063</v>
+        <v>3479.2802422389682</v>
       </c>
       <c r="G179">
-        <v>5787.0386166745211</v>
+        <v>4240.3727952287418</v>
       </c>
       <c r="H179">
-        <v>8680.5579250117808</v>
+        <v>6360.5591928431131</v>
       </c>
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A180">
+        <v>894</v>
+      </c>
+      <c r="B180" t="s">
+        <v>183</v>
+      </c>
+      <c r="C180" t="s">
+        <v>362</v>
+      </c>
+      <c r="D180">
+        <v>2723.3122901997745</v>
+      </c>
+      <c r="E180">
+        <v>3540.3059772597071</v>
+      </c>
+      <c r="F180">
+        <v>4765.7965078496063</v>
+      </c>
+      <c r="G180">
+        <v>5787.0386166745211</v>
+      </c>
+      <c r="H180">
+        <v>8680.5579250117808</v>
+      </c>
+    </row>
+    <row r="181" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A181">
         <v>716</v>
       </c>
-      <c r="B180" t="s">
+      <c r="B181" t="s">
         <v>184</v>
       </c>
-      <c r="C180" t="s">
+      <c r="C181" t="s">
         <v>363</v>
       </c>
-      <c r="D180">
+      <c r="D181">
         <v>4257.4089861668463</v>
       </c>
-      <c r="E180">
+      <c r="E181">
         <v>5534.6316820169013</v>
       </c>
-      <c r="F180">
+      <c r="F181">
         <v>7450.4657257919825</v>
       </c>
-      <c r="G180">
+      <c r="G181">
         <v>9046.9940956045484</v>
       </c>
-      <c r="H180">
+      <c r="H181">
         <v>13570.491143406824</v>
       </c>
     </row>

</xml_diff>